<commit_message>
update document Signed-off-by: LiuYiyang <lyy@shequchina.cn>
</commit_message>
<xml_diff>
--- a/document/AP_障害管理票_QDYL.xlsx
+++ b/document/AP_障害管理票_QDYL.xlsx
@@ -2596,6 +2596,201 @@
   </si>
   <si>
     <r>
+      <t>点</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>击</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t>入金按</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>钮</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t>后，会</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>给</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t>客</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>户发</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t>送一封主</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>题为</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t>“【エリア・パーキング】駐車場賃料に関するお知らせ”的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>邮</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">件。
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>该邮</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t>件与“繰越一覧”画面可以</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>发</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t>送的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>邮</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t>件内容一致，只是不包含客</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>户</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t>具体信息。疑似</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>为</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">多余操作。
+</t>
+    </r>
+    <phoneticPr fontId="52" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <rPr>
         <sz val="10"/>
         <rFont val="宋体"/>
@@ -2659,7 +2854,7 @@
         <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
       </rPr>
-      <t>4</t>
+      <t>5</t>
     </r>
     <r>
       <rPr>
@@ -2670,201 +2865,6 @@
         <charset val="134"/>
       </rPr>
       <t>秒</t>
-    </r>
-    <phoneticPr fontId="52" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>点</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>击</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-      </rPr>
-      <t>入金按</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>钮</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-      </rPr>
-      <t>后，会</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>给</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-      </rPr>
-      <t>客</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>户发</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-      </rPr>
-      <t>送一封主</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>题为</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-      </rPr>
-      <t>“【エリア・パーキング】駐車場賃料に関するお知らせ”的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>邮</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">件。
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>该邮</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-      </rPr>
-      <t>件与“繰越一覧”画面可以</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>发</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-      </rPr>
-      <t>送的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>邮</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-      </rPr>
-      <t>件内容一致，只是不包含客</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>户</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-      </rPr>
-      <t>具体信息。疑似</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>为</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">多余操作。
-</t>
     </r>
     <phoneticPr fontId="52" type="noConversion"/>
   </si>
@@ -2876,14 +2876,14 @@
   <numFmts count="10">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ \¥* #,##0_ ;_ \¥* \-#,##0_ ;_ \¥* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="181" formatCode="yyyy/m/d;@"/>
-    <numFmt numFmtId="182" formatCode="m/d"/>
-    <numFmt numFmtId="183" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="184" formatCode="0.0_ "/>
-    <numFmt numFmtId="185" formatCode="0_ "/>
+    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ \¥* #,##0_ ;_ \¥* \-#,##0_ ;_ \¥* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="180" formatCode="m/d"/>
+    <numFmt numFmtId="181" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="182" formatCode="0.0_ "/>
+    <numFmt numFmtId="183" formatCode="0_ "/>
   </numFmts>
   <fonts count="55">
     <font>
@@ -3581,7 +3581,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="179" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="177" fontId="31" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="23" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
@@ -3592,7 +3592,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0">
       <alignment vertical="center"/>
@@ -3613,7 +3613,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="180" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="32" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -3625,7 +3625,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
-    <xf numFmtId="180" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0">
       <alignment vertical="center"/>
@@ -3640,7 +3640,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
-    <xf numFmtId="178" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -3648,7 +3648,7 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="31" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
-    <xf numFmtId="179" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="177" fontId="31" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
@@ -4353,16 +4353,16 @@
     <xf numFmtId="56" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="183" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4386,7 +4386,7 @@
     <xf numFmtId="56" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4395,7 +4395,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4410,25 +4410,25 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="56" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="185" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4459,7 +4459,7 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4469,7 +4469,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="138"/>
-    <xf numFmtId="185" fontId="1" fillId="5" borderId="1" xfId="138" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="1" fillId="5" borderId="1" xfId="138" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="138" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4481,14 +4481,14 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="138" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="1" fillId="0" borderId="1" xfId="138" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="1" xfId="138" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="138" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="52"/>
-    <xf numFmtId="185" fontId="1" fillId="5" borderId="1" xfId="52" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="1" fillId="5" borderId="1" xfId="52" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="5" borderId="1" xfId="52" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4506,7 +4506,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="0" borderId="5" xfId="216" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="5" xfId="216" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="5" borderId="1" xfId="138" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4518,7 +4518,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="138" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="5" borderId="1" xfId="138" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4530,7 +4530,7 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="181" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4543,7 +4543,7 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="181" fontId="3" fillId="0" borderId="1" xfId="138" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="1" xfId="138" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="138" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4565,10 +4565,10 @@
     <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="138" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="0" borderId="25" xfId="52" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="25" xfId="52" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="0" borderId="25" xfId="228" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="25" xfId="228" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="52" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4597,7 +4597,7 @@
     <xf numFmtId="49" fontId="14" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="182" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4607,22 +4607,22 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="182" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="182" fontId="14" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="14" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4631,34 +4631,34 @@
     <xf numFmtId="49" fontId="14" fillId="5" borderId="1" xfId="138" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="0" borderId="25" xfId="222" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="25" xfId="222" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="14" fillId="0" borderId="25" xfId="216" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="14" fillId="0" borderId="25" xfId="216" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="0" borderId="25" xfId="216" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="25" xfId="216" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="0" borderId="25" xfId="217" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="25" xfId="217" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="5" borderId="1" xfId="138" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="0" borderId="25" xfId="225" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="25" xfId="225" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="16" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="16" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -4704,7 +4704,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="138" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="181" fontId="3" fillId="0" borderId="1" xfId="52" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="1" xfId="52" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="52" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4713,107 +4713,107 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="182" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="181" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="181" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="183" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="183" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="346">
@@ -5838,8 +5838,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674008"/>
-          <c:y val="3.5190678684544313E-2"/>
+          <c:x val="0.38523037913674013"/>
+          <c:y val="3.519067868454432E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -5856,7 +5856,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="8.5828510612584605E-2"/>
-          <c:y val="0.11730205278592401"/>
+          <c:y val="0.11730205278592402"/>
           <c:w val="0.80638879738335301"/>
           <c:h val="0.55131964809384204"/>
         </c:manualLayout>
@@ -5908,12 +5908,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="138401280"/>
-        <c:axId val="138402816"/>
+        <c:axId val="141016064"/>
+        <c:axId val="141021952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="138401280"/>
+        <c:axId val="141016064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5947,14 +5946,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="138402816"/>
+        <c:crossAx val="141021952"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="138402816"/>
+        <c:axId val="141021952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5988,7 +5987,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="138401280"/>
+        <c:crossAx val="141016064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6038,7 +6037,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6075,8 +6074,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674008"/>
-          <c:y val="3.0232730603965498E-2"/>
+          <c:x val="0.38523037913674013"/>
+          <c:y val="3.0232730603965505E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -6092,10 +6091,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11177666498383203"/>
+          <c:x val="0.11177666498383206"/>
           <c:y val="0.100000113553908"/>
           <c:w val="0.78044064301210703"/>
-          <c:h val="0.65814028222689125"/>
+          <c:h val="0.65814028222689147"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -6202,12 +6201,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="130431616"/>
-        <c:axId val="130453888"/>
+        <c:axId val="141074816"/>
+        <c:axId val="141076352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="130431616"/>
+        <c:axId val="141074816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6241,14 +6239,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="130453888"/>
+        <c:crossAx val="141076352"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="130453888"/>
+        <c:axId val="141076352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6282,7 +6280,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="130431616"/>
+        <c:crossAx val="141074816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6332,7 +6330,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6369,8 +6367,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.39506259248458309"/>
-          <c:y val="3.1476997578692802E-2"/>
+          <c:x val="0.3950625924845832"/>
+          <c:y val="3.1476997578692809E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -6386,10 +6384,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.2592778647397914E-2"/>
+          <c:x val="9.2592778647397928E-2"/>
           <c:y val="0.113801452784504"/>
-          <c:w val="0.77572172333487732"/>
-          <c:h val="0.6513317191283331"/>
+          <c:w val="0.77572172333487766"/>
+          <c:h val="0.65133171912833321"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -6690,10 +6688,9 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="143484800"/>
-        <c:axId val="143495168"/>
+        <c:axId val="141587584"/>
+        <c:axId val="141589120"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6791,13 +6788,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="143496704"/>
-        <c:axId val="143498240"/>
+        <c:axId val="141619584"/>
+        <c:axId val="141621120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="143484800"/>
+        <c:axId val="141587584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6831,14 +6827,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="143495168"/>
+        <c:crossAx val="141589120"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143495168"/>
+        <c:axId val="141589120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6872,29 +6868,29 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="143484800"/>
+        <c:crossAx val="141587584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="143496704"/>
+        <c:axId val="141619584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="143498240"/>
+        <c:crossAx val="141621120"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143498240"/>
+        <c:axId val="141621120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
-          <c:min val="0.75000000000000411"/>
+          <c:min val="0.75000000000000422"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
@@ -6926,7 +6922,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="143496704"/>
+        <c:crossAx val="141619584"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.05"/>
@@ -6949,10 +6945,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.22633788060443102"/>
-          <c:y val="0.93462469733656817"/>
-          <c:w val="0.50411630644934791"/>
-          <c:h val="4.842615012106511E-2"/>
+          <c:x val="0.22633788060443105"/>
+          <c:y val="0.93462469733656839"/>
+          <c:w val="0.5041163064493478"/>
+          <c:h val="4.8426150121065104E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -7018,7 +7014,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7055,8 +7051,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674008"/>
-          <c:y val="3.0232707900360201E-2"/>
+          <c:x val="0.38523037913674013"/>
+          <c:y val="3.0232707900360208E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -7072,10 +7068,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11177666498383203"/>
+          <c:x val="0.11177666498383206"/>
           <c:y val="0.100000113553908"/>
           <c:w val="0.78044064301210703"/>
-          <c:h val="0.65814028222689225"/>
+          <c:h val="0.65814028222689247"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -7137,12 +7133,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="137833088"/>
-        <c:axId val="137838976"/>
+        <c:axId val="141125504"/>
+        <c:axId val="141127040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="137833088"/>
+        <c:axId val="141125504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7176,14 +7171,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="137838976"/>
+        <c:crossAx val="141127040"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="137838976"/>
+        <c:axId val="141127040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7217,7 +7212,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="137833088"/>
+        <c:crossAx val="141125504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7267,7 +7262,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7304,8 +7299,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674008"/>
-          <c:y val="3.5190678684544313E-2"/>
+          <c:x val="0.38523037913674013"/>
+          <c:y val="3.519067868454432E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -7322,7 +7317,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="8.5828510612584605E-2"/>
-          <c:y val="0.11730205278592401"/>
+          <c:y val="0.11730205278592402"/>
           <c:w val="0.80638879738335301"/>
           <c:h val="0.55131964809384204"/>
         </c:manualLayout>
@@ -7422,12 +7417,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="137846144"/>
-        <c:axId val="137876608"/>
+        <c:axId val="141147136"/>
+        <c:axId val="142955264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="137846144"/>
+        <c:axId val="141147136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7461,14 +7455,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="137876608"/>
+        <c:crossAx val="142955264"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="137876608"/>
+        <c:axId val="142955264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7502,7 +7496,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="137846144"/>
+        <c:crossAx val="141147136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7552,7 +7546,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7589,8 +7583,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674008"/>
-          <c:y val="3.5190678684544313E-2"/>
+          <c:x val="0.38523037913674013"/>
+          <c:y val="3.519067868454432E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -7607,7 +7601,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="8.5828510612584605E-2"/>
-          <c:y val="0.11730205278592401"/>
+          <c:y val="0.11730205278592402"/>
           <c:w val="0.80638879738335301"/>
           <c:h val="0.55131964809384204"/>
         </c:manualLayout>
@@ -7707,12 +7701,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="143806848"/>
-        <c:axId val="143808384"/>
+        <c:axId val="142975360"/>
+        <c:axId val="142976896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="143806848"/>
+        <c:axId val="142975360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7746,14 +7739,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="143808384"/>
+        <c:crossAx val="142976896"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143808384"/>
+        <c:axId val="142976896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7787,7 +7780,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="143806848"/>
+        <c:crossAx val="142975360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7837,7 +7830,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7874,8 +7867,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674008"/>
-          <c:y val="3.0232707900360201E-2"/>
+          <c:x val="0.38523037913674013"/>
+          <c:y val="3.0232707900360208E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -7891,10 +7884,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11177666498383203"/>
+          <c:x val="0.11177666498383206"/>
           <c:y val="0.100000113553908"/>
           <c:w val="0.78044064301210703"/>
-          <c:h val="0.65814028222689225"/>
+          <c:h val="0.65814028222689247"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -7956,12 +7949,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="143824000"/>
-        <c:axId val="143825536"/>
+        <c:axId val="144254464"/>
+        <c:axId val="144256000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="143824000"/>
+        <c:axId val="144254464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7995,14 +7987,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="143825536"/>
+        <c:crossAx val="144256000"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143825536"/>
+        <c:axId val="144256000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8036,7 +8028,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="143824000"/>
+        <c:crossAx val="144254464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8086,7 +8078,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8836,10 +8828,10 @@
   <dimension ref="A1:AC111"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="1" topLeftCell="J29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="1" topLeftCell="J20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I43" sqref="I43"/>
+      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -10497,7 +10489,7 @@
         <v>38</v>
       </c>
       <c r="L32" s="164" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="M32" s="147"/>
       <c r="N32" s="128"/>
@@ -10599,7 +10591,7 @@
         <v>38</v>
       </c>
       <c r="L34" s="115" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="M34" s="147"/>
       <c r="N34" s="128"/>
@@ -12557,30 +12549,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="9" customHeight="1">
-      <c r="E1" s="216"/>
-      <c r="F1" s="216"/>
-      <c r="G1" s="216"/>
-      <c r="H1" s="216"/>
-      <c r="I1" s="216"/>
-      <c r="J1" s="216"/>
+      <c r="E1" s="187"/>
+      <c r="F1" s="187"/>
+      <c r="G1" s="187"/>
+      <c r="H1" s="187"/>
+      <c r="I1" s="187"/>
+      <c r="J1" s="187"/>
     </row>
     <row r="2" spans="2:10" ht="15" customHeight="1">
       <c r="B2" s="26" t="s">
         <v>128</v>
       </c>
       <c r="C2" s="26"/>
-      <c r="E2" s="216"/>
-      <c r="F2" s="216"/>
-      <c r="G2" s="216"/>
-      <c r="H2" s="216"/>
-      <c r="I2" s="216"/>
-      <c r="J2" s="216"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="187"/>
+      <c r="I2" s="187"/>
+      <c r="J2" s="187"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1">
-      <c r="B3" s="185" t="s">
+      <c r="B3" s="216" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="186"/>
+      <c r="C3" s="217"/>
       <c r="D3" s="27" t="s">
         <v>129</v>
       </c>
@@ -12658,30 +12650,30 @@
       </c>
     </row>
     <row r="13" spans="2:10" ht="17.25" customHeight="1">
-      <c r="B13" s="217" t="s">
+      <c r="B13" s="188" t="s">
         <v>134</v>
       </c>
-      <c r="C13" s="217"/>
-      <c r="D13" s="217"/>
-      <c r="E13" s="217"/>
+      <c r="C13" s="188"/>
+      <c r="D13" s="188"/>
+      <c r="E13" s="188"/>
     </row>
     <row r="14" spans="2:10" ht="17.25" customHeight="1">
-      <c r="B14" s="217"/>
-      <c r="C14" s="217"/>
-      <c r="D14" s="217"/>
-      <c r="E14" s="217"/>
+      <c r="B14" s="188"/>
+      <c r="C14" s="188"/>
+      <c r="D14" s="188"/>
+      <c r="E14" s="188"/>
     </row>
     <row r="15" spans="2:10" ht="17.25" customHeight="1">
-      <c r="B15" s="217"/>
-      <c r="C15" s="217"/>
-      <c r="D15" s="217"/>
-      <c r="E15" s="217"/>
+      <c r="B15" s="188"/>
+      <c r="C15" s="188"/>
+      <c r="D15" s="188"/>
+      <c r="E15" s="188"/>
     </row>
     <row r="16" spans="2:10" ht="17.25" customHeight="1">
-      <c r="B16" s="217"/>
-      <c r="C16" s="217"/>
-      <c r="D16" s="217"/>
-      <c r="E16" s="217"/>
+      <c r="B16" s="188"/>
+      <c r="C16" s="188"/>
+      <c r="D16" s="188"/>
+      <c r="E16" s="188"/>
     </row>
     <row r="21" spans="2:5" ht="15" customHeight="1">
       <c r="B21" s="26" t="s">
@@ -12690,10 +12682,10 @@
       <c r="C21" s="26"/>
     </row>
     <row r="22" spans="2:5" ht="15" customHeight="1">
-      <c r="B22" s="185" t="s">
+      <c r="B22" s="216" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="186"/>
+      <c r="C22" s="217"/>
       <c r="D22" s="27" t="s">
         <v>129</v>
       </c>
@@ -12875,30 +12867,30 @@
       </c>
     </row>
     <row r="36" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B36" s="217" t="s">
+      <c r="B36" s="188" t="s">
         <v>134</v>
       </c>
-      <c r="C36" s="217"/>
-      <c r="D36" s="217"/>
-      <c r="E36" s="217"/>
+      <c r="C36" s="188"/>
+      <c r="D36" s="188"/>
+      <c r="E36" s="188"/>
     </row>
     <row r="37" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B37" s="217"/>
-      <c r="C37" s="217"/>
-      <c r="D37" s="217"/>
-      <c r="E37" s="217"/>
+      <c r="B37" s="188"/>
+      <c r="C37" s="188"/>
+      <c r="D37" s="188"/>
+      <c r="E37" s="188"/>
     </row>
     <row r="38" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B38" s="217"/>
-      <c r="C38" s="217"/>
-      <c r="D38" s="217"/>
-      <c r="E38" s="217"/>
+      <c r="B38" s="188"/>
+      <c r="C38" s="188"/>
+      <c r="D38" s="188"/>
+      <c r="E38" s="188"/>
     </row>
     <row r="39" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B39" s="217"/>
-      <c r="C39" s="217"/>
-      <c r="D39" s="217"/>
-      <c r="E39" s="217"/>
+      <c r="B39" s="188"/>
+      <c r="C39" s="188"/>
+      <c r="D39" s="188"/>
+      <c r="E39" s="188"/>
     </row>
     <row r="43" spans="2:5" ht="15" customHeight="1">
       <c r="B43" s="26" t="s">
@@ -12907,10 +12899,10 @@
       <c r="C43" s="26"/>
     </row>
     <row r="44" spans="2:5" ht="15" customHeight="1">
-      <c r="B44" s="185" t="s">
+      <c r="B44" s="216" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="186"/>
+      <c r="C44" s="217"/>
       <c r="D44" s="27" t="s">
         <v>129</v>
       </c>
@@ -13064,30 +13056,30 @@
       </c>
     </row>
     <row r="56" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B56" s="217" t="s">
+      <c r="B56" s="188" t="s">
         <v>134</v>
       </c>
-      <c r="C56" s="217"/>
-      <c r="D56" s="217"/>
-      <c r="E56" s="217"/>
+      <c r="C56" s="188"/>
+      <c r="D56" s="188"/>
+      <c r="E56" s="188"/>
     </row>
     <row r="57" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B57" s="217"/>
-      <c r="C57" s="217"/>
-      <c r="D57" s="217"/>
-      <c r="E57" s="217"/>
+      <c r="B57" s="188"/>
+      <c r="C57" s="188"/>
+      <c r="D57" s="188"/>
+      <c r="E57" s="188"/>
     </row>
     <row r="58" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B58" s="217"/>
-      <c r="C58" s="217"/>
-      <c r="D58" s="217"/>
-      <c r="E58" s="217"/>
+      <c r="B58" s="188"/>
+      <c r="C58" s="188"/>
+      <c r="D58" s="188"/>
+      <c r="E58" s="188"/>
     </row>
     <row r="59" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B59" s="217"/>
-      <c r="C59" s="217"/>
-      <c r="D59" s="217"/>
-      <c r="E59" s="217"/>
+      <c r="B59" s="188"/>
+      <c r="C59" s="188"/>
+      <c r="D59" s="188"/>
+      <c r="E59" s="188"/>
     </row>
     <row r="64" spans="2:5" ht="17.25" customHeight="1">
       <c r="B64" s="26" t="s">
@@ -13096,10 +13088,10 @@
       <c r="C64" s="26"/>
     </row>
     <row r="65" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B65" s="187" t="s">
+      <c r="B65" s="209" t="s">
         <v>17</v>
       </c>
-      <c r="C65" s="188"/>
+      <c r="C65" s="210"/>
       <c r="D65" s="27" t="s">
         <v>129</v>
       </c>
@@ -13279,28 +13271,28 @@
       <c r="E79" s="24"/>
     </row>
     <row r="80" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B80" s="217" t="s">
+      <c r="B80" s="188" t="s">
         <v>173</v>
       </c>
-      <c r="C80" s="217"/>
-      <c r="D80" s="217"/>
-      <c r="E80" s="217"/>
+      <c r="C80" s="188"/>
+      <c r="D80" s="188"/>
+      <c r="E80" s="188"/>
       <c r="F80" s="24"/>
       <c r="G80" s="24"/>
     </row>
     <row r="81" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B81" s="217"/>
-      <c r="C81" s="217"/>
-      <c r="D81" s="217"/>
-      <c r="E81" s="217"/>
+      <c r="B81" s="188"/>
+      <c r="C81" s="188"/>
+      <c r="D81" s="188"/>
+      <c r="E81" s="188"/>
       <c r="F81" s="50"/>
       <c r="G81" s="50"/>
     </row>
     <row r="82" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B82" s="217"/>
-      <c r="C82" s="217"/>
-      <c r="D82" s="217"/>
-      <c r="E82" s="217"/>
+      <c r="B82" s="188"/>
+      <c r="C82" s="188"/>
+      <c r="D82" s="188"/>
+      <c r="E82" s="188"/>
       <c r="F82" s="50"/>
       <c r="G82" s="50"/>
     </row>
@@ -13319,10 +13311,10 @@
       <c r="C84" s="26"/>
     </row>
     <row r="85" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B85" s="187" t="s">
+      <c r="B85" s="209" t="s">
         <v>18</v>
       </c>
-      <c r="C85" s="188"/>
+      <c r="C85" s="210"/>
       <c r="D85" s="27" t="s">
         <v>129</v>
       </c>
@@ -13394,28 +13386,28 @@
       <c r="E90" s="24"/>
     </row>
     <row r="91" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B91" s="217" t="s">
+      <c r="B91" s="188" t="s">
         <v>173</v>
       </c>
-      <c r="C91" s="217"/>
-      <c r="D91" s="217"/>
-      <c r="E91" s="217"/>
+      <c r="C91" s="188"/>
+      <c r="D91" s="188"/>
+      <c r="E91" s="188"/>
       <c r="F91" s="24"/>
       <c r="G91" s="24"/>
     </row>
     <row r="92" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B92" s="217"/>
-      <c r="C92" s="217"/>
-      <c r="D92" s="217"/>
-      <c r="E92" s="217"/>
+      <c r="B92" s="188"/>
+      <c r="C92" s="188"/>
+      <c r="D92" s="188"/>
+      <c r="E92" s="188"/>
       <c r="F92" s="50"/>
       <c r="G92" s="50"/>
     </row>
     <row r="93" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B93" s="217"/>
-      <c r="C93" s="217"/>
-      <c r="D93" s="217"/>
-      <c r="E93" s="217"/>
+      <c r="B93" s="188"/>
+      <c r="C93" s="188"/>
+      <c r="D93" s="188"/>
+      <c r="E93" s="188"/>
       <c r="F93" s="50"/>
       <c r="G93" s="50"/>
     </row>
@@ -13434,10 +13426,10 @@
       <c r="C95" s="26"/>
     </row>
     <row r="96" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B96" s="187" t="s">
+      <c r="B96" s="209" t="s">
         <v>18</v>
       </c>
-      <c r="C96" s="188"/>
+      <c r="C96" s="210"/>
       <c r="D96" s="27" t="s">
         <v>129</v>
       </c>
@@ -13495,28 +13487,28 @@
       <c r="E100" s="24"/>
     </row>
     <row r="101" spans="1:50" ht="23.25" customHeight="1">
-      <c r="B101" s="217" t="s">
+      <c r="B101" s="188" t="s">
         <v>173</v>
       </c>
-      <c r="C101" s="217"/>
-      <c r="D101" s="217"/>
-      <c r="E101" s="217"/>
+      <c r="C101" s="188"/>
+      <c r="D101" s="188"/>
+      <c r="E101" s="188"/>
       <c r="F101" s="24"/>
       <c r="G101" s="24"/>
     </row>
     <row r="102" spans="1:50" ht="23.25" customHeight="1">
-      <c r="B102" s="217"/>
-      <c r="C102" s="217"/>
-      <c r="D102" s="217"/>
-      <c r="E102" s="217"/>
+      <c r="B102" s="188"/>
+      <c r="C102" s="188"/>
+      <c r="D102" s="188"/>
+      <c r="E102" s="188"/>
       <c r="F102" s="50"/>
       <c r="G102" s="50"/>
     </row>
     <row r="103" spans="1:50" ht="23.25" customHeight="1">
-      <c r="B103" s="217"/>
-      <c r="C103" s="217"/>
-      <c r="D103" s="217"/>
-      <c r="E103" s="217"/>
+      <c r="B103" s="188"/>
+      <c r="C103" s="188"/>
+      <c r="D103" s="188"/>
+      <c r="E103" s="188"/>
       <c r="F103" s="50"/>
       <c r="G103" s="50"/>
     </row>
@@ -13558,27 +13550,27 @@
       <c r="C106" s="55" t="s">
         <v>183</v>
       </c>
-      <c r="D106" s="189" t="s">
+      <c r="D106" s="211" t="s">
         <v>184</v>
       </c>
-      <c r="E106" s="190"/>
-      <c r="F106" s="191" t="s">
+      <c r="E106" s="212"/>
+      <c r="F106" s="213" t="s">
         <v>185</v>
       </c>
-      <c r="G106" s="192"/>
-      <c r="H106" s="193"/>
-      <c r="I106" s="191" t="s">
+      <c r="G106" s="214"/>
+      <c r="H106" s="215"/>
+      <c r="I106" s="213" t="s">
         <v>186</v>
       </c>
-      <c r="J106" s="192"/>
-      <c r="K106" s="192"/>
-      <c r="L106" s="193"/>
-      <c r="M106" s="191" t="s">
+      <c r="J106" s="214"/>
+      <c r="K106" s="214"/>
+      <c r="L106" s="215"/>
+      <c r="M106" s="213" t="s">
         <v>187</v>
       </c>
-      <c r="N106" s="192"/>
-      <c r="O106" s="192"/>
-      <c r="P106" s="193"/>
+      <c r="N106" s="214"/>
+      <c r="O106" s="214"/>
+      <c r="P106" s="215"/>
       <c r="Q106" s="63" t="s">
         <v>188</v>
       </c>
@@ -13599,27 +13591,27 @@
       <c r="C107" s="57" t="s">
         <v>191</v>
       </c>
-      <c r="D107" s="194" t="s">
+      <c r="D107" s="203" t="s">
         <v>192</v>
       </c>
-      <c r="E107" s="195"/>
-      <c r="F107" s="196" t="s">
+      <c r="E107" s="204"/>
+      <c r="F107" s="205" t="s">
         <v>193</v>
       </c>
-      <c r="G107" s="197"/>
-      <c r="H107" s="198"/>
-      <c r="I107" s="196" t="s">
+      <c r="G107" s="206"/>
+      <c r="H107" s="207"/>
+      <c r="I107" s="205" t="s">
         <v>194</v>
       </c>
-      <c r="J107" s="197"/>
-      <c r="K107" s="197"/>
-      <c r="L107" s="198"/>
-      <c r="M107" s="199" t="s">
+      <c r="J107" s="206"/>
+      <c r="K107" s="206"/>
+      <c r="L107" s="207"/>
+      <c r="M107" s="208" t="s">
         <v>195</v>
       </c>
-      <c r="N107" s="199"/>
-      <c r="O107" s="199"/>
-      <c r="P107" s="199"/>
+      <c r="N107" s="208"/>
+      <c r="O107" s="208"/>
+      <c r="P107" s="208"/>
       <c r="Q107" s="71" t="s">
         <v>196</v>
       </c>
@@ -13636,19 +13628,19 @@
     <row r="108" spans="1:50" s="23" customFormat="1" ht="11.25">
       <c r="B108" s="58"/>
       <c r="C108" s="59"/>
-      <c r="D108" s="200"/>
-      <c r="E108" s="201"/>
-      <c r="F108" s="202"/>
-      <c r="G108" s="203"/>
-      <c r="H108" s="204"/>
-      <c r="I108" s="202"/>
-      <c r="J108" s="203"/>
-      <c r="K108" s="203"/>
-      <c r="L108" s="204"/>
-      <c r="M108" s="205"/>
-      <c r="N108" s="205"/>
-      <c r="O108" s="205"/>
-      <c r="P108" s="205"/>
+      <c r="D108" s="197"/>
+      <c r="E108" s="198"/>
+      <c r="F108" s="199"/>
+      <c r="G108" s="200"/>
+      <c r="H108" s="201"/>
+      <c r="I108" s="199"/>
+      <c r="J108" s="200"/>
+      <c r="K108" s="200"/>
+      <c r="L108" s="201"/>
+      <c r="M108" s="202"/>
+      <c r="N108" s="202"/>
+      <c r="O108" s="202"/>
+      <c r="P108" s="202"/>
       <c r="Q108" s="73"/>
       <c r="R108" s="74"/>
       <c r="U108" s="70"/>
@@ -13661,19 +13653,19 @@
     <row r="109" spans="1:50" s="23" customFormat="1" ht="11.25">
       <c r="B109" s="58"/>
       <c r="C109" s="59"/>
-      <c r="D109" s="200"/>
-      <c r="E109" s="201"/>
-      <c r="F109" s="202"/>
-      <c r="G109" s="203"/>
-      <c r="H109" s="204"/>
-      <c r="I109" s="202"/>
-      <c r="J109" s="203"/>
-      <c r="K109" s="203"/>
-      <c r="L109" s="204"/>
-      <c r="M109" s="205"/>
-      <c r="N109" s="205"/>
-      <c r="O109" s="205"/>
-      <c r="P109" s="205"/>
+      <c r="D109" s="197"/>
+      <c r="E109" s="198"/>
+      <c r="F109" s="199"/>
+      <c r="G109" s="200"/>
+      <c r="H109" s="201"/>
+      <c r="I109" s="199"/>
+      <c r="J109" s="200"/>
+      <c r="K109" s="200"/>
+      <c r="L109" s="201"/>
+      <c r="M109" s="202"/>
+      <c r="N109" s="202"/>
+      <c r="O109" s="202"/>
+      <c r="P109" s="202"/>
       <c r="Q109" s="73"/>
       <c r="R109" s="74"/>
       <c r="U109" s="70"/>
@@ -13686,19 +13678,19 @@
     <row r="110" spans="1:50" s="23" customFormat="1" ht="11.25">
       <c r="B110" s="58"/>
       <c r="C110" s="59"/>
-      <c r="D110" s="200"/>
-      <c r="E110" s="201"/>
-      <c r="F110" s="202"/>
-      <c r="G110" s="203"/>
-      <c r="H110" s="204"/>
-      <c r="I110" s="202"/>
-      <c r="J110" s="203"/>
-      <c r="K110" s="203"/>
-      <c r="L110" s="204"/>
-      <c r="M110" s="205"/>
-      <c r="N110" s="205"/>
-      <c r="O110" s="205"/>
-      <c r="P110" s="205"/>
+      <c r="D110" s="197"/>
+      <c r="E110" s="198"/>
+      <c r="F110" s="199"/>
+      <c r="G110" s="200"/>
+      <c r="H110" s="201"/>
+      <c r="I110" s="199"/>
+      <c r="J110" s="200"/>
+      <c r="K110" s="200"/>
+      <c r="L110" s="201"/>
+      <c r="M110" s="202"/>
+      <c r="N110" s="202"/>
+      <c r="O110" s="202"/>
+      <c r="P110" s="202"/>
       <c r="Q110" s="73"/>
       <c r="R110" s="74"/>
       <c r="U110" s="70"/>
@@ -13711,19 +13703,19 @@
     <row r="111" spans="1:50" s="23" customFormat="1" ht="11.25">
       <c r="B111" s="58"/>
       <c r="C111" s="59"/>
-      <c r="D111" s="200"/>
-      <c r="E111" s="201"/>
-      <c r="F111" s="202"/>
-      <c r="G111" s="203"/>
-      <c r="H111" s="204"/>
-      <c r="I111" s="202"/>
-      <c r="J111" s="203"/>
-      <c r="K111" s="203"/>
-      <c r="L111" s="204"/>
-      <c r="M111" s="205"/>
-      <c r="N111" s="205"/>
-      <c r="O111" s="205"/>
-      <c r="P111" s="205"/>
+      <c r="D111" s="197"/>
+      <c r="E111" s="198"/>
+      <c r="F111" s="199"/>
+      <c r="G111" s="200"/>
+      <c r="H111" s="201"/>
+      <c r="I111" s="199"/>
+      <c r="J111" s="200"/>
+      <c r="K111" s="200"/>
+      <c r="L111" s="201"/>
+      <c r="M111" s="202"/>
+      <c r="N111" s="202"/>
+      <c r="O111" s="202"/>
+      <c r="P111" s="202"/>
       <c r="Q111" s="73"/>
       <c r="R111" s="74"/>
       <c r="U111" s="70"/>
@@ -13736,19 +13728,19 @@
     <row r="112" spans="1:50" s="23" customFormat="1" ht="11.25">
       <c r="B112" s="58"/>
       <c r="C112" s="59"/>
-      <c r="D112" s="200"/>
-      <c r="E112" s="201"/>
-      <c r="F112" s="202"/>
-      <c r="G112" s="203"/>
-      <c r="H112" s="204"/>
-      <c r="I112" s="202"/>
-      <c r="J112" s="203"/>
-      <c r="K112" s="203"/>
-      <c r="L112" s="204"/>
-      <c r="M112" s="205"/>
-      <c r="N112" s="205"/>
-      <c r="O112" s="205"/>
-      <c r="P112" s="205"/>
+      <c r="D112" s="197"/>
+      <c r="E112" s="198"/>
+      <c r="F112" s="199"/>
+      <c r="G112" s="200"/>
+      <c r="H112" s="201"/>
+      <c r="I112" s="199"/>
+      <c r="J112" s="200"/>
+      <c r="K112" s="200"/>
+      <c r="L112" s="201"/>
+      <c r="M112" s="202"/>
+      <c r="N112" s="202"/>
+      <c r="O112" s="202"/>
+      <c r="P112" s="202"/>
       <c r="Q112" s="73"/>
       <c r="R112" s="74"/>
       <c r="U112" s="70"/>
@@ -13761,19 +13753,19 @@
     <row r="113" spans="2:26" s="23" customFormat="1" ht="11.25">
       <c r="B113" s="58"/>
       <c r="C113" s="59"/>
-      <c r="D113" s="200"/>
-      <c r="E113" s="201"/>
-      <c r="F113" s="202"/>
-      <c r="G113" s="203"/>
-      <c r="H113" s="204"/>
-      <c r="I113" s="202"/>
-      <c r="J113" s="203"/>
-      <c r="K113" s="203"/>
-      <c r="L113" s="204"/>
-      <c r="M113" s="205"/>
-      <c r="N113" s="205"/>
-      <c r="O113" s="205"/>
-      <c r="P113" s="205"/>
+      <c r="D113" s="197"/>
+      <c r="E113" s="198"/>
+      <c r="F113" s="199"/>
+      <c r="G113" s="200"/>
+      <c r="H113" s="201"/>
+      <c r="I113" s="199"/>
+      <c r="J113" s="200"/>
+      <c r="K113" s="200"/>
+      <c r="L113" s="201"/>
+      <c r="M113" s="202"/>
+      <c r="N113" s="202"/>
+      <c r="O113" s="202"/>
+      <c r="P113" s="202"/>
       <c r="Q113" s="73"/>
       <c r="R113" s="74"/>
       <c r="U113" s="70"/>
@@ -13786,19 +13778,19 @@
     <row r="114" spans="2:26" s="23" customFormat="1" ht="11.25">
       <c r="B114" s="58"/>
       <c r="C114" s="59"/>
-      <c r="D114" s="200"/>
-      <c r="E114" s="201"/>
-      <c r="F114" s="202"/>
-      <c r="G114" s="203"/>
-      <c r="H114" s="204"/>
-      <c r="I114" s="202"/>
-      <c r="J114" s="203"/>
-      <c r="K114" s="203"/>
-      <c r="L114" s="204"/>
-      <c r="M114" s="205"/>
-      <c r="N114" s="205"/>
-      <c r="O114" s="205"/>
-      <c r="P114" s="205"/>
+      <c r="D114" s="197"/>
+      <c r="E114" s="198"/>
+      <c r="F114" s="199"/>
+      <c r="G114" s="200"/>
+      <c r="H114" s="201"/>
+      <c r="I114" s="199"/>
+      <c r="J114" s="200"/>
+      <c r="K114" s="200"/>
+      <c r="L114" s="201"/>
+      <c r="M114" s="202"/>
+      <c r="N114" s="202"/>
+      <c r="O114" s="202"/>
+      <c r="P114" s="202"/>
       <c r="Q114" s="73"/>
       <c r="R114" s="74"/>
       <c r="U114" s="70"/>
@@ -13811,19 +13803,19 @@
     <row r="115" spans="2:26" s="23" customFormat="1" ht="11.25">
       <c r="B115" s="58"/>
       <c r="C115" s="59"/>
-      <c r="D115" s="200"/>
-      <c r="E115" s="201"/>
-      <c r="F115" s="202"/>
-      <c r="G115" s="203"/>
-      <c r="H115" s="204"/>
-      <c r="I115" s="202"/>
-      <c r="J115" s="203"/>
-      <c r="K115" s="203"/>
-      <c r="L115" s="204"/>
-      <c r="M115" s="205"/>
-      <c r="N115" s="205"/>
-      <c r="O115" s="205"/>
-      <c r="P115" s="205"/>
+      <c r="D115" s="197"/>
+      <c r="E115" s="198"/>
+      <c r="F115" s="199"/>
+      <c r="G115" s="200"/>
+      <c r="H115" s="201"/>
+      <c r="I115" s="199"/>
+      <c r="J115" s="200"/>
+      <c r="K115" s="200"/>
+      <c r="L115" s="201"/>
+      <c r="M115" s="202"/>
+      <c r="N115" s="202"/>
+      <c r="O115" s="202"/>
+      <c r="P115" s="202"/>
       <c r="Q115" s="73"/>
       <c r="R115" s="74"/>
       <c r="U115" s="70"/>
@@ -13836,19 +13828,19 @@
     <row r="116" spans="2:26" s="23" customFormat="1" ht="11.25">
       <c r="B116" s="58"/>
       <c r="C116" s="59"/>
-      <c r="D116" s="200"/>
-      <c r="E116" s="201"/>
-      <c r="F116" s="202"/>
-      <c r="G116" s="203"/>
-      <c r="H116" s="204"/>
-      <c r="I116" s="202"/>
-      <c r="J116" s="203"/>
-      <c r="K116" s="203"/>
-      <c r="L116" s="204"/>
-      <c r="M116" s="205"/>
-      <c r="N116" s="205"/>
-      <c r="O116" s="205"/>
-      <c r="P116" s="205"/>
+      <c r="D116" s="197"/>
+      <c r="E116" s="198"/>
+      <c r="F116" s="199"/>
+      <c r="G116" s="200"/>
+      <c r="H116" s="201"/>
+      <c r="I116" s="199"/>
+      <c r="J116" s="200"/>
+      <c r="K116" s="200"/>
+      <c r="L116" s="201"/>
+      <c r="M116" s="202"/>
+      <c r="N116" s="202"/>
+      <c r="O116" s="202"/>
+      <c r="P116" s="202"/>
       <c r="Q116" s="73"/>
       <c r="R116" s="74"/>
       <c r="U116" s="70"/>
@@ -13875,32 +13867,32 @@
       <c r="G118" s="50"/>
     </row>
     <row r="119" spans="2:26" ht="17.25" customHeight="1">
-      <c r="B119" s="211" t="s">
+      <c r="B119" s="189" t="s">
         <v>183</v>
       </c>
-      <c r="C119" s="211" t="s">
+      <c r="C119" s="189" t="s">
         <v>198</v>
       </c>
-      <c r="D119" s="211" t="s">
+      <c r="D119" s="189" t="s">
         <v>199</v>
       </c>
-      <c r="E119" s="211" t="s">
+      <c r="E119" s="189" t="s">
         <v>200</v>
       </c>
-      <c r="F119" s="213" t="s">
+      <c r="F119" s="191" t="s">
         <v>201</v>
       </c>
-      <c r="G119" s="214" t="s">
+      <c r="G119" s="185" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="120" spans="2:26" ht="17.25" customHeight="1">
-      <c r="B120" s="212"/>
-      <c r="C120" s="212"/>
-      <c r="D120" s="212"/>
-      <c r="E120" s="212"/>
-      <c r="F120" s="213"/>
-      <c r="G120" s="215"/>
+      <c r="B120" s="190"/>
+      <c r="C120" s="190"/>
+      <c r="D120" s="190"/>
+      <c r="E120" s="190"/>
+      <c r="F120" s="191"/>
+      <c r="G120" s="186"/>
     </row>
     <row r="121" spans="2:26" ht="17.25" customHeight="1">
       <c r="B121" s="64">
@@ -14316,19 +14308,19 @@
       <c r="L137" s="88"/>
     </row>
     <row r="138" spans="2:13" s="24" customFormat="1" ht="59.25" customHeight="1">
-      <c r="B138" s="206" t="s">
+      <c r="B138" s="194" t="s">
         <v>203</v>
       </c>
-      <c r="C138" s="206"/>
-      <c r="D138" s="206"/>
-      <c r="E138" s="206"/>
-      <c r="F138" s="206"/>
-      <c r="G138" s="206"/>
-      <c r="H138" s="206"/>
-      <c r="I138" s="206"/>
-      <c r="J138" s="206"/>
-      <c r="K138" s="206"/>
-      <c r="L138" s="206"/>
+      <c r="C138" s="194"/>
+      <c r="D138" s="194"/>
+      <c r="E138" s="194"/>
+      <c r="F138" s="194"/>
+      <c r="G138" s="194"/>
+      <c r="H138" s="194"/>
+      <c r="I138" s="194"/>
+      <c r="J138" s="194"/>
+      <c r="K138" s="194"/>
+      <c r="L138" s="194"/>
     </row>
     <row r="139" spans="2:13" s="24" customFormat="1" ht="12" customHeight="1">
       <c r="B139" s="82"/>
@@ -14365,20 +14357,20 @@
       <c r="C141" s="84" t="s">
         <v>205</v>
       </c>
-      <c r="D141" s="207" t="s">
+      <c r="D141" s="195" t="s">
         <v>206</v>
       </c>
-      <c r="E141" s="207"/>
-      <c r="F141" s="207"/>
-      <c r="G141" s="207"/>
-      <c r="H141" s="208" t="s">
+      <c r="E141" s="195"/>
+      <c r="F141" s="195"/>
+      <c r="G141" s="195"/>
+      <c r="H141" s="196" t="s">
         <v>11</v>
       </c>
-      <c r="I141" s="208"/>
-      <c r="J141" s="208"/>
-      <c r="K141" s="208"/>
-      <c r="L141" s="208"/>
-      <c r="M141" s="208"/>
+      <c r="I141" s="196"/>
+      <c r="J141" s="196"/>
+      <c r="K141" s="196"/>
+      <c r="L141" s="196"/>
+      <c r="M141" s="196"/>
     </row>
     <row r="142" spans="2:13" s="24" customFormat="1" ht="14.25" customHeight="1">
       <c r="B142" s="85">
@@ -14387,61 +14379,119 @@
       <c r="C142" s="86" t="s">
         <v>207</v>
       </c>
-      <c r="D142" s="209"/>
-      <c r="E142" s="209"/>
-      <c r="F142" s="209"/>
-      <c r="G142" s="209"/>
-      <c r="H142" s="210"/>
-      <c r="I142" s="210"/>
-      <c r="J142" s="210"/>
-      <c r="K142" s="210"/>
-      <c r="L142" s="210"/>
-      <c r="M142" s="210"/>
+      <c r="D142" s="192"/>
+      <c r="E142" s="192"/>
+      <c r="F142" s="192"/>
+      <c r="G142" s="192"/>
+      <c r="H142" s="193"/>
+      <c r="I142" s="193"/>
+      <c r="J142" s="193"/>
+      <c r="K142" s="193"/>
+      <c r="L142" s="193"/>
+      <c r="M142" s="193"/>
     </row>
     <row r="143" spans="2:13" s="24" customFormat="1" ht="14.25" customHeight="1">
       <c r="B143" s="85"/>
       <c r="C143" s="86"/>
-      <c r="D143" s="209"/>
-      <c r="E143" s="209"/>
-      <c r="F143" s="209"/>
-      <c r="G143" s="209"/>
-      <c r="H143" s="210"/>
-      <c r="I143" s="210"/>
-      <c r="J143" s="210"/>
-      <c r="K143" s="210"/>
-      <c r="L143" s="210"/>
-      <c r="M143" s="210"/>
+      <c r="D143" s="192"/>
+      <c r="E143" s="192"/>
+      <c r="F143" s="192"/>
+      <c r="G143" s="192"/>
+      <c r="H143" s="193"/>
+      <c r="I143" s="193"/>
+      <c r="J143" s="193"/>
+      <c r="K143" s="193"/>
+      <c r="L143" s="193"/>
+      <c r="M143" s="193"/>
     </row>
     <row r="144" spans="2:13" s="24" customFormat="1" ht="14.25" customHeight="1">
       <c r="B144" s="85"/>
       <c r="C144" s="86"/>
-      <c r="D144" s="209"/>
-      <c r="E144" s="209"/>
-      <c r="F144" s="209"/>
-      <c r="G144" s="209"/>
-      <c r="H144" s="210"/>
-      <c r="I144" s="210"/>
-      <c r="J144" s="210"/>
-      <c r="K144" s="210"/>
-      <c r="L144" s="210"/>
-      <c r="M144" s="210"/>
+      <c r="D144" s="192"/>
+      <c r="E144" s="192"/>
+      <c r="F144" s="192"/>
+      <c r="G144" s="192"/>
+      <c r="H144" s="193"/>
+      <c r="I144" s="193"/>
+      <c r="J144" s="193"/>
+      <c r="K144" s="193"/>
+      <c r="L144" s="193"/>
+      <c r="M144" s="193"/>
     </row>
     <row r="145" spans="2:13" s="24" customFormat="1" ht="14.25" customHeight="1">
       <c r="B145" s="85"/>
       <c r="C145" s="86"/>
-      <c r="D145" s="209"/>
-      <c r="E145" s="209"/>
-      <c r="F145" s="209"/>
-      <c r="G145" s="209"/>
-      <c r="H145" s="210"/>
-      <c r="I145" s="210"/>
-      <c r="J145" s="210"/>
-      <c r="K145" s="210"/>
-      <c r="L145" s="210"/>
-      <c r="M145" s="210"/>
+      <c r="D145" s="192"/>
+      <c r="E145" s="192"/>
+      <c r="F145" s="192"/>
+      <c r="G145" s="192"/>
+      <c r="H145" s="193"/>
+      <c r="I145" s="193"/>
+      <c r="J145" s="193"/>
+      <c r="K145" s="193"/>
+      <c r="L145" s="193"/>
+      <c r="M145" s="193"/>
     </row>
   </sheetData>
   <mergeCells count="74">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="F106:H106"/>
+    <mergeCell ref="I106:L106"/>
+    <mergeCell ref="M106:P106"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="F107:H107"/>
+    <mergeCell ref="I107:L107"/>
+    <mergeCell ref="M107:P107"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="I108:L108"/>
+    <mergeCell ref="M108:P108"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="F109:H109"/>
+    <mergeCell ref="I109:L109"/>
+    <mergeCell ref="M109:P109"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="F110:H110"/>
+    <mergeCell ref="I110:L110"/>
+    <mergeCell ref="M110:P110"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="F111:H111"/>
+    <mergeCell ref="I111:L111"/>
+    <mergeCell ref="M111:P111"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="F112:H112"/>
+    <mergeCell ref="I112:L112"/>
+    <mergeCell ref="M112:P112"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="F113:H113"/>
+    <mergeCell ref="I113:L113"/>
+    <mergeCell ref="M113:P113"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="F114:H114"/>
+    <mergeCell ref="I114:L114"/>
+    <mergeCell ref="M114:P114"/>
+    <mergeCell ref="M115:P115"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="F116:H116"/>
+    <mergeCell ref="I116:L116"/>
+    <mergeCell ref="M116:P116"/>
+    <mergeCell ref="B138:L138"/>
+    <mergeCell ref="D141:G141"/>
+    <mergeCell ref="H141:M141"/>
+    <mergeCell ref="D142:G142"/>
+    <mergeCell ref="H142:M142"/>
+    <mergeCell ref="D143:G143"/>
+    <mergeCell ref="H143:M143"/>
+    <mergeCell ref="D144:G144"/>
+    <mergeCell ref="H144:M144"/>
+    <mergeCell ref="D145:G145"/>
+    <mergeCell ref="H145:M145"/>
     <mergeCell ref="G119:G120"/>
     <mergeCell ref="E1:J2"/>
     <mergeCell ref="B80:E82"/>
@@ -14455,67 +14505,9 @@
     <mergeCell ref="D119:D120"/>
     <mergeCell ref="E119:E120"/>
     <mergeCell ref="F119:F120"/>
-    <mergeCell ref="D143:G143"/>
-    <mergeCell ref="H143:M143"/>
-    <mergeCell ref="D144:G144"/>
-    <mergeCell ref="H144:M144"/>
-    <mergeCell ref="D145:G145"/>
-    <mergeCell ref="H145:M145"/>
-    <mergeCell ref="B138:L138"/>
-    <mergeCell ref="D141:G141"/>
-    <mergeCell ref="H141:M141"/>
-    <mergeCell ref="D142:G142"/>
-    <mergeCell ref="H142:M142"/>
     <mergeCell ref="D115:E115"/>
     <mergeCell ref="F115:H115"/>
     <mergeCell ref="I115:L115"/>
-    <mergeCell ref="M115:P115"/>
-    <mergeCell ref="D116:E116"/>
-    <mergeCell ref="F116:H116"/>
-    <mergeCell ref="I116:L116"/>
-    <mergeCell ref="M116:P116"/>
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="F113:H113"/>
-    <mergeCell ref="I113:L113"/>
-    <mergeCell ref="M113:P113"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="F114:H114"/>
-    <mergeCell ref="I114:L114"/>
-    <mergeCell ref="M114:P114"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="F111:H111"/>
-    <mergeCell ref="I111:L111"/>
-    <mergeCell ref="M111:P111"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="F112:H112"/>
-    <mergeCell ref="I112:L112"/>
-    <mergeCell ref="M112:P112"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="I109:L109"/>
-    <mergeCell ref="M109:P109"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="F110:H110"/>
-    <mergeCell ref="I110:L110"/>
-    <mergeCell ref="M110:P110"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="F107:H107"/>
-    <mergeCell ref="I107:L107"/>
-    <mergeCell ref="M107:P107"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="F108:H108"/>
-    <mergeCell ref="I108:L108"/>
-    <mergeCell ref="M108:P108"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="F106:H106"/>
-    <mergeCell ref="I106:L106"/>
-    <mergeCell ref="M106:P106"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B85:C85"/>
   </mergeCells>
   <phoneticPr fontId="52" type="noConversion"/>
   <pageMargins left="0.78680555555555598" right="0.78680555555555598" top="0.98263888888888895" bottom="0.98263888888888895" header="0.51180555555555596" footer="0.51180555555555596"/>

</xml_diff>

<commit_message>
update WBS Signed-off-by: LiuYiyang <lyy@shequchina.cn>
</commit_message>
<xml_diff>
--- a/document/AP_障害管理票_QDYL.xlsx
+++ b/document/AP_障害管理票_QDYL.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27765" windowHeight="13650" tabRatio="490"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="222">
   <si>
     <t>通番</t>
   </si>
@@ -2867,6 +2867,281 @@
       <t>秒</t>
     </r>
     <phoneticPr fontId="52" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>今日早晨更新areaparking代</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>码后发现项目主页</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>home无法打</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>开，见</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>No.002-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>图</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>013。且数据</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>库</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>有</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>变动</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，其中一</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>处变动</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>删</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>除表ap_waiting_contact,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>对测试</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>工作有较大影</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>响</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>。具体影</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>响为</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>所有包含此表的EXCEL的IN_DB都需要修改并重新</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>检查测试</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>。因主</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>页</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>home无法</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>显</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>示，故退回6月26日19:20的代</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>码</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>版本以</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>继续测试</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>工作，IN_DB中表ap_waiting_contact未作修改。</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2885,7 +3160,7 @@
     <numFmt numFmtId="182" formatCode="0.0_ "/>
     <numFmt numFmtId="183" formatCode="0_ "/>
   </numFmts>
-  <fonts count="55">
+  <fonts count="65">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -3224,6 +3499,80 @@
       <color theme="0" tint="-0.499984740745262"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="ＭＳ ゴシック"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Meiryo UI"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -3577,7 +3926,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="346">
+  <cellStyleXfs count="460">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
@@ -4151,8 +4500,189 @@
     <xf numFmtId="43" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
+    <xf numFmtId="38" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="38" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="64" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="64" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="64" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="64" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="64" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="64" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="64" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="64" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="218">
+  <cellXfs count="219">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4716,6 +5246,84 @@
     <xf numFmtId="180" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="181" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="181" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4737,86 +5345,11 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="180" fontId="15" fillId="0" borderId="25" xfId="346" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="346">
+  <cellStyles count="460">
     <cellStyle name="Comma [0]" xfId="46"/>
     <cellStyle name="Comma [0] 2" xfId="17"/>
     <cellStyle name="Comma [0] 3" xfId="10"/>
@@ -4831,142 +5364,190 @@
     <cellStyle name="ハイパーリンク 2 2 2" xfId="22"/>
     <cellStyle name="ハイパーリンク 2 2 2 2" xfId="56"/>
     <cellStyle name="ハイパーリンク 2 2 2 2 2" xfId="41"/>
+    <cellStyle name="ハイパーリンク 2 2 2 2 3" xfId="350"/>
     <cellStyle name="ハイパーリンク 2 2 2 3" xfId="57"/>
+    <cellStyle name="ハイパーリンク 2 2 2 4" xfId="349"/>
     <cellStyle name="ハイパーリンク 2 2 3" xfId="14"/>
     <cellStyle name="ハイパーリンク 2 2 3 2" xfId="58"/>
+    <cellStyle name="ハイパーリンク 2 2 3 3" xfId="351"/>
     <cellStyle name="ハイパーリンク 2 2 4" xfId="59"/>
     <cellStyle name="ハイパーリンク 2 2 5" xfId="61"/>
     <cellStyle name="ハイパーリンク 2 2 6" xfId="62"/>
+    <cellStyle name="ハイパーリンク 2 2 7" xfId="348"/>
     <cellStyle name="ハイパーリンク 2 3" xfId="63"/>
     <cellStyle name="ハイパーリンク 2 3 2" xfId="66"/>
     <cellStyle name="ハイパーリンク 2 3 2 2" xfId="67"/>
     <cellStyle name="ハイパーリンク 2 3 2 3" xfId="48"/>
     <cellStyle name="ハイパーリンク 2 3 2 4" xfId="69"/>
+    <cellStyle name="ハイパーリンク 2 3 2 5" xfId="353"/>
     <cellStyle name="ハイパーリンク 2 3 3" xfId="72"/>
     <cellStyle name="ハイパーリンク 2 3 4" xfId="74"/>
     <cellStyle name="ハイパーリンク 2 3 5" xfId="53"/>
+    <cellStyle name="ハイパーリンク 2 3 6" xfId="352"/>
     <cellStyle name="ハイパーリンク 2 4" xfId="75"/>
     <cellStyle name="ハイパーリンク 2 4 2" xfId="77"/>
+    <cellStyle name="ハイパーリンク 2 4 3" xfId="354"/>
     <cellStyle name="ハイパーリンク 2 5" xfId="78"/>
     <cellStyle name="ハイパーリンク 2 6" xfId="79"/>
     <cellStyle name="ハイパーリンク 2 7" xfId="80"/>
+    <cellStyle name="ハイパーリンク 2 8" xfId="347"/>
     <cellStyle name="標準 2" xfId="82"/>
     <cellStyle name="標準 2 2" xfId="83"/>
     <cellStyle name="標準 2 2 2" xfId="84"/>
     <cellStyle name="標準 2 2 2 2" xfId="85"/>
     <cellStyle name="標準 2 2 2 2 2" xfId="86"/>
     <cellStyle name="標準 2 2 2 2 2 2" xfId="87"/>
+    <cellStyle name="標準 2 2 2 2 2 3" xfId="359"/>
     <cellStyle name="標準 2 2 2 2 3" xfId="88"/>
+    <cellStyle name="標準 2 2 2 2 4" xfId="358"/>
     <cellStyle name="標準 2 2 2 3" xfId="89"/>
     <cellStyle name="標準 2 2 2 3 2" xfId="90"/>
+    <cellStyle name="標準 2 2 2 3 3" xfId="360"/>
     <cellStyle name="標準 2 2 2 4" xfId="92"/>
     <cellStyle name="標準 2 2 2 5" xfId="93"/>
     <cellStyle name="標準 2 2 2 6" xfId="94"/>
+    <cellStyle name="標準 2 2 2 7" xfId="357"/>
     <cellStyle name="標準 2 2 3" xfId="95"/>
     <cellStyle name="標準 2 2 3 2" xfId="97"/>
     <cellStyle name="標準 2 2 3 2 2" xfId="99"/>
     <cellStyle name="標準 2 2 3 2 3" xfId="100"/>
     <cellStyle name="標準 2 2 3 2 4" xfId="101"/>
+    <cellStyle name="標準 2 2 3 2 5" xfId="362"/>
     <cellStyle name="標準 2 2 3 3" xfId="103"/>
     <cellStyle name="標準 2 2 3 4" xfId="105"/>
     <cellStyle name="標準 2 2 3 5" xfId="31"/>
+    <cellStyle name="標準 2 2 3 6" xfId="361"/>
     <cellStyle name="標準 2 2 4" xfId="106"/>
     <cellStyle name="標準 2 2 4 2" xfId="108"/>
+    <cellStyle name="標準 2 2 4 3" xfId="363"/>
     <cellStyle name="標準 2 2 5" xfId="109"/>
     <cellStyle name="標準 2 2 6" xfId="110"/>
     <cellStyle name="標準 2 2 7" xfId="111"/>
+    <cellStyle name="標準 2 2 8" xfId="356"/>
     <cellStyle name="標準 2 3" xfId="112"/>
     <cellStyle name="標準 2 3 2" xfId="42"/>
     <cellStyle name="標準 2 3 2 2" xfId="114"/>
     <cellStyle name="標準 2 3 2 2 2" xfId="116"/>
+    <cellStyle name="標準 2 3 2 2 3" xfId="366"/>
     <cellStyle name="標準 2 3 2 3" xfId="45"/>
+    <cellStyle name="標準 2 3 2 4" xfId="365"/>
     <cellStyle name="標準 2 3 3" xfId="43"/>
     <cellStyle name="標準 2 3 3 2" xfId="117"/>
+    <cellStyle name="標準 2 3 3 3" xfId="367"/>
     <cellStyle name="標準 2 3 4" xfId="118"/>
     <cellStyle name="標準 2 3 5" xfId="119"/>
     <cellStyle name="標準 2 3 6" xfId="120"/>
+    <cellStyle name="標準 2 3 7" xfId="364"/>
     <cellStyle name="標準 2 4" xfId="121"/>
     <cellStyle name="標準 2 4 2" xfId="122"/>
     <cellStyle name="標準 2 4 2 2" xfId="123"/>
     <cellStyle name="標準 2 4 2 3" xfId="124"/>
     <cellStyle name="標準 2 4 2 4" xfId="126"/>
+    <cellStyle name="標準 2 4 2 5" xfId="369"/>
     <cellStyle name="標準 2 4 3" xfId="2"/>
     <cellStyle name="標準 2 4 4" xfId="127"/>
     <cellStyle name="標準 2 4 5" xfId="129"/>
+    <cellStyle name="標準 2 4 6" xfId="368"/>
     <cellStyle name="標準 2 5" xfId="130"/>
     <cellStyle name="標準 2 5 2" xfId="131"/>
+    <cellStyle name="標準 2 5 3" xfId="370"/>
     <cellStyle name="標準 2 6" xfId="20"/>
     <cellStyle name="標準 2 7" xfId="133"/>
     <cellStyle name="標準 2 8" xfId="135"/>
+    <cellStyle name="標準 2 9" xfId="355"/>
     <cellStyle name="標準 2_大興電子様向け）単価マスタ管理システム（ネタ)fukunaga" xfId="37"/>
     <cellStyle name="標準 26" xfId="16"/>
     <cellStyle name="標準 26 2" xfId="136"/>
     <cellStyle name="標準 26 2 2" xfId="137"/>
     <cellStyle name="標準 26 2 2 2" xfId="139"/>
+    <cellStyle name="標準 26 2 2 3" xfId="373"/>
     <cellStyle name="標準 26 2 3" xfId="141"/>
+    <cellStyle name="標準 26 2 4" xfId="372"/>
     <cellStyle name="標準 26 3" xfId="142"/>
     <cellStyle name="標準 26 3 2" xfId="143"/>
+    <cellStyle name="標準 26 3 3" xfId="374"/>
     <cellStyle name="標準 26 4" xfId="145"/>
     <cellStyle name="標準 26 5" xfId="147"/>
     <cellStyle name="標準 26 6" xfId="150"/>
+    <cellStyle name="標準 26 7" xfId="371"/>
     <cellStyle name="標準 3" xfId="152"/>
     <cellStyle name="標準 3 2" xfId="153"/>
     <cellStyle name="標準 3 2 2" xfId="154"/>
     <cellStyle name="標準 3 2 2 2" xfId="156"/>
     <cellStyle name="標準 3 2 2 2 2" xfId="23"/>
+    <cellStyle name="標準 3 2 2 2 3" xfId="378"/>
     <cellStyle name="標準 3 2 2 3" xfId="158"/>
+    <cellStyle name="標準 3 2 2 4" xfId="377"/>
     <cellStyle name="標準 3 2 3" xfId="159"/>
     <cellStyle name="標準 3 2 3 2" xfId="161"/>
+    <cellStyle name="標準 3 2 3 3" xfId="379"/>
     <cellStyle name="標準 3 2 4" xfId="155"/>
     <cellStyle name="標準 3 2 5" xfId="157"/>
     <cellStyle name="標準 3 2 6" xfId="162"/>
+    <cellStyle name="標準 3 2 7" xfId="376"/>
     <cellStyle name="標準 3 3" xfId="163"/>
     <cellStyle name="標準 3 3 2" xfId="164"/>
     <cellStyle name="標準 3 3 2 2" xfId="149"/>
     <cellStyle name="標準 3 3 2 3" xfId="166"/>
     <cellStyle name="標準 3 3 2 4" xfId="168"/>
+    <cellStyle name="標準 3 3 2 5" xfId="381"/>
     <cellStyle name="標準 3 3 3" xfId="169"/>
     <cellStyle name="標準 3 3 4" xfId="160"/>
     <cellStyle name="標準 3 3 5" xfId="170"/>
+    <cellStyle name="標準 3 3 6" xfId="380"/>
     <cellStyle name="標準 3 4" xfId="171"/>
     <cellStyle name="標準 3 4 2" xfId="172"/>
+    <cellStyle name="標準 3 4 3" xfId="382"/>
     <cellStyle name="標準 3 5" xfId="173"/>
     <cellStyle name="標準 3 6" xfId="176"/>
     <cellStyle name="標準 3 7" xfId="178"/>
+    <cellStyle name="標準 3 8" xfId="375"/>
     <cellStyle name="標準 4" xfId="180"/>
     <cellStyle name="標準 4 2" xfId="181"/>
     <cellStyle name="標準 4 2 2" xfId="144"/>
     <cellStyle name="標準 4 2 2 2" xfId="39"/>
     <cellStyle name="標準 4 2 2 2 2" xfId="182"/>
+    <cellStyle name="標準 4 2 2 2 3" xfId="386"/>
     <cellStyle name="標準 4 2 2 3" xfId="6"/>
+    <cellStyle name="標準 4 2 2 4" xfId="385"/>
     <cellStyle name="標準 4 2 3" xfId="146"/>
     <cellStyle name="標準 4 2 3 2" xfId="183"/>
+    <cellStyle name="標準 4 2 3 3" xfId="387"/>
     <cellStyle name="標準 4 2 4" xfId="148"/>
     <cellStyle name="標準 4 2 5" xfId="165"/>
     <cellStyle name="標準 4 2 6" xfId="167"/>
+    <cellStyle name="標準 4 2 7" xfId="384"/>
     <cellStyle name="標準 4 3" xfId="184"/>
     <cellStyle name="標準 4 3 2" xfId="186"/>
     <cellStyle name="標準 4 3 2 2" xfId="188"/>
     <cellStyle name="標準 4 3 2 3" xfId="190"/>
     <cellStyle name="標準 4 3 2 4" xfId="192"/>
+    <cellStyle name="標準 4 3 2 5" xfId="389"/>
     <cellStyle name="標準 4 3 3" xfId="81"/>
     <cellStyle name="標準 4 3 4" xfId="151"/>
     <cellStyle name="標準 4 3 5" xfId="179"/>
+    <cellStyle name="標準 4 3 6" xfId="388"/>
     <cellStyle name="標準 4 4" xfId="193"/>
     <cellStyle name="標準 4 4 2" xfId="194"/>
+    <cellStyle name="標準 4 4 3" xfId="390"/>
     <cellStyle name="標準 4 5" xfId="195"/>
     <cellStyle name="標準 4 6" xfId="197"/>
     <cellStyle name="標準 4 7" xfId="9"/>
+    <cellStyle name="標準 4 8" xfId="383"/>
     <cellStyle name="標準 5" xfId="198"/>
     <cellStyle name="標準 5 2" xfId="36"/>
     <cellStyle name="標準 5 2 2" xfId="199"/>
     <cellStyle name="標準 5 2 2 2" xfId="201"/>
+    <cellStyle name="標準 5 2 2 3" xfId="393"/>
     <cellStyle name="標準 5 2 3" xfId="202"/>
+    <cellStyle name="標準 5 2 4" xfId="392"/>
     <cellStyle name="標準 5 3" xfId="38"/>
     <cellStyle name="標準 5 3 2" xfId="91"/>
+    <cellStyle name="標準 5 3 3" xfId="394"/>
     <cellStyle name="標準 5 4" xfId="4"/>
     <cellStyle name="標準 5 5" xfId="40"/>
     <cellStyle name="標準 5 6" xfId="33"/>
+    <cellStyle name="標準 5 7" xfId="391"/>
     <cellStyle name="標準_Sheet1" xfId="204"/>
     <cellStyle name="標準_sst107" xfId="175"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -4974,24 +5555,36 @@
     <cellStyle name="常规 10 2" xfId="206"/>
     <cellStyle name="常规 10 2 2" xfId="207"/>
     <cellStyle name="常规 10 2 2 2" xfId="209"/>
+    <cellStyle name="常规 10 2 2 3" xfId="397"/>
     <cellStyle name="常规 10 2 3" xfId="210"/>
+    <cellStyle name="常规 10 2 4" xfId="396"/>
     <cellStyle name="常规 10 3" xfId="211"/>
     <cellStyle name="常规 10 3 2" xfId="213"/>
+    <cellStyle name="常规 10 3 3" xfId="398"/>
     <cellStyle name="常规 10 4" xfId="214"/>
+    <cellStyle name="常规 10 5" xfId="395"/>
     <cellStyle name="常规 11" xfId="215"/>
     <cellStyle name="常规 11 2" xfId="216"/>
     <cellStyle name="常规 11 2 2" xfId="128"/>
+    <cellStyle name="常规 11 2 2 2" xfId="401"/>
     <cellStyle name="常规 11 2 3" xfId="217"/>
+    <cellStyle name="常规 11 2 4" xfId="400"/>
     <cellStyle name="常规 11 3" xfId="218"/>
     <cellStyle name="常规 11 3 2" xfId="125"/>
+    <cellStyle name="常规 11 3 3" xfId="402"/>
     <cellStyle name="常规 11 4" xfId="200"/>
+    <cellStyle name="常规 11 5" xfId="399"/>
     <cellStyle name="常规 12" xfId="219"/>
     <cellStyle name="常规 12 2" xfId="220"/>
+    <cellStyle name="常规 12 2 2" xfId="404"/>
     <cellStyle name="常规 12 3" xfId="221"/>
+    <cellStyle name="常规 12 4" xfId="403"/>
     <cellStyle name="常规 13" xfId="222"/>
     <cellStyle name="常规 13 2" xfId="223"/>
+    <cellStyle name="常规 13 3" xfId="405"/>
     <cellStyle name="常规 14" xfId="224"/>
     <cellStyle name="常规 15" xfId="225"/>
+    <cellStyle name="常规 16" xfId="346"/>
     <cellStyle name="常规 2" xfId="227"/>
     <cellStyle name="常规 2 2" xfId="71"/>
     <cellStyle name="常规 2 3" xfId="73"/>
@@ -4999,70 +5592,95 @@
     <cellStyle name="常规 2 4 2" xfId="228"/>
     <cellStyle name="常规 2 4 2 2" xfId="229"/>
     <cellStyle name="常规 2 4 2 2 2" xfId="230"/>
+    <cellStyle name="常规 2 4 2 2 3" xfId="408"/>
     <cellStyle name="常规 2 4 2 3" xfId="231"/>
+    <cellStyle name="常规 2 4 2 4" xfId="407"/>
     <cellStyle name="常规 2 4 3" xfId="232"/>
     <cellStyle name="常规 2 4 3 2" xfId="233"/>
+    <cellStyle name="常规 2 4 3 3" xfId="409"/>
     <cellStyle name="常规 2 4 4" xfId="234"/>
     <cellStyle name="常规 2 4 5" xfId="236"/>
+    <cellStyle name="常规 2 4 6" xfId="406"/>
     <cellStyle name="常规 3" xfId="238"/>
     <cellStyle name="常规 3 2" xfId="239"/>
     <cellStyle name="常规 3 2 2" xfId="240"/>
     <cellStyle name="常规 3 2 2 2" xfId="241"/>
     <cellStyle name="常规 3 2 2 2 2" xfId="242"/>
+    <cellStyle name="常规 3 2 2 2 3" xfId="413"/>
     <cellStyle name="常规 3 2 2 3" xfId="243"/>
+    <cellStyle name="常规 3 2 2 4" xfId="412"/>
     <cellStyle name="常规 3 2 3" xfId="96"/>
     <cellStyle name="常规 3 2 3 2" xfId="98"/>
+    <cellStyle name="常规 3 2 3 3" xfId="414"/>
     <cellStyle name="常规 3 2 4" xfId="102"/>
     <cellStyle name="常规 3 2 5" xfId="104"/>
     <cellStyle name="常规 3 2 6" xfId="30"/>
+    <cellStyle name="常规 3 2 7" xfId="411"/>
     <cellStyle name="常规 3 3" xfId="244"/>
     <cellStyle name="常规 3 3 2" xfId="245"/>
     <cellStyle name="常规 3 3 2 2" xfId="246"/>
     <cellStyle name="常规 3 3 2 3" xfId="208"/>
     <cellStyle name="常规 3 3 2 4" xfId="12"/>
+    <cellStyle name="常规 3 3 2 5" xfId="416"/>
     <cellStyle name="常规 3 3 3" xfId="107"/>
     <cellStyle name="常规 3 3 4" xfId="226"/>
     <cellStyle name="常规 3 3 5" xfId="237"/>
+    <cellStyle name="常规 3 3 6" xfId="415"/>
     <cellStyle name="常规 3 4" xfId="247"/>
     <cellStyle name="常规 3 4 2" xfId="250"/>
+    <cellStyle name="常规 3 4 3" xfId="417"/>
     <cellStyle name="常规 3 5" xfId="113"/>
     <cellStyle name="常规 3 6" xfId="44"/>
     <cellStyle name="常规 3 7" xfId="212"/>
+    <cellStyle name="常规 3 8" xfId="410"/>
     <cellStyle name="常规 4" xfId="251"/>
     <cellStyle name="常规 5" xfId="252"/>
     <cellStyle name="常规 5 2" xfId="19"/>
     <cellStyle name="常规 5 2 2" xfId="21"/>
     <cellStyle name="常规 5 2 2 2" xfId="253"/>
+    <cellStyle name="常规 5 2 2 3" xfId="420"/>
     <cellStyle name="常规 5 2 3" xfId="24"/>
+    <cellStyle name="常规 5 2 4" xfId="419"/>
     <cellStyle name="常规 5 3" xfId="132"/>
     <cellStyle name="常规 5 3 2" xfId="254"/>
+    <cellStyle name="常规 5 3 3" xfId="421"/>
     <cellStyle name="常规 5 4" xfId="134"/>
     <cellStyle name="常规 5 5" xfId="255"/>
     <cellStyle name="常规 5 6" xfId="256"/>
+    <cellStyle name="常规 5 7" xfId="418"/>
     <cellStyle name="常规 6" xfId="13"/>
     <cellStyle name="常规 6 2" xfId="174"/>
     <cellStyle name="常规 7" xfId="257"/>
     <cellStyle name="常规 7 2" xfId="196"/>
     <cellStyle name="常规 7 2 2" xfId="235"/>
     <cellStyle name="常规 7 2 2 2" xfId="258"/>
+    <cellStyle name="常规 7 2 2 3" xfId="424"/>
     <cellStyle name="常规 7 2 3" xfId="259"/>
+    <cellStyle name="常规 7 2 4" xfId="423"/>
     <cellStyle name="常规 7 3" xfId="8"/>
     <cellStyle name="常规 7 3 2" xfId="262"/>
+    <cellStyle name="常规 7 3 3" xfId="425"/>
     <cellStyle name="常规 7 4" xfId="264"/>
     <cellStyle name="常规 7 5" xfId="266"/>
     <cellStyle name="常规 7 6" xfId="268"/>
+    <cellStyle name="常规 7 7" xfId="422"/>
     <cellStyle name="常规 8" xfId="269"/>
     <cellStyle name="常规 8 2" xfId="32"/>
     <cellStyle name="常规 8 3" xfId="29"/>
     <cellStyle name="常规 8 4" xfId="203"/>
     <cellStyle name="常规 8 5" xfId="270"/>
+    <cellStyle name="常规 8 6" xfId="426"/>
     <cellStyle name="常规 9" xfId="138"/>
     <cellStyle name="常规 9 2" xfId="271"/>
     <cellStyle name="常规 9 2 2" xfId="273"/>
+    <cellStyle name="常规 9 2 2 2" xfId="429"/>
     <cellStyle name="常规 9 2 3" xfId="274"/>
+    <cellStyle name="常规 9 2 4" xfId="428"/>
     <cellStyle name="常规 9 3" xfId="275"/>
     <cellStyle name="常规 9 3 2" xfId="276"/>
+    <cellStyle name="常规 9 3 3" xfId="430"/>
     <cellStyle name="常规 9 4" xfId="277"/>
+    <cellStyle name="常规 9 5" xfId="427"/>
     <cellStyle name="超链接 2" xfId="47"/>
     <cellStyle name="超链接 2 2" xfId="278"/>
     <cellStyle name="超链接 2 2 2" xfId="279"/>
@@ -5070,6 +5688,7 @@
     <cellStyle name="超链接 2 2 3" xfId="282"/>
     <cellStyle name="超链接 2 2 4" xfId="283"/>
     <cellStyle name="超链接 2 2 5" xfId="284"/>
+    <cellStyle name="超链接 2 2 6" xfId="432"/>
     <cellStyle name="超链接 2 3" xfId="286"/>
     <cellStyle name="超链接 2 3 2" xfId="287"/>
     <cellStyle name="超链接 2 3 3" xfId="288"/>
@@ -5077,12 +5696,14 @@
     <cellStyle name="超链接 2 4" xfId="292"/>
     <cellStyle name="超链接 2 5" xfId="65"/>
     <cellStyle name="超链接 2 6" xfId="70"/>
+    <cellStyle name="超链接 2 7" xfId="431"/>
     <cellStyle name="超链接 3" xfId="68"/>
     <cellStyle name="超链接 3 2" xfId="293"/>
     <cellStyle name="超链接 3 2 2" xfId="294"/>
     <cellStyle name="超链接 3 3" xfId="295"/>
     <cellStyle name="超链接 3 4" xfId="296"/>
     <cellStyle name="超链接 3 5" xfId="76"/>
+    <cellStyle name="超链接 3 6" xfId="433"/>
     <cellStyle name="超链接 4" xfId="185"/>
     <cellStyle name="超链接 4 2" xfId="187"/>
     <cellStyle name="超链接 4 2 2" xfId="11"/>
@@ -5090,79 +5711,105 @@
     <cellStyle name="超链接 4 2 3" xfId="50"/>
     <cellStyle name="超链接 4 2 4" xfId="34"/>
     <cellStyle name="超链接 4 2 5" xfId="298"/>
+    <cellStyle name="超链接 4 2 6" xfId="435"/>
     <cellStyle name="超链接 4 3" xfId="189"/>
     <cellStyle name="超链接 4 3 2" xfId="60"/>
     <cellStyle name="超链接 4 4" xfId="191"/>
     <cellStyle name="超链接 4 5" xfId="299"/>
     <cellStyle name="超链接 4 6" xfId="300"/>
+    <cellStyle name="超链接 4 7" xfId="434"/>
     <cellStyle name="桁区切り 2" xfId="301"/>
     <cellStyle name="桁区切り 2 2" xfId="302"/>
     <cellStyle name="桁区切り 2 2 2" xfId="303"/>
     <cellStyle name="桁区切り 2 2 2 2" xfId="140"/>
     <cellStyle name="桁区切り 2 2 2 2 2" xfId="291"/>
+    <cellStyle name="桁区切り 2 2 2 2 3" xfId="439"/>
     <cellStyle name="桁区切り 2 2 2 3" xfId="304"/>
+    <cellStyle name="桁区切り 2 2 2 4" xfId="438"/>
     <cellStyle name="桁区切り 2 2 3" xfId="305"/>
     <cellStyle name="桁区切り 2 2 3 2" xfId="306"/>
+    <cellStyle name="桁区切り 2 2 3 3" xfId="440"/>
     <cellStyle name="桁区切り 2 2 4" xfId="26"/>
     <cellStyle name="桁区切り 2 2 5" xfId="307"/>
     <cellStyle name="桁区切り 2 2 6" xfId="308"/>
+    <cellStyle name="桁区切り 2 2 7" xfId="437"/>
     <cellStyle name="桁区切り 2 3" xfId="309"/>
     <cellStyle name="桁区切り 2 3 2" xfId="310"/>
     <cellStyle name="桁区切り 2 3 2 2" xfId="285"/>
     <cellStyle name="桁区切り 2 3 2 3" xfId="290"/>
     <cellStyle name="桁区切り 2 3 2 4" xfId="64"/>
+    <cellStyle name="桁区切り 2 3 2 5" xfId="442"/>
     <cellStyle name="桁区切り 2 3 3" xfId="311"/>
     <cellStyle name="桁区切り 2 3 4" xfId="312"/>
     <cellStyle name="桁区切り 2 3 5" xfId="313"/>
+    <cellStyle name="桁区切り 2 3 6" xfId="441"/>
     <cellStyle name="桁区切り 2 4" xfId="314"/>
     <cellStyle name="桁区切り 2 4 2" xfId="315"/>
+    <cellStyle name="桁区切り 2 4 3" xfId="443"/>
     <cellStyle name="桁区切り 2 5" xfId="316"/>
     <cellStyle name="桁区切り 2 6" xfId="317"/>
     <cellStyle name="桁区切り 2 7" xfId="318"/>
+    <cellStyle name="桁区切り 2 8" xfId="436"/>
     <cellStyle name="千位分隔 2" xfId="261"/>
     <cellStyle name="千位分隔 2 2" xfId="319"/>
     <cellStyle name="千位分隔 2 2 2" xfId="321"/>
     <cellStyle name="千位分隔 2 2 2 2" xfId="323"/>
+    <cellStyle name="千位分隔 2 2 2 3" xfId="446"/>
     <cellStyle name="千位分隔 2 2 3" xfId="249"/>
+    <cellStyle name="千位分隔 2 2 4" xfId="445"/>
     <cellStyle name="千位分隔 2 3" xfId="324"/>
     <cellStyle name="千位分隔 2 3 2" xfId="326"/>
+    <cellStyle name="千位分隔 2 3 3" xfId="447"/>
     <cellStyle name="千位分隔 2 4" xfId="320"/>
     <cellStyle name="千位分隔 2 5" xfId="248"/>
     <cellStyle name="千位分隔 2 6" xfId="5"/>
+    <cellStyle name="千位分隔 2 7" xfId="444"/>
     <cellStyle name="千位分隔 3" xfId="328"/>
     <cellStyle name="千位分隔 3 2" xfId="329"/>
     <cellStyle name="千位分隔 3 2 2" xfId="177"/>
     <cellStyle name="千位分隔 3 2 2 2" xfId="330"/>
     <cellStyle name="千位分隔 3 2 2 2 2" xfId="25"/>
+    <cellStyle name="千位分隔 3 2 2 2 3" xfId="451"/>
     <cellStyle name="千位分隔 3 2 2 3" xfId="331"/>
+    <cellStyle name="千位分隔 3 2 2 4" xfId="450"/>
     <cellStyle name="千位分隔 3 2 3" xfId="332"/>
     <cellStyle name="千位分隔 3 2 3 2" xfId="333"/>
+    <cellStyle name="千位分隔 3 2 3 3" xfId="452"/>
     <cellStyle name="千位分隔 3 2 4" xfId="18"/>
     <cellStyle name="千位分隔 3 2 5" xfId="334"/>
     <cellStyle name="千位分隔 3 2 6" xfId="272"/>
+    <cellStyle name="千位分隔 3 2 7" xfId="449"/>
     <cellStyle name="千位分隔 3 3" xfId="335"/>
     <cellStyle name="千位分隔 3 3 2" xfId="7"/>
     <cellStyle name="千位分隔 3 3 2 2" xfId="260"/>
     <cellStyle name="千位分隔 3 3 2 3" xfId="327"/>
     <cellStyle name="千位分隔 3 3 2 4" xfId="337"/>
+    <cellStyle name="千位分隔 3 3 2 5" xfId="454"/>
     <cellStyle name="千位分隔 3 3 3" xfId="263"/>
     <cellStyle name="千位分隔 3 3 4" xfId="265"/>
     <cellStyle name="千位分隔 3 3 5" xfId="267"/>
+    <cellStyle name="千位分隔 3 3 6" xfId="453"/>
     <cellStyle name="千位分隔 3 4" xfId="325"/>
     <cellStyle name="千位分隔 3 4 2" xfId="28"/>
+    <cellStyle name="千位分隔 3 4 3" xfId="455"/>
     <cellStyle name="千位分隔 3 5" xfId="115"/>
     <cellStyle name="千位分隔 3 6" xfId="338"/>
     <cellStyle name="千位分隔 3 7" xfId="339"/>
+    <cellStyle name="千位分隔 3 8" xfId="448"/>
     <cellStyle name="千位分隔 4" xfId="336"/>
     <cellStyle name="千位分隔 4 2" xfId="340"/>
     <cellStyle name="千位分隔 4 2 2" xfId="341"/>
     <cellStyle name="千位分隔 4 2 2 2" xfId="342"/>
+    <cellStyle name="千位分隔 4 2 2 3" xfId="458"/>
     <cellStyle name="千位分隔 4 2 3" xfId="343"/>
     <cellStyle name="千位分隔 4 2 4" xfId="344"/>
+    <cellStyle name="千位分隔 4 2 5" xfId="457"/>
     <cellStyle name="千位分隔 4 3" xfId="345"/>
     <cellStyle name="千位分隔 4 3 2" xfId="281"/>
+    <cellStyle name="千位分隔 4 3 3" xfId="459"/>
     <cellStyle name="千位分隔 4 4" xfId="322"/>
     <cellStyle name="千位分隔 4 5" xfId="15"/>
+    <cellStyle name="千位分隔 4 6" xfId="456"/>
   </cellStyles>
   <dxfs count="88">
     <dxf>
@@ -5799,11 +6446,6 @@
       <color rgb="FF3333FF"/>
     </mruColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -5838,8 +6480,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674013"/>
-          <c:y val="3.519067868454432E-2"/>
+          <c:x val="0.38523037913674024"/>
+          <c:y val="3.5190678684544327E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -5908,11 +6550,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="141016064"/>
-        <c:axId val="141021952"/>
+        <c:axId val="139438336"/>
+        <c:axId val="139440128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="141016064"/>
+        <c:axId val="139438336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5946,14 +6588,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141021952"/>
+        <c:crossAx val="139440128"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141021952"/>
+        <c:axId val="139440128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5987,7 +6629,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141016064"/>
+        <c:crossAx val="139438336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6037,7 +6679,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6074,8 +6716,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674013"/>
-          <c:y val="3.0232730603965505E-2"/>
+          <c:x val="0.38523037913674024"/>
+          <c:y val="3.0232730603965512E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -6091,10 +6733,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11177666498383206"/>
+          <c:x val="0.11177666498383208"/>
           <c:y val="0.100000113553908"/>
           <c:w val="0.78044064301210703"/>
-          <c:h val="0.65814028222689147"/>
+          <c:h val="0.6581402822268918"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -6201,11 +6843,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="141074816"/>
-        <c:axId val="141076352"/>
+        <c:axId val="140184960"/>
+        <c:axId val="140215424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="141074816"/>
+        <c:axId val="140184960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6239,14 +6881,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141076352"/>
+        <c:crossAx val="140215424"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141076352"/>
+        <c:axId val="140215424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6280,7 +6922,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141074816"/>
+        <c:crossAx val="140184960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6330,7 +6972,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6367,8 +7009,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.3950625924845832"/>
-          <c:y val="3.1476997578692809E-2"/>
+          <c:x val="0.39506259248458331"/>
+          <c:y val="3.1476997578692816E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -6386,8 +7028,8 @@
           <c:yMode val="edge"/>
           <c:x val="9.2592778647397928E-2"/>
           <c:y val="0.113801452784504"/>
-          <c:w val="0.77572172333487766"/>
-          <c:h val="0.65133171912833321"/>
+          <c:w val="0.77572172333487799"/>
+          <c:h val="0.65133171912833332"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -6689,8 +7331,8 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="141587584"/>
-        <c:axId val="141589120"/>
+        <c:axId val="142170752"/>
+        <c:axId val="142177024"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6789,11 +7431,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="141619584"/>
-        <c:axId val="141621120"/>
+        <c:axId val="142178560"/>
+        <c:axId val="142184448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="141587584"/>
+        <c:axId val="142170752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6827,14 +7469,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141589120"/>
+        <c:crossAx val="142177024"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141589120"/>
+        <c:axId val="142177024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6868,29 +7510,29 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141587584"/>
+        <c:crossAx val="142170752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="141619584"/>
+        <c:axId val="142178560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="141621120"/>
+        <c:crossAx val="142184448"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141621120"/>
+        <c:axId val="142184448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
-          <c:min val="0.75000000000000422"/>
+          <c:min val="0.75000000000000433"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
@@ -6922,7 +7564,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141619584"/>
+        <c:crossAx val="142178560"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.05"/>
@@ -6945,10 +7587,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.22633788060443105"/>
-          <c:y val="0.93462469733656839"/>
-          <c:w val="0.5041163064493478"/>
-          <c:h val="4.8426150121065104E-2"/>
+          <c:x val="0.22633788060443108"/>
+          <c:y val="0.93462469733656861"/>
+          <c:w val="0.50411630644934768"/>
+          <c:h val="4.8426150121065097E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -7014,7 +7656,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7051,8 +7693,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674013"/>
-          <c:y val="3.0232707900360208E-2"/>
+          <c:x val="0.38523037913674024"/>
+          <c:y val="3.0232707900360214E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -7068,10 +7710,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11177666498383206"/>
+          <c:x val="0.11177666498383208"/>
           <c:y val="0.100000113553908"/>
           <c:w val="0.78044064301210703"/>
-          <c:h val="0.65814028222689247"/>
+          <c:h val="0.6581402822268928"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -7133,11 +7775,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="141125504"/>
-        <c:axId val="141127040"/>
+        <c:axId val="142220672"/>
+        <c:axId val="142230656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="141125504"/>
+        <c:axId val="142220672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7171,14 +7813,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141127040"/>
+        <c:crossAx val="142230656"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141127040"/>
+        <c:axId val="142230656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7212,7 +7854,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141125504"/>
+        <c:crossAx val="142220672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7262,7 +7904,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7299,8 +7941,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674013"/>
-          <c:y val="3.519067868454432E-2"/>
+          <c:x val="0.38523037913674024"/>
+          <c:y val="3.5190678684544327E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -7417,11 +8059,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="141147136"/>
-        <c:axId val="142955264"/>
+        <c:axId val="142258560"/>
+        <c:axId val="142260096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="141147136"/>
+        <c:axId val="142258560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7455,14 +8097,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142955264"/>
+        <c:crossAx val="142260096"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142955264"/>
+        <c:axId val="142260096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7496,7 +8138,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141147136"/>
+        <c:crossAx val="142258560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7546,7 +8188,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7583,8 +8225,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674013"/>
-          <c:y val="3.519067868454432E-2"/>
+          <c:x val="0.38523037913674024"/>
+          <c:y val="3.5190678684544327E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -7701,11 +8343,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="142975360"/>
-        <c:axId val="142976896"/>
+        <c:axId val="141055104"/>
+        <c:axId val="141056640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="142975360"/>
+        <c:axId val="141055104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7739,14 +8381,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142976896"/>
+        <c:crossAx val="141056640"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142976896"/>
+        <c:axId val="141056640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7780,7 +8422,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142975360"/>
+        <c:crossAx val="141055104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7830,7 +8472,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7867,8 +8509,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674013"/>
-          <c:y val="3.0232707900360208E-2"/>
+          <c:x val="0.38523037913674024"/>
+          <c:y val="3.0232707900360214E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -7884,10 +8526,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11177666498383206"/>
+          <c:x val="0.11177666498383208"/>
           <c:y val="0.100000113553908"/>
           <c:w val="0.78044064301210703"/>
-          <c:h val="0.65814028222689247"/>
+          <c:h val="0.6581402822268928"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -7949,11 +8591,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="144254464"/>
-        <c:axId val="144256000"/>
+        <c:axId val="141076352"/>
+        <c:axId val="141077888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="144254464"/>
+        <c:axId val="141076352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7987,14 +8629,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="144256000"/>
+        <c:crossAx val="141077888"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144256000"/>
+        <c:axId val="141077888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8028,7 +8670,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="144254464"/>
+        <c:crossAx val="141076352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8078,7 +8720,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8828,10 +9470,10 @@
   <dimension ref="A1:AC111"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="1" topLeftCell="J20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="1" topLeftCell="J32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomRight" activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -10610,18 +11252,32 @@
       <c r="AA34" s="179"/>
       <c r="AB34" s="183"/>
     </row>
-    <row r="35" spans="2:28" ht="14.25" customHeight="1">
-      <c r="B35" s="90"/>
-      <c r="C35" s="105"/>
-      <c r="D35" s="114"/>
+    <row r="35" spans="2:28" ht="57.75" customHeight="1">
+      <c r="B35" s="90">
+        <v>33</v>
+      </c>
+      <c r="C35" s="101" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="114" t="s">
+        <v>27</v>
+      </c>
       <c r="E35" s="113"/>
-      <c r="F35" s="108"/>
+      <c r="F35" s="108" t="s">
+        <v>29</v>
+      </c>
       <c r="G35" s="101"/>
       <c r="H35" s="116"/>
       <c r="I35" s="144"/>
-      <c r="J35" s="129"/>
-      <c r="K35" s="145"/>
-      <c r="L35" s="115"/>
+      <c r="J35" s="129">
+        <v>43279</v>
+      </c>
+      <c r="K35" s="156" t="s">
+        <v>38</v>
+      </c>
+      <c r="L35" s="218" t="s">
+        <v>221</v>
+      </c>
       <c r="M35" s="147"/>
       <c r="N35" s="128"/>
       <c r="O35" s="128"/>
@@ -12486,7 +13142,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F84">
       <formula1>発生段階</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G85">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G85 C35">
       <formula1>"DB,ソース,テストケース,その他"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7">
@@ -12549,30 +13205,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="9" customHeight="1">
-      <c r="E1" s="187"/>
-      <c r="F1" s="187"/>
-      <c r="G1" s="187"/>
-      <c r="H1" s="187"/>
-      <c r="I1" s="187"/>
-      <c r="J1" s="187"/>
+      <c r="E1" s="213"/>
+      <c r="F1" s="213"/>
+      <c r="G1" s="213"/>
+      <c r="H1" s="213"/>
+      <c r="I1" s="213"/>
+      <c r="J1" s="213"/>
     </row>
     <row r="2" spans="2:10" ht="15" customHeight="1">
       <c r="B2" s="26" t="s">
         <v>128</v>
       </c>
       <c r="C2" s="26"/>
-      <c r="E2" s="187"/>
-      <c r="F2" s="187"/>
-      <c r="G2" s="187"/>
-      <c r="H2" s="187"/>
-      <c r="I2" s="187"/>
-      <c r="J2" s="187"/>
+      <c r="E2" s="213"/>
+      <c r="F2" s="213"/>
+      <c r="G2" s="213"/>
+      <c r="H2" s="213"/>
+      <c r="I2" s="213"/>
+      <c r="J2" s="213"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1">
-      <c r="B3" s="216" t="s">
+      <c r="B3" s="185" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="217"/>
+      <c r="C3" s="186"/>
       <c r="D3" s="27" t="s">
         <v>129</v>
       </c>
@@ -12650,30 +13306,30 @@
       </c>
     </row>
     <row r="13" spans="2:10" ht="17.25" customHeight="1">
-      <c r="B13" s="188" t="s">
+      <c r="B13" s="214" t="s">
         <v>134</v>
       </c>
-      <c r="C13" s="188"/>
-      <c r="D13" s="188"/>
-      <c r="E13" s="188"/>
+      <c r="C13" s="214"/>
+      <c r="D13" s="214"/>
+      <c r="E13" s="214"/>
     </row>
     <row r="14" spans="2:10" ht="17.25" customHeight="1">
-      <c r="B14" s="188"/>
-      <c r="C14" s="188"/>
-      <c r="D14" s="188"/>
-      <c r="E14" s="188"/>
+      <c r="B14" s="214"/>
+      <c r="C14" s="214"/>
+      <c r="D14" s="214"/>
+      <c r="E14" s="214"/>
     </row>
     <row r="15" spans="2:10" ht="17.25" customHeight="1">
-      <c r="B15" s="188"/>
-      <c r="C15" s="188"/>
-      <c r="D15" s="188"/>
-      <c r="E15" s="188"/>
+      <c r="B15" s="214"/>
+      <c r="C15" s="214"/>
+      <c r="D15" s="214"/>
+      <c r="E15" s="214"/>
     </row>
     <row r="16" spans="2:10" ht="17.25" customHeight="1">
-      <c r="B16" s="188"/>
-      <c r="C16" s="188"/>
-      <c r="D16" s="188"/>
-      <c r="E16" s="188"/>
+      <c r="B16" s="214"/>
+      <c r="C16" s="214"/>
+      <c r="D16" s="214"/>
+      <c r="E16" s="214"/>
     </row>
     <row r="21" spans="2:5" ht="15" customHeight="1">
       <c r="B21" s="26" t="s">
@@ -12682,10 +13338,10 @@
       <c r="C21" s="26"/>
     </row>
     <row r="22" spans="2:5" ht="15" customHeight="1">
-      <c r="B22" s="216" t="s">
+      <c r="B22" s="185" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="217"/>
+      <c r="C22" s="186"/>
       <c r="D22" s="27" t="s">
         <v>129</v>
       </c>
@@ -12867,30 +13523,30 @@
       </c>
     </row>
     <row r="36" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B36" s="188" t="s">
+      <c r="B36" s="214" t="s">
         <v>134</v>
       </c>
-      <c r="C36" s="188"/>
-      <c r="D36" s="188"/>
-      <c r="E36" s="188"/>
+      <c r="C36" s="214"/>
+      <c r="D36" s="214"/>
+      <c r="E36" s="214"/>
     </row>
     <row r="37" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B37" s="188"/>
-      <c r="C37" s="188"/>
-      <c r="D37" s="188"/>
-      <c r="E37" s="188"/>
+      <c r="B37" s="214"/>
+      <c r="C37" s="214"/>
+      <c r="D37" s="214"/>
+      <c r="E37" s="214"/>
     </row>
     <row r="38" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B38" s="188"/>
-      <c r="C38" s="188"/>
-      <c r="D38" s="188"/>
-      <c r="E38" s="188"/>
+      <c r="B38" s="214"/>
+      <c r="C38" s="214"/>
+      <c r="D38" s="214"/>
+      <c r="E38" s="214"/>
     </row>
     <row r="39" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B39" s="188"/>
-      <c r="C39" s="188"/>
-      <c r="D39" s="188"/>
-      <c r="E39" s="188"/>
+      <c r="B39" s="214"/>
+      <c r="C39" s="214"/>
+      <c r="D39" s="214"/>
+      <c r="E39" s="214"/>
     </row>
     <row r="43" spans="2:5" ht="15" customHeight="1">
       <c r="B43" s="26" t="s">
@@ -12899,10 +13555,10 @@
       <c r="C43" s="26"/>
     </row>
     <row r="44" spans="2:5" ht="15" customHeight="1">
-      <c r="B44" s="216" t="s">
+      <c r="B44" s="185" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="217"/>
+      <c r="C44" s="186"/>
       <c r="D44" s="27" t="s">
         <v>129</v>
       </c>
@@ -13056,30 +13712,30 @@
       </c>
     </row>
     <row r="56" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B56" s="188" t="s">
+      <c r="B56" s="214" t="s">
         <v>134</v>
       </c>
-      <c r="C56" s="188"/>
-      <c r="D56" s="188"/>
-      <c r="E56" s="188"/>
+      <c r="C56" s="214"/>
+      <c r="D56" s="214"/>
+      <c r="E56" s="214"/>
     </row>
     <row r="57" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B57" s="188"/>
-      <c r="C57" s="188"/>
-      <c r="D57" s="188"/>
-      <c r="E57" s="188"/>
+      <c r="B57" s="214"/>
+      <c r="C57" s="214"/>
+      <c r="D57" s="214"/>
+      <c r="E57" s="214"/>
     </row>
     <row r="58" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B58" s="188"/>
-      <c r="C58" s="188"/>
-      <c r="D58" s="188"/>
-      <c r="E58" s="188"/>
+      <c r="B58" s="214"/>
+      <c r="C58" s="214"/>
+      <c r="D58" s="214"/>
+      <c r="E58" s="214"/>
     </row>
     <row r="59" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B59" s="188"/>
-      <c r="C59" s="188"/>
-      <c r="D59" s="188"/>
-      <c r="E59" s="188"/>
+      <c r="B59" s="214"/>
+      <c r="C59" s="214"/>
+      <c r="D59" s="214"/>
+      <c r="E59" s="214"/>
     </row>
     <row r="64" spans="2:5" ht="17.25" customHeight="1">
       <c r="B64" s="26" t="s">
@@ -13088,10 +13744,10 @@
       <c r="C64" s="26"/>
     </row>
     <row r="65" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B65" s="209" t="s">
+      <c r="B65" s="187" t="s">
         <v>17</v>
       </c>
-      <c r="C65" s="210"/>
+      <c r="C65" s="188"/>
       <c r="D65" s="27" t="s">
         <v>129</v>
       </c>
@@ -13271,28 +13927,28 @@
       <c r="E79" s="24"/>
     </row>
     <row r="80" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B80" s="188" t="s">
+      <c r="B80" s="214" t="s">
         <v>173</v>
       </c>
-      <c r="C80" s="188"/>
-      <c r="D80" s="188"/>
-      <c r="E80" s="188"/>
+      <c r="C80" s="214"/>
+      <c r="D80" s="214"/>
+      <c r="E80" s="214"/>
       <c r="F80" s="24"/>
       <c r="G80" s="24"/>
     </row>
     <row r="81" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B81" s="188"/>
-      <c r="C81" s="188"/>
-      <c r="D81" s="188"/>
-      <c r="E81" s="188"/>
+      <c r="B81" s="214"/>
+      <c r="C81" s="214"/>
+      <c r="D81" s="214"/>
+      <c r="E81" s="214"/>
       <c r="F81" s="50"/>
       <c r="G81" s="50"/>
     </row>
     <row r="82" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B82" s="188"/>
-      <c r="C82" s="188"/>
-      <c r="D82" s="188"/>
-      <c r="E82" s="188"/>
+      <c r="B82" s="214"/>
+      <c r="C82" s="214"/>
+      <c r="D82" s="214"/>
+      <c r="E82" s="214"/>
       <c r="F82" s="50"/>
       <c r="G82" s="50"/>
     </row>
@@ -13311,10 +13967,10 @@
       <c r="C84" s="26"/>
     </row>
     <row r="85" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B85" s="209" t="s">
+      <c r="B85" s="187" t="s">
         <v>18</v>
       </c>
-      <c r="C85" s="210"/>
+      <c r="C85" s="188"/>
       <c r="D85" s="27" t="s">
         <v>129</v>
       </c>
@@ -13386,28 +14042,28 @@
       <c r="E90" s="24"/>
     </row>
     <row r="91" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B91" s="188" t="s">
+      <c r="B91" s="214" t="s">
         <v>173</v>
       </c>
-      <c r="C91" s="188"/>
-      <c r="D91" s="188"/>
-      <c r="E91" s="188"/>
+      <c r="C91" s="214"/>
+      <c r="D91" s="214"/>
+      <c r="E91" s="214"/>
       <c r="F91" s="24"/>
       <c r="G91" s="24"/>
     </row>
     <row r="92" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B92" s="188"/>
-      <c r="C92" s="188"/>
-      <c r="D92" s="188"/>
-      <c r="E92" s="188"/>
+      <c r="B92" s="214"/>
+      <c r="C92" s="214"/>
+      <c r="D92" s="214"/>
+      <c r="E92" s="214"/>
       <c r="F92" s="50"/>
       <c r="G92" s="50"/>
     </row>
     <row r="93" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B93" s="188"/>
-      <c r="C93" s="188"/>
-      <c r="D93" s="188"/>
-      <c r="E93" s="188"/>
+      <c r="B93" s="214"/>
+      <c r="C93" s="214"/>
+      <c r="D93" s="214"/>
+      <c r="E93" s="214"/>
       <c r="F93" s="50"/>
       <c r="G93" s="50"/>
     </row>
@@ -13426,10 +14082,10 @@
       <c r="C95" s="26"/>
     </row>
     <row r="96" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B96" s="209" t="s">
+      <c r="B96" s="187" t="s">
         <v>18</v>
       </c>
-      <c r="C96" s="210"/>
+      <c r="C96" s="188"/>
       <c r="D96" s="27" t="s">
         <v>129</v>
       </c>
@@ -13487,28 +14143,28 @@
       <c r="E100" s="24"/>
     </row>
     <row r="101" spans="1:50" ht="23.25" customHeight="1">
-      <c r="B101" s="188" t="s">
+      <c r="B101" s="214" t="s">
         <v>173</v>
       </c>
-      <c r="C101" s="188"/>
-      <c r="D101" s="188"/>
-      <c r="E101" s="188"/>
+      <c r="C101" s="214"/>
+      <c r="D101" s="214"/>
+      <c r="E101" s="214"/>
       <c r="F101" s="24"/>
       <c r="G101" s="24"/>
     </row>
     <row r="102" spans="1:50" ht="23.25" customHeight="1">
-      <c r="B102" s="188"/>
-      <c r="C102" s="188"/>
-      <c r="D102" s="188"/>
-      <c r="E102" s="188"/>
+      <c r="B102" s="214"/>
+      <c r="C102" s="214"/>
+      <c r="D102" s="214"/>
+      <c r="E102" s="214"/>
       <c r="F102" s="50"/>
       <c r="G102" s="50"/>
     </row>
     <row r="103" spans="1:50" ht="23.25" customHeight="1">
-      <c r="B103" s="188"/>
-      <c r="C103" s="188"/>
-      <c r="D103" s="188"/>
-      <c r="E103" s="188"/>
+      <c r="B103" s="214"/>
+      <c r="C103" s="214"/>
+      <c r="D103" s="214"/>
+      <c r="E103" s="214"/>
       <c r="F103" s="50"/>
       <c r="G103" s="50"/>
     </row>
@@ -13550,27 +14206,27 @@
       <c r="C106" s="55" t="s">
         <v>183</v>
       </c>
-      <c r="D106" s="211" t="s">
+      <c r="D106" s="189" t="s">
         <v>184</v>
       </c>
-      <c r="E106" s="212"/>
-      <c r="F106" s="213" t="s">
+      <c r="E106" s="190"/>
+      <c r="F106" s="191" t="s">
         <v>185</v>
       </c>
-      <c r="G106" s="214"/>
-      <c r="H106" s="215"/>
-      <c r="I106" s="213" t="s">
+      <c r="G106" s="192"/>
+      <c r="H106" s="193"/>
+      <c r="I106" s="191" t="s">
         <v>186</v>
       </c>
-      <c r="J106" s="214"/>
-      <c r="K106" s="214"/>
-      <c r="L106" s="215"/>
-      <c r="M106" s="213" t="s">
+      <c r="J106" s="192"/>
+      <c r="K106" s="192"/>
+      <c r="L106" s="193"/>
+      <c r="M106" s="191" t="s">
         <v>187</v>
       </c>
-      <c r="N106" s="214"/>
-      <c r="O106" s="214"/>
-      <c r="P106" s="215"/>
+      <c r="N106" s="192"/>
+      <c r="O106" s="192"/>
+      <c r="P106" s="193"/>
       <c r="Q106" s="63" t="s">
         <v>188</v>
       </c>
@@ -13591,27 +14247,27 @@
       <c r="C107" s="57" t="s">
         <v>191</v>
       </c>
-      <c r="D107" s="203" t="s">
+      <c r="D107" s="194" t="s">
         <v>192</v>
       </c>
-      <c r="E107" s="204"/>
-      <c r="F107" s="205" t="s">
+      <c r="E107" s="195"/>
+      <c r="F107" s="196" t="s">
         <v>193</v>
       </c>
-      <c r="G107" s="206"/>
-      <c r="H107" s="207"/>
-      <c r="I107" s="205" t="s">
+      <c r="G107" s="197"/>
+      <c r="H107" s="198"/>
+      <c r="I107" s="196" t="s">
         <v>194</v>
       </c>
-      <c r="J107" s="206"/>
-      <c r="K107" s="206"/>
-      <c r="L107" s="207"/>
-      <c r="M107" s="208" t="s">
+      <c r="J107" s="197"/>
+      <c r="K107" s="197"/>
+      <c r="L107" s="198"/>
+      <c r="M107" s="199" t="s">
         <v>195</v>
       </c>
-      <c r="N107" s="208"/>
-      <c r="O107" s="208"/>
-      <c r="P107" s="208"/>
+      <c r="N107" s="199"/>
+      <c r="O107" s="199"/>
+      <c r="P107" s="199"/>
       <c r="Q107" s="71" t="s">
         <v>196</v>
       </c>
@@ -13628,19 +14284,19 @@
     <row r="108" spans="1:50" s="23" customFormat="1" ht="11.25">
       <c r="B108" s="58"/>
       <c r="C108" s="59"/>
-      <c r="D108" s="197"/>
-      <c r="E108" s="198"/>
-      <c r="F108" s="199"/>
-      <c r="G108" s="200"/>
-      <c r="H108" s="201"/>
-      <c r="I108" s="199"/>
-      <c r="J108" s="200"/>
-      <c r="K108" s="200"/>
-      <c r="L108" s="201"/>
-      <c r="M108" s="202"/>
-      <c r="N108" s="202"/>
-      <c r="O108" s="202"/>
-      <c r="P108" s="202"/>
+      <c r="D108" s="200"/>
+      <c r="E108" s="201"/>
+      <c r="F108" s="202"/>
+      <c r="G108" s="203"/>
+      <c r="H108" s="204"/>
+      <c r="I108" s="202"/>
+      <c r="J108" s="203"/>
+      <c r="K108" s="203"/>
+      <c r="L108" s="204"/>
+      <c r="M108" s="205"/>
+      <c r="N108" s="205"/>
+      <c r="O108" s="205"/>
+      <c r="P108" s="205"/>
       <c r="Q108" s="73"/>
       <c r="R108" s="74"/>
       <c r="U108" s="70"/>
@@ -13653,19 +14309,19 @@
     <row r="109" spans="1:50" s="23" customFormat="1" ht="11.25">
       <c r="B109" s="58"/>
       <c r="C109" s="59"/>
-      <c r="D109" s="197"/>
-      <c r="E109" s="198"/>
-      <c r="F109" s="199"/>
-      <c r="G109" s="200"/>
-      <c r="H109" s="201"/>
-      <c r="I109" s="199"/>
-      <c r="J109" s="200"/>
-      <c r="K109" s="200"/>
-      <c r="L109" s="201"/>
-      <c r="M109" s="202"/>
-      <c r="N109" s="202"/>
-      <c r="O109" s="202"/>
-      <c r="P109" s="202"/>
+      <c r="D109" s="200"/>
+      <c r="E109" s="201"/>
+      <c r="F109" s="202"/>
+      <c r="G109" s="203"/>
+      <c r="H109" s="204"/>
+      <c r="I109" s="202"/>
+      <c r="J109" s="203"/>
+      <c r="K109" s="203"/>
+      <c r="L109" s="204"/>
+      <c r="M109" s="205"/>
+      <c r="N109" s="205"/>
+      <c r="O109" s="205"/>
+      <c r="P109" s="205"/>
       <c r="Q109" s="73"/>
       <c r="R109" s="74"/>
       <c r="U109" s="70"/>
@@ -13678,19 +14334,19 @@
     <row r="110" spans="1:50" s="23" customFormat="1" ht="11.25">
       <c r="B110" s="58"/>
       <c r="C110" s="59"/>
-      <c r="D110" s="197"/>
-      <c r="E110" s="198"/>
-      <c r="F110" s="199"/>
-      <c r="G110" s="200"/>
-      <c r="H110" s="201"/>
-      <c r="I110" s="199"/>
-      <c r="J110" s="200"/>
-      <c r="K110" s="200"/>
-      <c r="L110" s="201"/>
-      <c r="M110" s="202"/>
-      <c r="N110" s="202"/>
-      <c r="O110" s="202"/>
-      <c r="P110" s="202"/>
+      <c r="D110" s="200"/>
+      <c r="E110" s="201"/>
+      <c r="F110" s="202"/>
+      <c r="G110" s="203"/>
+      <c r="H110" s="204"/>
+      <c r="I110" s="202"/>
+      <c r="J110" s="203"/>
+      <c r="K110" s="203"/>
+      <c r="L110" s="204"/>
+      <c r="M110" s="205"/>
+      <c r="N110" s="205"/>
+      <c r="O110" s="205"/>
+      <c r="P110" s="205"/>
       <c r="Q110" s="73"/>
       <c r="R110" s="74"/>
       <c r="U110" s="70"/>
@@ -13703,19 +14359,19 @@
     <row r="111" spans="1:50" s="23" customFormat="1" ht="11.25">
       <c r="B111" s="58"/>
       <c r="C111" s="59"/>
-      <c r="D111" s="197"/>
-      <c r="E111" s="198"/>
-      <c r="F111" s="199"/>
-      <c r="G111" s="200"/>
-      <c r="H111" s="201"/>
-      <c r="I111" s="199"/>
-      <c r="J111" s="200"/>
-      <c r="K111" s="200"/>
-      <c r="L111" s="201"/>
-      <c r="M111" s="202"/>
-      <c r="N111" s="202"/>
-      <c r="O111" s="202"/>
-      <c r="P111" s="202"/>
+      <c r="D111" s="200"/>
+      <c r="E111" s="201"/>
+      <c r="F111" s="202"/>
+      <c r="G111" s="203"/>
+      <c r="H111" s="204"/>
+      <c r="I111" s="202"/>
+      <c r="J111" s="203"/>
+      <c r="K111" s="203"/>
+      <c r="L111" s="204"/>
+      <c r="M111" s="205"/>
+      <c r="N111" s="205"/>
+      <c r="O111" s="205"/>
+      <c r="P111" s="205"/>
       <c r="Q111" s="73"/>
       <c r="R111" s="74"/>
       <c r="U111" s="70"/>
@@ -13728,19 +14384,19 @@
     <row r="112" spans="1:50" s="23" customFormat="1" ht="11.25">
       <c r="B112" s="58"/>
       <c r="C112" s="59"/>
-      <c r="D112" s="197"/>
-      <c r="E112" s="198"/>
-      <c r="F112" s="199"/>
-      <c r="G112" s="200"/>
-      <c r="H112" s="201"/>
-      <c r="I112" s="199"/>
-      <c r="J112" s="200"/>
-      <c r="K112" s="200"/>
-      <c r="L112" s="201"/>
-      <c r="M112" s="202"/>
-      <c r="N112" s="202"/>
-      <c r="O112" s="202"/>
-      <c r="P112" s="202"/>
+      <c r="D112" s="200"/>
+      <c r="E112" s="201"/>
+      <c r="F112" s="202"/>
+      <c r="G112" s="203"/>
+      <c r="H112" s="204"/>
+      <c r="I112" s="202"/>
+      <c r="J112" s="203"/>
+      <c r="K112" s="203"/>
+      <c r="L112" s="204"/>
+      <c r="M112" s="205"/>
+      <c r="N112" s="205"/>
+      <c r="O112" s="205"/>
+      <c r="P112" s="205"/>
       <c r="Q112" s="73"/>
       <c r="R112" s="74"/>
       <c r="U112" s="70"/>
@@ -13753,19 +14409,19 @@
     <row r="113" spans="2:26" s="23" customFormat="1" ht="11.25">
       <c r="B113" s="58"/>
       <c r="C113" s="59"/>
-      <c r="D113" s="197"/>
-      <c r="E113" s="198"/>
-      <c r="F113" s="199"/>
-      <c r="G113" s="200"/>
-      <c r="H113" s="201"/>
-      <c r="I113" s="199"/>
-      <c r="J113" s="200"/>
-      <c r="K113" s="200"/>
-      <c r="L113" s="201"/>
-      <c r="M113" s="202"/>
-      <c r="N113" s="202"/>
-      <c r="O113" s="202"/>
-      <c r="P113" s="202"/>
+      <c r="D113" s="200"/>
+      <c r="E113" s="201"/>
+      <c r="F113" s="202"/>
+      <c r="G113" s="203"/>
+      <c r="H113" s="204"/>
+      <c r="I113" s="202"/>
+      <c r="J113" s="203"/>
+      <c r="K113" s="203"/>
+      <c r="L113" s="204"/>
+      <c r="M113" s="205"/>
+      <c r="N113" s="205"/>
+      <c r="O113" s="205"/>
+      <c r="P113" s="205"/>
       <c r="Q113" s="73"/>
       <c r="R113" s="74"/>
       <c r="U113" s="70"/>
@@ -13778,19 +14434,19 @@
     <row r="114" spans="2:26" s="23" customFormat="1" ht="11.25">
       <c r="B114" s="58"/>
       <c r="C114" s="59"/>
-      <c r="D114" s="197"/>
-      <c r="E114" s="198"/>
-      <c r="F114" s="199"/>
-      <c r="G114" s="200"/>
-      <c r="H114" s="201"/>
-      <c r="I114" s="199"/>
-      <c r="J114" s="200"/>
-      <c r="K114" s="200"/>
-      <c r="L114" s="201"/>
-      <c r="M114" s="202"/>
-      <c r="N114" s="202"/>
-      <c r="O114" s="202"/>
-      <c r="P114" s="202"/>
+      <c r="D114" s="200"/>
+      <c r="E114" s="201"/>
+      <c r="F114" s="202"/>
+      <c r="G114" s="203"/>
+      <c r="H114" s="204"/>
+      <c r="I114" s="202"/>
+      <c r="J114" s="203"/>
+      <c r="K114" s="203"/>
+      <c r="L114" s="204"/>
+      <c r="M114" s="205"/>
+      <c r="N114" s="205"/>
+      <c r="O114" s="205"/>
+      <c r="P114" s="205"/>
       <c r="Q114" s="73"/>
       <c r="R114" s="74"/>
       <c r="U114" s="70"/>
@@ -13803,19 +14459,19 @@
     <row r="115" spans="2:26" s="23" customFormat="1" ht="11.25">
       <c r="B115" s="58"/>
       <c r="C115" s="59"/>
-      <c r="D115" s="197"/>
-      <c r="E115" s="198"/>
-      <c r="F115" s="199"/>
-      <c r="G115" s="200"/>
-      <c r="H115" s="201"/>
-      <c r="I115" s="199"/>
-      <c r="J115" s="200"/>
-      <c r="K115" s="200"/>
-      <c r="L115" s="201"/>
-      <c r="M115" s="202"/>
-      <c r="N115" s="202"/>
-      <c r="O115" s="202"/>
-      <c r="P115" s="202"/>
+      <c r="D115" s="200"/>
+      <c r="E115" s="201"/>
+      <c r="F115" s="202"/>
+      <c r="G115" s="203"/>
+      <c r="H115" s="204"/>
+      <c r="I115" s="202"/>
+      <c r="J115" s="203"/>
+      <c r="K115" s="203"/>
+      <c r="L115" s="204"/>
+      <c r="M115" s="205"/>
+      <c r="N115" s="205"/>
+      <c r="O115" s="205"/>
+      <c r="P115" s="205"/>
       <c r="Q115" s="73"/>
       <c r="R115" s="74"/>
       <c r="U115" s="70"/>
@@ -13828,19 +14484,19 @@
     <row r="116" spans="2:26" s="23" customFormat="1" ht="11.25">
       <c r="B116" s="58"/>
       <c r="C116" s="59"/>
-      <c r="D116" s="197"/>
-      <c r="E116" s="198"/>
-      <c r="F116" s="199"/>
-      <c r="G116" s="200"/>
-      <c r="H116" s="201"/>
-      <c r="I116" s="199"/>
-      <c r="J116" s="200"/>
-      <c r="K116" s="200"/>
-      <c r="L116" s="201"/>
-      <c r="M116" s="202"/>
-      <c r="N116" s="202"/>
-      <c r="O116" s="202"/>
-      <c r="P116" s="202"/>
+      <c r="D116" s="200"/>
+      <c r="E116" s="201"/>
+      <c r="F116" s="202"/>
+      <c r="G116" s="203"/>
+      <c r="H116" s="204"/>
+      <c r="I116" s="202"/>
+      <c r="J116" s="203"/>
+      <c r="K116" s="203"/>
+      <c r="L116" s="204"/>
+      <c r="M116" s="205"/>
+      <c r="N116" s="205"/>
+      <c r="O116" s="205"/>
+      <c r="P116" s="205"/>
       <c r="Q116" s="73"/>
       <c r="R116" s="74"/>
       <c r="U116" s="70"/>
@@ -13867,32 +14523,32 @@
       <c r="G118" s="50"/>
     </row>
     <row r="119" spans="2:26" ht="17.25" customHeight="1">
-      <c r="B119" s="189" t="s">
+      <c r="B119" s="215" t="s">
         <v>183</v>
       </c>
-      <c r="C119" s="189" t="s">
+      <c r="C119" s="215" t="s">
         <v>198</v>
       </c>
-      <c r="D119" s="189" t="s">
+      <c r="D119" s="215" t="s">
         <v>199</v>
       </c>
-      <c r="E119" s="189" t="s">
+      <c r="E119" s="215" t="s">
         <v>200</v>
       </c>
-      <c r="F119" s="191" t="s">
+      <c r="F119" s="217" t="s">
         <v>201</v>
       </c>
-      <c r="G119" s="185" t="s">
+      <c r="G119" s="211" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="120" spans="2:26" ht="17.25" customHeight="1">
-      <c r="B120" s="190"/>
-      <c r="C120" s="190"/>
-      <c r="D120" s="190"/>
-      <c r="E120" s="190"/>
-      <c r="F120" s="191"/>
-      <c r="G120" s="186"/>
+      <c r="B120" s="216"/>
+      <c r="C120" s="216"/>
+      <c r="D120" s="216"/>
+      <c r="E120" s="216"/>
+      <c r="F120" s="217"/>
+      <c r="G120" s="212"/>
     </row>
     <row r="121" spans="2:26" ht="17.25" customHeight="1">
       <c r="B121" s="64">
@@ -14308,19 +14964,19 @@
       <c r="L137" s="88"/>
     </row>
     <row r="138" spans="2:13" s="24" customFormat="1" ht="59.25" customHeight="1">
-      <c r="B138" s="194" t="s">
+      <c r="B138" s="206" t="s">
         <v>203</v>
       </c>
-      <c r="C138" s="194"/>
-      <c r="D138" s="194"/>
-      <c r="E138" s="194"/>
-      <c r="F138" s="194"/>
-      <c r="G138" s="194"/>
-      <c r="H138" s="194"/>
-      <c r="I138" s="194"/>
-      <c r="J138" s="194"/>
-      <c r="K138" s="194"/>
-      <c r="L138" s="194"/>
+      <c r="C138" s="206"/>
+      <c r="D138" s="206"/>
+      <c r="E138" s="206"/>
+      <c r="F138" s="206"/>
+      <c r="G138" s="206"/>
+      <c r="H138" s="206"/>
+      <c r="I138" s="206"/>
+      <c r="J138" s="206"/>
+      <c r="K138" s="206"/>
+      <c r="L138" s="206"/>
     </row>
     <row r="139" spans="2:13" s="24" customFormat="1" ht="12" customHeight="1">
       <c r="B139" s="82"/>
@@ -14357,20 +15013,20 @@
       <c r="C141" s="84" t="s">
         <v>205</v>
       </c>
-      <c r="D141" s="195" t="s">
+      <c r="D141" s="207" t="s">
         <v>206</v>
       </c>
-      <c r="E141" s="195"/>
-      <c r="F141" s="195"/>
-      <c r="G141" s="195"/>
-      <c r="H141" s="196" t="s">
+      <c r="E141" s="207"/>
+      <c r="F141" s="207"/>
+      <c r="G141" s="207"/>
+      <c r="H141" s="208" t="s">
         <v>11</v>
       </c>
-      <c r="I141" s="196"/>
-      <c r="J141" s="196"/>
-      <c r="K141" s="196"/>
-      <c r="L141" s="196"/>
-      <c r="M141" s="196"/>
+      <c r="I141" s="208"/>
+      <c r="J141" s="208"/>
+      <c r="K141" s="208"/>
+      <c r="L141" s="208"/>
+      <c r="M141" s="208"/>
     </row>
     <row r="142" spans="2:13" s="24" customFormat="1" ht="14.25" customHeight="1">
       <c r="B142" s="85">
@@ -14379,119 +15035,61 @@
       <c r="C142" s="86" t="s">
         <v>207</v>
       </c>
-      <c r="D142" s="192"/>
-      <c r="E142" s="192"/>
-      <c r="F142" s="192"/>
-      <c r="G142" s="192"/>
-      <c r="H142" s="193"/>
-      <c r="I142" s="193"/>
-      <c r="J142" s="193"/>
-      <c r="K142" s="193"/>
-      <c r="L142" s="193"/>
-      <c r="M142" s="193"/>
+      <c r="D142" s="209"/>
+      <c r="E142" s="209"/>
+      <c r="F142" s="209"/>
+      <c r="G142" s="209"/>
+      <c r="H142" s="210"/>
+      <c r="I142" s="210"/>
+      <c r="J142" s="210"/>
+      <c r="K142" s="210"/>
+      <c r="L142" s="210"/>
+      <c r="M142" s="210"/>
     </row>
     <row r="143" spans="2:13" s="24" customFormat="1" ht="14.25" customHeight="1">
       <c r="B143" s="85"/>
       <c r="C143" s="86"/>
-      <c r="D143" s="192"/>
-      <c r="E143" s="192"/>
-      <c r="F143" s="192"/>
-      <c r="G143" s="192"/>
-      <c r="H143" s="193"/>
-      <c r="I143" s="193"/>
-      <c r="J143" s="193"/>
-      <c r="K143" s="193"/>
-      <c r="L143" s="193"/>
-      <c r="M143" s="193"/>
+      <c r="D143" s="209"/>
+      <c r="E143" s="209"/>
+      <c r="F143" s="209"/>
+      <c r="G143" s="209"/>
+      <c r="H143" s="210"/>
+      <c r="I143" s="210"/>
+      <c r="J143" s="210"/>
+      <c r="K143" s="210"/>
+      <c r="L143" s="210"/>
+      <c r="M143" s="210"/>
     </row>
     <row r="144" spans="2:13" s="24" customFormat="1" ht="14.25" customHeight="1">
       <c r="B144" s="85"/>
       <c r="C144" s="86"/>
-      <c r="D144" s="192"/>
-      <c r="E144" s="192"/>
-      <c r="F144" s="192"/>
-      <c r="G144" s="192"/>
-      <c r="H144" s="193"/>
-      <c r="I144" s="193"/>
-      <c r="J144" s="193"/>
-      <c r="K144" s="193"/>
-      <c r="L144" s="193"/>
-      <c r="M144" s="193"/>
+      <c r="D144" s="209"/>
+      <c r="E144" s="209"/>
+      <c r="F144" s="209"/>
+      <c r="G144" s="209"/>
+      <c r="H144" s="210"/>
+      <c r="I144" s="210"/>
+      <c r="J144" s="210"/>
+      <c r="K144" s="210"/>
+      <c r="L144" s="210"/>
+      <c r="M144" s="210"/>
     </row>
     <row r="145" spans="2:13" s="24" customFormat="1" ht="14.25" customHeight="1">
       <c r="B145" s="85"/>
       <c r="C145" s="86"/>
-      <c r="D145" s="192"/>
-      <c r="E145" s="192"/>
-      <c r="F145" s="192"/>
-      <c r="G145" s="192"/>
-      <c r="H145" s="193"/>
-      <c r="I145" s="193"/>
-      <c r="J145" s="193"/>
-      <c r="K145" s="193"/>
-      <c r="L145" s="193"/>
-      <c r="M145" s="193"/>
+      <c r="D145" s="209"/>
+      <c r="E145" s="209"/>
+      <c r="F145" s="209"/>
+      <c r="G145" s="209"/>
+      <c r="H145" s="210"/>
+      <c r="I145" s="210"/>
+      <c r="J145" s="210"/>
+      <c r="K145" s="210"/>
+      <c r="L145" s="210"/>
+      <c r="M145" s="210"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="F106:H106"/>
-    <mergeCell ref="I106:L106"/>
-    <mergeCell ref="M106:P106"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="F107:H107"/>
-    <mergeCell ref="I107:L107"/>
-    <mergeCell ref="M107:P107"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="F108:H108"/>
-    <mergeCell ref="I108:L108"/>
-    <mergeCell ref="M108:P108"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="I109:L109"/>
-    <mergeCell ref="M109:P109"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="F110:H110"/>
-    <mergeCell ref="I110:L110"/>
-    <mergeCell ref="M110:P110"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="F111:H111"/>
-    <mergeCell ref="I111:L111"/>
-    <mergeCell ref="M111:P111"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="F112:H112"/>
-    <mergeCell ref="I112:L112"/>
-    <mergeCell ref="M112:P112"/>
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="F113:H113"/>
-    <mergeCell ref="I113:L113"/>
-    <mergeCell ref="M113:P113"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="F114:H114"/>
-    <mergeCell ref="I114:L114"/>
-    <mergeCell ref="M114:P114"/>
-    <mergeCell ref="M115:P115"/>
-    <mergeCell ref="D116:E116"/>
-    <mergeCell ref="F116:H116"/>
-    <mergeCell ref="I116:L116"/>
-    <mergeCell ref="M116:P116"/>
-    <mergeCell ref="B138:L138"/>
-    <mergeCell ref="D141:G141"/>
-    <mergeCell ref="H141:M141"/>
-    <mergeCell ref="D142:G142"/>
-    <mergeCell ref="H142:M142"/>
-    <mergeCell ref="D143:G143"/>
-    <mergeCell ref="H143:M143"/>
-    <mergeCell ref="D144:G144"/>
-    <mergeCell ref="H144:M144"/>
-    <mergeCell ref="D145:G145"/>
-    <mergeCell ref="H145:M145"/>
     <mergeCell ref="G119:G120"/>
     <mergeCell ref="E1:J2"/>
     <mergeCell ref="B80:E82"/>
@@ -14508,6 +15106,64 @@
     <mergeCell ref="D115:E115"/>
     <mergeCell ref="F115:H115"/>
     <mergeCell ref="I115:L115"/>
+    <mergeCell ref="D143:G143"/>
+    <mergeCell ref="H143:M143"/>
+    <mergeCell ref="D144:G144"/>
+    <mergeCell ref="H144:M144"/>
+    <mergeCell ref="D145:G145"/>
+    <mergeCell ref="H145:M145"/>
+    <mergeCell ref="B138:L138"/>
+    <mergeCell ref="D141:G141"/>
+    <mergeCell ref="H141:M141"/>
+    <mergeCell ref="D142:G142"/>
+    <mergeCell ref="H142:M142"/>
+    <mergeCell ref="M115:P115"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="F116:H116"/>
+    <mergeCell ref="I116:L116"/>
+    <mergeCell ref="M116:P116"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="F113:H113"/>
+    <mergeCell ref="I113:L113"/>
+    <mergeCell ref="M113:P113"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="F114:H114"/>
+    <mergeCell ref="I114:L114"/>
+    <mergeCell ref="M114:P114"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="F111:H111"/>
+    <mergeCell ref="I111:L111"/>
+    <mergeCell ref="M111:P111"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="F112:H112"/>
+    <mergeCell ref="I112:L112"/>
+    <mergeCell ref="M112:P112"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="F109:H109"/>
+    <mergeCell ref="I109:L109"/>
+    <mergeCell ref="M109:P109"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="F110:H110"/>
+    <mergeCell ref="I110:L110"/>
+    <mergeCell ref="M110:P110"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="F107:H107"/>
+    <mergeCell ref="I107:L107"/>
+    <mergeCell ref="M107:P107"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="I108:L108"/>
+    <mergeCell ref="M108:P108"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="F106:H106"/>
+    <mergeCell ref="I106:L106"/>
+    <mergeCell ref="M106:P106"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B85:C85"/>
   </mergeCells>
   <phoneticPr fontId="52" type="noConversion"/>
   <pageMargins left="0.78680555555555598" right="0.78680555555555598" top="0.98263888888888895" bottom="0.98263888888888895" header="0.51180555555555596" footer="0.51180555555555596"/>

</xml_diff>

<commit_message>
修改数据库 Signed-off-by: LiuYiyang <lyy@shequchina.cn>
</commit_message>
<xml_diff>
--- a/document/AP_障害管理票_QDYL.xlsx
+++ b/document/AP_障害管理票_QDYL.xlsx
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="224">
   <si>
     <t>通番</t>
   </si>
@@ -3141,6 +3141,102 @@
         <charset val="134"/>
       </rPr>
       <t>工作，IN_DB中表ap_waiting_contact未作修改。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>更新代</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>码后未执行</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t>DDL文件</t>
+    </r>
+    <phoneticPr fontId="52" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>表ap_subscription必</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>须</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t>有数据，否</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>则</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t>主</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>页</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t>不能正常</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>显</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t>示。</t>
     </r>
   </si>
 </sst>
@@ -3160,7 +3256,7 @@
     <numFmt numFmtId="182" formatCode="0.0_ "/>
     <numFmt numFmtId="183" formatCode="0_ "/>
   </numFmts>
-  <fonts count="65">
+  <fonts count="64">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -3511,12 +3607,6 @@
       <color indexed="8"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="ＭＳ ゴシック"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -4501,20 +4591,20 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
@@ -4534,17 +4624,17 @@
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4561,30 +4651,30 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
@@ -4596,43 +4686,43 @@
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0"/>
     <xf numFmtId="38" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -4649,36 +4739,36 @@
     <xf numFmtId="38" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="64" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="58" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="64" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="64" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="64" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="64" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="64" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="64" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="64" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="63" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="63" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="63" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="63" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="63" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="63" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="63" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="63" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -5246,107 +5336,107 @@
     <xf numFmtId="180" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="180" fontId="15" fillId="0" borderId="25" xfId="346" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="181" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="181" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="10" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="15" fillId="0" borderId="25" xfId="346" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="460">
@@ -6480,8 +6570,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674024"/>
-          <c:y val="3.5190678684544327E-2"/>
+          <c:x val="0.38523037913674035"/>
+          <c:y val="3.5190678684544341E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -6550,11 +6640,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="139438336"/>
-        <c:axId val="139440128"/>
+        <c:axId val="97052928"/>
+        <c:axId val="97054720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="139438336"/>
+        <c:axId val="97052928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6588,14 +6678,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="139440128"/>
+        <c:crossAx val="97054720"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="139440128"/>
+        <c:axId val="97054720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6629,7 +6719,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="139438336"/>
+        <c:crossAx val="97052928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6679,7 +6769,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6716,8 +6806,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674024"/>
-          <c:y val="3.0232730603965512E-2"/>
+          <c:x val="0.38523037913674035"/>
+          <c:y val="3.0232730603965516E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -6733,10 +6823,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11177666498383208"/>
+          <c:x val="0.11177666498383211"/>
           <c:y val="0.100000113553908"/>
           <c:w val="0.78044064301210703"/>
-          <c:h val="0.6581402822268918"/>
+          <c:h val="0.65814028222689203"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -6843,11 +6933,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="140184960"/>
-        <c:axId val="140215424"/>
+        <c:axId val="132521344"/>
+        <c:axId val="132547712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="140184960"/>
+        <c:axId val="132521344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6881,14 +6971,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140215424"/>
+        <c:crossAx val="132547712"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140215424"/>
+        <c:axId val="132547712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6922,7 +7012,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140184960"/>
+        <c:crossAx val="132521344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6972,7 +7062,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7009,8 +7099,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.39506259248458331"/>
-          <c:y val="3.1476997578692816E-2"/>
+          <c:x val="0.39506259248458336"/>
+          <c:y val="3.1476997578692822E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -7028,8 +7118,8 @@
           <c:yMode val="edge"/>
           <c:x val="9.2592778647397928E-2"/>
           <c:y val="0.113801452784504"/>
-          <c:w val="0.77572172333487799"/>
-          <c:h val="0.65133171912833332"/>
+          <c:w val="0.77572172333487832"/>
+          <c:h val="0.65133171912833343"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -7331,8 +7421,8 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="142170752"/>
-        <c:axId val="142177024"/>
+        <c:axId val="134048384"/>
+        <c:axId val="134062848"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -7431,11 +7521,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="142178560"/>
-        <c:axId val="142184448"/>
+        <c:axId val="134064384"/>
+        <c:axId val="134078464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="142170752"/>
+        <c:axId val="134048384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7469,14 +7559,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142177024"/>
+        <c:crossAx val="134062848"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142177024"/>
+        <c:axId val="134062848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7510,29 +7600,29 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142170752"/>
+        <c:crossAx val="134048384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="142178560"/>
+        <c:axId val="134064384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="142184448"/>
+        <c:crossAx val="134078464"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142184448"/>
+        <c:axId val="134078464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
-          <c:min val="0.75000000000000433"/>
+          <c:min val="0.75000000000000444"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
@@ -7564,7 +7654,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142178560"/>
+        <c:crossAx val="134064384"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.05"/>
@@ -7587,9 +7677,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.22633788060443108"/>
-          <c:y val="0.93462469733656861"/>
-          <c:w val="0.50411630644934768"/>
+          <c:x val="0.22633788060443111"/>
+          <c:y val="0.93462469733656872"/>
+          <c:w val="0.50411630644934757"/>
           <c:h val="4.8426150121065097E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -7656,7 +7746,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7693,8 +7783,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674024"/>
-          <c:y val="3.0232707900360214E-2"/>
+          <c:x val="0.38523037913674035"/>
+          <c:y val="3.0232707900360218E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -7710,10 +7800,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11177666498383208"/>
+          <c:x val="0.11177666498383211"/>
           <c:y val="0.100000113553908"/>
           <c:w val="0.78044064301210703"/>
-          <c:h val="0.6581402822268928"/>
+          <c:h val="0.65814028222689303"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -7775,11 +7865,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="142220672"/>
-        <c:axId val="142230656"/>
+        <c:axId val="133578112"/>
+        <c:axId val="133588096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="142220672"/>
+        <c:axId val="133578112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7813,14 +7903,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142230656"/>
+        <c:crossAx val="133588096"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142230656"/>
+        <c:axId val="133588096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7854,7 +7944,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142220672"/>
+        <c:crossAx val="133578112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7904,7 +7994,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7941,8 +8031,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674024"/>
-          <c:y val="3.5190678684544327E-2"/>
+          <c:x val="0.38523037913674035"/>
+          <c:y val="3.5190678684544341E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -8059,11 +8149,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="142258560"/>
-        <c:axId val="142260096"/>
+        <c:axId val="133607808"/>
+        <c:axId val="133609344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="142258560"/>
+        <c:axId val="133607808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8097,14 +8187,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142260096"/>
+        <c:crossAx val="133609344"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142260096"/>
+        <c:axId val="133609344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8138,7 +8228,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142258560"/>
+        <c:crossAx val="133607808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8188,7 +8278,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8225,8 +8315,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674024"/>
-          <c:y val="3.5190678684544327E-2"/>
+          <c:x val="0.38523037913674035"/>
+          <c:y val="3.5190678684544341E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -8343,11 +8433,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="141055104"/>
-        <c:axId val="141056640"/>
+        <c:axId val="134501504"/>
+        <c:axId val="134503040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="141055104"/>
+        <c:axId val="134501504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8381,14 +8471,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141056640"/>
+        <c:crossAx val="134503040"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141056640"/>
+        <c:axId val="134503040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8422,7 +8512,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141055104"/>
+        <c:crossAx val="134501504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8472,7 +8562,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8509,8 +8599,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674024"/>
-          <c:y val="3.0232707900360214E-2"/>
+          <c:x val="0.38523037913674035"/>
+          <c:y val="3.0232707900360218E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -8526,10 +8616,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11177666498383208"/>
+          <c:x val="0.11177666498383211"/>
           <c:y val="0.100000113553908"/>
           <c:w val="0.78044064301210703"/>
-          <c:h val="0.6581402822268928"/>
+          <c:h val="0.65814028222689303"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -8591,11 +8681,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="141076352"/>
-        <c:axId val="141077888"/>
+        <c:axId val="134526848"/>
+        <c:axId val="134528384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="141076352"/>
+        <c:axId val="134526848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8629,14 +8719,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141077888"/>
+        <c:crossAx val="134528384"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141077888"/>
+        <c:axId val="134528384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8670,7 +8760,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141076352"/>
+        <c:crossAx val="134526848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8720,7 +8810,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9473,7 +9563,7 @@
       <pane xSplit="9" ySplit="1" topLeftCell="J32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I40" sqref="I40"/>
+      <selection pane="bottomRight" activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -11260,7 +11350,7 @@
         <v>41</v>
       </c>
       <c r="D35" s="114" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="E35" s="113"/>
       <c r="F35" s="108" t="s">
@@ -11275,10 +11365,12 @@
       <c r="K35" s="156" t="s">
         <v>38</v>
       </c>
-      <c r="L35" s="218" t="s">
+      <c r="L35" s="185" t="s">
         <v>221</v>
       </c>
-      <c r="M35" s="147"/>
+      <c r="M35" s="147" t="s">
+        <v>222</v>
+      </c>
       <c r="N35" s="128"/>
       <c r="O35" s="128"/>
       <c r="P35" s="148"/>
@@ -11296,17 +11388,31 @@
       <c r="AB35" s="183"/>
     </row>
     <row r="36" spans="2:28" ht="14.25" customHeight="1">
-      <c r="B36" s="90"/>
-      <c r="C36" s="105"/>
-      <c r="D36" s="114"/>
+      <c r="B36" s="90">
+        <v>34</v>
+      </c>
+      <c r="C36" s="101" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" s="114" t="s">
+        <v>27</v>
+      </c>
       <c r="E36" s="113"/>
-      <c r="F36" s="108"/>
+      <c r="F36" s="108" t="s">
+        <v>29</v>
+      </c>
       <c r="G36" s="101"/>
       <c r="H36" s="116"/>
       <c r="I36" s="144"/>
-      <c r="J36" s="129"/>
-      <c r="K36" s="145"/>
-      <c r="L36" s="115"/>
+      <c r="J36" s="129">
+        <v>43280</v>
+      </c>
+      <c r="K36" s="156" t="s">
+        <v>38</v>
+      </c>
+      <c r="L36" s="115" t="s">
+        <v>223</v>
+      </c>
       <c r="M36" s="147"/>
       <c r="N36" s="128"/>
       <c r="O36" s="128"/>
@@ -13142,7 +13248,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F84">
       <formula1>発生段階</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G85 C35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G85 C35:C36">
       <formula1>"DB,ソース,テストケース,その他"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7">
@@ -13205,30 +13311,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="9" customHeight="1">
-      <c r="E1" s="213"/>
-      <c r="F1" s="213"/>
-      <c r="G1" s="213"/>
-      <c r="H1" s="213"/>
-      <c r="I1" s="213"/>
-      <c r="J1" s="213"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="188"/>
+      <c r="G1" s="188"/>
+      <c r="H1" s="188"/>
+      <c r="I1" s="188"/>
+      <c r="J1" s="188"/>
     </row>
     <row r="2" spans="2:10" ht="15" customHeight="1">
       <c r="B2" s="26" t="s">
         <v>128</v>
       </c>
       <c r="C2" s="26"/>
-      <c r="E2" s="213"/>
-      <c r="F2" s="213"/>
-      <c r="G2" s="213"/>
-      <c r="H2" s="213"/>
-      <c r="I2" s="213"/>
-      <c r="J2" s="213"/>
+      <c r="E2" s="188"/>
+      <c r="F2" s="188"/>
+      <c r="G2" s="188"/>
+      <c r="H2" s="188"/>
+      <c r="I2" s="188"/>
+      <c r="J2" s="188"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1">
-      <c r="B3" s="185" t="s">
+      <c r="B3" s="217" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="186"/>
+      <c r="C3" s="218"/>
       <c r="D3" s="27" t="s">
         <v>129</v>
       </c>
@@ -13306,30 +13412,30 @@
       </c>
     </row>
     <row r="13" spans="2:10" ht="17.25" customHeight="1">
-      <c r="B13" s="214" t="s">
+      <c r="B13" s="189" t="s">
         <v>134</v>
       </c>
-      <c r="C13" s="214"/>
-      <c r="D13" s="214"/>
-      <c r="E13" s="214"/>
+      <c r="C13" s="189"/>
+      <c r="D13" s="189"/>
+      <c r="E13" s="189"/>
     </row>
     <row r="14" spans="2:10" ht="17.25" customHeight="1">
-      <c r="B14" s="214"/>
-      <c r="C14" s="214"/>
-      <c r="D14" s="214"/>
-      <c r="E14" s="214"/>
+      <c r="B14" s="189"/>
+      <c r="C14" s="189"/>
+      <c r="D14" s="189"/>
+      <c r="E14" s="189"/>
     </row>
     <row r="15" spans="2:10" ht="17.25" customHeight="1">
-      <c r="B15" s="214"/>
-      <c r="C15" s="214"/>
-      <c r="D15" s="214"/>
-      <c r="E15" s="214"/>
+      <c r="B15" s="189"/>
+      <c r="C15" s="189"/>
+      <c r="D15" s="189"/>
+      <c r="E15" s="189"/>
     </row>
     <row r="16" spans="2:10" ht="17.25" customHeight="1">
-      <c r="B16" s="214"/>
-      <c r="C16" s="214"/>
-      <c r="D16" s="214"/>
-      <c r="E16" s="214"/>
+      <c r="B16" s="189"/>
+      <c r="C16" s="189"/>
+      <c r="D16" s="189"/>
+      <c r="E16" s="189"/>
     </row>
     <row r="21" spans="2:5" ht="15" customHeight="1">
       <c r="B21" s="26" t="s">
@@ -13338,10 +13444,10 @@
       <c r="C21" s="26"/>
     </row>
     <row r="22" spans="2:5" ht="15" customHeight="1">
-      <c r="B22" s="185" t="s">
+      <c r="B22" s="217" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="186"/>
+      <c r="C22" s="218"/>
       <c r="D22" s="27" t="s">
         <v>129</v>
       </c>
@@ -13523,30 +13629,30 @@
       </c>
     </row>
     <row r="36" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B36" s="214" t="s">
+      <c r="B36" s="189" t="s">
         <v>134</v>
       </c>
-      <c r="C36" s="214"/>
-      <c r="D36" s="214"/>
-      <c r="E36" s="214"/>
+      <c r="C36" s="189"/>
+      <c r="D36" s="189"/>
+      <c r="E36" s="189"/>
     </row>
     <row r="37" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B37" s="214"/>
-      <c r="C37" s="214"/>
-      <c r="D37" s="214"/>
-      <c r="E37" s="214"/>
+      <c r="B37" s="189"/>
+      <c r="C37" s="189"/>
+      <c r="D37" s="189"/>
+      <c r="E37" s="189"/>
     </row>
     <row r="38" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B38" s="214"/>
-      <c r="C38" s="214"/>
-      <c r="D38" s="214"/>
-      <c r="E38" s="214"/>
+      <c r="B38" s="189"/>
+      <c r="C38" s="189"/>
+      <c r="D38" s="189"/>
+      <c r="E38" s="189"/>
     </row>
     <row r="39" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B39" s="214"/>
-      <c r="C39" s="214"/>
-      <c r="D39" s="214"/>
-      <c r="E39" s="214"/>
+      <c r="B39" s="189"/>
+      <c r="C39" s="189"/>
+      <c r="D39" s="189"/>
+      <c r="E39" s="189"/>
     </row>
     <row r="43" spans="2:5" ht="15" customHeight="1">
       <c r="B43" s="26" t="s">
@@ -13555,10 +13661,10 @@
       <c r="C43" s="26"/>
     </row>
     <row r="44" spans="2:5" ht="15" customHeight="1">
-      <c r="B44" s="185" t="s">
+      <c r="B44" s="217" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="186"/>
+      <c r="C44" s="218"/>
       <c r="D44" s="27" t="s">
         <v>129</v>
       </c>
@@ -13712,30 +13818,30 @@
       </c>
     </row>
     <row r="56" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B56" s="214" t="s">
+      <c r="B56" s="189" t="s">
         <v>134</v>
       </c>
-      <c r="C56" s="214"/>
-      <c r="D56" s="214"/>
-      <c r="E56" s="214"/>
+      <c r="C56" s="189"/>
+      <c r="D56" s="189"/>
+      <c r="E56" s="189"/>
     </row>
     <row r="57" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B57" s="214"/>
-      <c r="C57" s="214"/>
-      <c r="D57" s="214"/>
-      <c r="E57" s="214"/>
+      <c r="B57" s="189"/>
+      <c r="C57" s="189"/>
+      <c r="D57" s="189"/>
+      <c r="E57" s="189"/>
     </row>
     <row r="58" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B58" s="214"/>
-      <c r="C58" s="214"/>
-      <c r="D58" s="214"/>
-      <c r="E58" s="214"/>
+      <c r="B58" s="189"/>
+      <c r="C58" s="189"/>
+      <c r="D58" s="189"/>
+      <c r="E58" s="189"/>
     </row>
     <row r="59" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B59" s="214"/>
-      <c r="C59" s="214"/>
-      <c r="D59" s="214"/>
-      <c r="E59" s="214"/>
+      <c r="B59" s="189"/>
+      <c r="C59" s="189"/>
+      <c r="D59" s="189"/>
+      <c r="E59" s="189"/>
     </row>
     <row r="64" spans="2:5" ht="17.25" customHeight="1">
       <c r="B64" s="26" t="s">
@@ -13744,10 +13850,10 @@
       <c r="C64" s="26"/>
     </row>
     <row r="65" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B65" s="187" t="s">
+      <c r="B65" s="210" t="s">
         <v>17</v>
       </c>
-      <c r="C65" s="188"/>
+      <c r="C65" s="211"/>
       <c r="D65" s="27" t="s">
         <v>129</v>
       </c>
@@ -13927,28 +14033,28 @@
       <c r="E79" s="24"/>
     </row>
     <row r="80" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B80" s="214" t="s">
+      <c r="B80" s="189" t="s">
         <v>173</v>
       </c>
-      <c r="C80" s="214"/>
-      <c r="D80" s="214"/>
-      <c r="E80" s="214"/>
+      <c r="C80" s="189"/>
+      <c r="D80" s="189"/>
+      <c r="E80" s="189"/>
       <c r="F80" s="24"/>
       <c r="G80" s="24"/>
     </row>
     <row r="81" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B81" s="214"/>
-      <c r="C81" s="214"/>
-      <c r="D81" s="214"/>
-      <c r="E81" s="214"/>
+      <c r="B81" s="189"/>
+      <c r="C81" s="189"/>
+      <c r="D81" s="189"/>
+      <c r="E81" s="189"/>
       <c r="F81" s="50"/>
       <c r="G81" s="50"/>
     </row>
     <row r="82" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B82" s="214"/>
-      <c r="C82" s="214"/>
-      <c r="D82" s="214"/>
-      <c r="E82" s="214"/>
+      <c r="B82" s="189"/>
+      <c r="C82" s="189"/>
+      <c r="D82" s="189"/>
+      <c r="E82" s="189"/>
       <c r="F82" s="50"/>
       <c r="G82" s="50"/>
     </row>
@@ -13967,10 +14073,10 @@
       <c r="C84" s="26"/>
     </row>
     <row r="85" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B85" s="187" t="s">
+      <c r="B85" s="210" t="s">
         <v>18</v>
       </c>
-      <c r="C85" s="188"/>
+      <c r="C85" s="211"/>
       <c r="D85" s="27" t="s">
         <v>129</v>
       </c>
@@ -14042,28 +14148,28 @@
       <c r="E90" s="24"/>
     </row>
     <row r="91" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B91" s="214" t="s">
+      <c r="B91" s="189" t="s">
         <v>173</v>
       </c>
-      <c r="C91" s="214"/>
-      <c r="D91" s="214"/>
-      <c r="E91" s="214"/>
+      <c r="C91" s="189"/>
+      <c r="D91" s="189"/>
+      <c r="E91" s="189"/>
       <c r="F91" s="24"/>
       <c r="G91" s="24"/>
     </row>
     <row r="92" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B92" s="214"/>
-      <c r="C92" s="214"/>
-      <c r="D92" s="214"/>
-      <c r="E92" s="214"/>
+      <c r="B92" s="189"/>
+      <c r="C92" s="189"/>
+      <c r="D92" s="189"/>
+      <c r="E92" s="189"/>
       <c r="F92" s="50"/>
       <c r="G92" s="50"/>
     </row>
     <row r="93" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B93" s="214"/>
-      <c r="C93" s="214"/>
-      <c r="D93" s="214"/>
-      <c r="E93" s="214"/>
+      <c r="B93" s="189"/>
+      <c r="C93" s="189"/>
+      <c r="D93" s="189"/>
+      <c r="E93" s="189"/>
       <c r="F93" s="50"/>
       <c r="G93" s="50"/>
     </row>
@@ -14082,10 +14188,10 @@
       <c r="C95" s="26"/>
     </row>
     <row r="96" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B96" s="187" t="s">
+      <c r="B96" s="210" t="s">
         <v>18</v>
       </c>
-      <c r="C96" s="188"/>
+      <c r="C96" s="211"/>
       <c r="D96" s="27" t="s">
         <v>129</v>
       </c>
@@ -14143,28 +14249,28 @@
       <c r="E100" s="24"/>
     </row>
     <row r="101" spans="1:50" ht="23.25" customHeight="1">
-      <c r="B101" s="214" t="s">
+      <c r="B101" s="189" t="s">
         <v>173</v>
       </c>
-      <c r="C101" s="214"/>
-      <c r="D101" s="214"/>
-      <c r="E101" s="214"/>
+      <c r="C101" s="189"/>
+      <c r="D101" s="189"/>
+      <c r="E101" s="189"/>
       <c r="F101" s="24"/>
       <c r="G101" s="24"/>
     </row>
     <row r="102" spans="1:50" ht="23.25" customHeight="1">
-      <c r="B102" s="214"/>
-      <c r="C102" s="214"/>
-      <c r="D102" s="214"/>
-      <c r="E102" s="214"/>
+      <c r="B102" s="189"/>
+      <c r="C102" s="189"/>
+      <c r="D102" s="189"/>
+      <c r="E102" s="189"/>
       <c r="F102" s="50"/>
       <c r="G102" s="50"/>
     </row>
     <row r="103" spans="1:50" ht="23.25" customHeight="1">
-      <c r="B103" s="214"/>
-      <c r="C103" s="214"/>
-      <c r="D103" s="214"/>
-      <c r="E103" s="214"/>
+      <c r="B103" s="189"/>
+      <c r="C103" s="189"/>
+      <c r="D103" s="189"/>
+      <c r="E103" s="189"/>
       <c r="F103" s="50"/>
       <c r="G103" s="50"/>
     </row>
@@ -14206,27 +14312,27 @@
       <c r="C106" s="55" t="s">
         <v>183</v>
       </c>
-      <c r="D106" s="189" t="s">
+      <c r="D106" s="212" t="s">
         <v>184</v>
       </c>
-      <c r="E106" s="190"/>
-      <c r="F106" s="191" t="s">
+      <c r="E106" s="213"/>
+      <c r="F106" s="214" t="s">
         <v>185</v>
       </c>
-      <c r="G106" s="192"/>
-      <c r="H106" s="193"/>
-      <c r="I106" s="191" t="s">
+      <c r="G106" s="215"/>
+      <c r="H106" s="216"/>
+      <c r="I106" s="214" t="s">
         <v>186</v>
       </c>
-      <c r="J106" s="192"/>
-      <c r="K106" s="192"/>
-      <c r="L106" s="193"/>
-      <c r="M106" s="191" t="s">
+      <c r="J106" s="215"/>
+      <c r="K106" s="215"/>
+      <c r="L106" s="216"/>
+      <c r="M106" s="214" t="s">
         <v>187</v>
       </c>
-      <c r="N106" s="192"/>
-      <c r="O106" s="192"/>
-      <c r="P106" s="193"/>
+      <c r="N106" s="215"/>
+      <c r="O106" s="215"/>
+      <c r="P106" s="216"/>
       <c r="Q106" s="63" t="s">
         <v>188</v>
       </c>
@@ -14247,27 +14353,27 @@
       <c r="C107" s="57" t="s">
         <v>191</v>
       </c>
-      <c r="D107" s="194" t="s">
+      <c r="D107" s="204" t="s">
         <v>192</v>
       </c>
-      <c r="E107" s="195"/>
-      <c r="F107" s="196" t="s">
+      <c r="E107" s="205"/>
+      <c r="F107" s="206" t="s">
         <v>193</v>
       </c>
-      <c r="G107" s="197"/>
-      <c r="H107" s="198"/>
-      <c r="I107" s="196" t="s">
+      <c r="G107" s="207"/>
+      <c r="H107" s="208"/>
+      <c r="I107" s="206" t="s">
         <v>194</v>
       </c>
-      <c r="J107" s="197"/>
-      <c r="K107" s="197"/>
-      <c r="L107" s="198"/>
-      <c r="M107" s="199" t="s">
+      <c r="J107" s="207"/>
+      <c r="K107" s="207"/>
+      <c r="L107" s="208"/>
+      <c r="M107" s="209" t="s">
         <v>195</v>
       </c>
-      <c r="N107" s="199"/>
-      <c r="O107" s="199"/>
-      <c r="P107" s="199"/>
+      <c r="N107" s="209"/>
+      <c r="O107" s="209"/>
+      <c r="P107" s="209"/>
       <c r="Q107" s="71" t="s">
         <v>196</v>
       </c>
@@ -14284,19 +14390,19 @@
     <row r="108" spans="1:50" s="23" customFormat="1" ht="11.25">
       <c r="B108" s="58"/>
       <c r="C108" s="59"/>
-      <c r="D108" s="200"/>
-      <c r="E108" s="201"/>
-      <c r="F108" s="202"/>
-      <c r="G108" s="203"/>
-      <c r="H108" s="204"/>
-      <c r="I108" s="202"/>
-      <c r="J108" s="203"/>
-      <c r="K108" s="203"/>
-      <c r="L108" s="204"/>
-      <c r="M108" s="205"/>
-      <c r="N108" s="205"/>
-      <c r="O108" s="205"/>
-      <c r="P108" s="205"/>
+      <c r="D108" s="193"/>
+      <c r="E108" s="194"/>
+      <c r="F108" s="195"/>
+      <c r="G108" s="196"/>
+      <c r="H108" s="197"/>
+      <c r="I108" s="195"/>
+      <c r="J108" s="196"/>
+      <c r="K108" s="196"/>
+      <c r="L108" s="197"/>
+      <c r="M108" s="203"/>
+      <c r="N108" s="203"/>
+      <c r="O108" s="203"/>
+      <c r="P108" s="203"/>
       <c r="Q108" s="73"/>
       <c r="R108" s="74"/>
       <c r="U108" s="70"/>
@@ -14309,19 +14415,19 @@
     <row r="109" spans="1:50" s="23" customFormat="1" ht="11.25">
       <c r="B109" s="58"/>
       <c r="C109" s="59"/>
-      <c r="D109" s="200"/>
-      <c r="E109" s="201"/>
-      <c r="F109" s="202"/>
-      <c r="G109" s="203"/>
-      <c r="H109" s="204"/>
-      <c r="I109" s="202"/>
-      <c r="J109" s="203"/>
-      <c r="K109" s="203"/>
-      <c r="L109" s="204"/>
-      <c r="M109" s="205"/>
-      <c r="N109" s="205"/>
-      <c r="O109" s="205"/>
-      <c r="P109" s="205"/>
+      <c r="D109" s="193"/>
+      <c r="E109" s="194"/>
+      <c r="F109" s="195"/>
+      <c r="G109" s="196"/>
+      <c r="H109" s="197"/>
+      <c r="I109" s="195"/>
+      <c r="J109" s="196"/>
+      <c r="K109" s="196"/>
+      <c r="L109" s="197"/>
+      <c r="M109" s="203"/>
+      <c r="N109" s="203"/>
+      <c r="O109" s="203"/>
+      <c r="P109" s="203"/>
       <c r="Q109" s="73"/>
       <c r="R109" s="74"/>
       <c r="U109" s="70"/>
@@ -14334,19 +14440,19 @@
     <row r="110" spans="1:50" s="23" customFormat="1" ht="11.25">
       <c r="B110" s="58"/>
       <c r="C110" s="59"/>
-      <c r="D110" s="200"/>
-      <c r="E110" s="201"/>
-      <c r="F110" s="202"/>
-      <c r="G110" s="203"/>
-      <c r="H110" s="204"/>
-      <c r="I110" s="202"/>
-      <c r="J110" s="203"/>
-      <c r="K110" s="203"/>
-      <c r="L110" s="204"/>
-      <c r="M110" s="205"/>
-      <c r="N110" s="205"/>
-      <c r="O110" s="205"/>
-      <c r="P110" s="205"/>
+      <c r="D110" s="193"/>
+      <c r="E110" s="194"/>
+      <c r="F110" s="195"/>
+      <c r="G110" s="196"/>
+      <c r="H110" s="197"/>
+      <c r="I110" s="195"/>
+      <c r="J110" s="196"/>
+      <c r="K110" s="196"/>
+      <c r="L110" s="197"/>
+      <c r="M110" s="203"/>
+      <c r="N110" s="203"/>
+      <c r="O110" s="203"/>
+      <c r="P110" s="203"/>
       <c r="Q110" s="73"/>
       <c r="R110" s="74"/>
       <c r="U110" s="70"/>
@@ -14359,19 +14465,19 @@
     <row r="111" spans="1:50" s="23" customFormat="1" ht="11.25">
       <c r="B111" s="58"/>
       <c r="C111" s="59"/>
-      <c r="D111" s="200"/>
-      <c r="E111" s="201"/>
-      <c r="F111" s="202"/>
-      <c r="G111" s="203"/>
-      <c r="H111" s="204"/>
-      <c r="I111" s="202"/>
-      <c r="J111" s="203"/>
-      <c r="K111" s="203"/>
-      <c r="L111" s="204"/>
-      <c r="M111" s="205"/>
-      <c r="N111" s="205"/>
-      <c r="O111" s="205"/>
-      <c r="P111" s="205"/>
+      <c r="D111" s="193"/>
+      <c r="E111" s="194"/>
+      <c r="F111" s="195"/>
+      <c r="G111" s="196"/>
+      <c r="H111" s="197"/>
+      <c r="I111" s="195"/>
+      <c r="J111" s="196"/>
+      <c r="K111" s="196"/>
+      <c r="L111" s="197"/>
+      <c r="M111" s="203"/>
+      <c r="N111" s="203"/>
+      <c r="O111" s="203"/>
+      <c r="P111" s="203"/>
       <c r="Q111" s="73"/>
       <c r="R111" s="74"/>
       <c r="U111" s="70"/>
@@ -14384,19 +14490,19 @@
     <row r="112" spans="1:50" s="23" customFormat="1" ht="11.25">
       <c r="B112" s="58"/>
       <c r="C112" s="59"/>
-      <c r="D112" s="200"/>
-      <c r="E112" s="201"/>
-      <c r="F112" s="202"/>
-      <c r="G112" s="203"/>
-      <c r="H112" s="204"/>
-      <c r="I112" s="202"/>
-      <c r="J112" s="203"/>
-      <c r="K112" s="203"/>
-      <c r="L112" s="204"/>
-      <c r="M112" s="205"/>
-      <c r="N112" s="205"/>
-      <c r="O112" s="205"/>
-      <c r="P112" s="205"/>
+      <c r="D112" s="193"/>
+      <c r="E112" s="194"/>
+      <c r="F112" s="195"/>
+      <c r="G112" s="196"/>
+      <c r="H112" s="197"/>
+      <c r="I112" s="195"/>
+      <c r="J112" s="196"/>
+      <c r="K112" s="196"/>
+      <c r="L112" s="197"/>
+      <c r="M112" s="203"/>
+      <c r="N112" s="203"/>
+      <c r="O112" s="203"/>
+      <c r="P112" s="203"/>
       <c r="Q112" s="73"/>
       <c r="R112" s="74"/>
       <c r="U112" s="70"/>
@@ -14409,19 +14515,19 @@
     <row r="113" spans="2:26" s="23" customFormat="1" ht="11.25">
       <c r="B113" s="58"/>
       <c r="C113" s="59"/>
-      <c r="D113" s="200"/>
-      <c r="E113" s="201"/>
-      <c r="F113" s="202"/>
-      <c r="G113" s="203"/>
-      <c r="H113" s="204"/>
-      <c r="I113" s="202"/>
-      <c r="J113" s="203"/>
-      <c r="K113" s="203"/>
-      <c r="L113" s="204"/>
-      <c r="M113" s="205"/>
-      <c r="N113" s="205"/>
-      <c r="O113" s="205"/>
-      <c r="P113" s="205"/>
+      <c r="D113" s="193"/>
+      <c r="E113" s="194"/>
+      <c r="F113" s="195"/>
+      <c r="G113" s="196"/>
+      <c r="H113" s="197"/>
+      <c r="I113" s="195"/>
+      <c r="J113" s="196"/>
+      <c r="K113" s="196"/>
+      <c r="L113" s="197"/>
+      <c r="M113" s="203"/>
+      <c r="N113" s="203"/>
+      <c r="O113" s="203"/>
+      <c r="P113" s="203"/>
       <c r="Q113" s="73"/>
       <c r="R113" s="74"/>
       <c r="U113" s="70"/>
@@ -14434,19 +14540,19 @@
     <row r="114" spans="2:26" s="23" customFormat="1" ht="11.25">
       <c r="B114" s="58"/>
       <c r="C114" s="59"/>
-      <c r="D114" s="200"/>
-      <c r="E114" s="201"/>
-      <c r="F114" s="202"/>
-      <c r="G114" s="203"/>
-      <c r="H114" s="204"/>
-      <c r="I114" s="202"/>
-      <c r="J114" s="203"/>
-      <c r="K114" s="203"/>
-      <c r="L114" s="204"/>
-      <c r="M114" s="205"/>
-      <c r="N114" s="205"/>
-      <c r="O114" s="205"/>
-      <c r="P114" s="205"/>
+      <c r="D114" s="193"/>
+      <c r="E114" s="194"/>
+      <c r="F114" s="195"/>
+      <c r="G114" s="196"/>
+      <c r="H114" s="197"/>
+      <c r="I114" s="195"/>
+      <c r="J114" s="196"/>
+      <c r="K114" s="196"/>
+      <c r="L114" s="197"/>
+      <c r="M114" s="203"/>
+      <c r="N114" s="203"/>
+      <c r="O114" s="203"/>
+      <c r="P114" s="203"/>
       <c r="Q114" s="73"/>
       <c r="R114" s="74"/>
       <c r="U114" s="70"/>
@@ -14459,19 +14565,19 @@
     <row r="115" spans="2:26" s="23" customFormat="1" ht="11.25">
       <c r="B115" s="58"/>
       <c r="C115" s="59"/>
-      <c r="D115" s="200"/>
-      <c r="E115" s="201"/>
-      <c r="F115" s="202"/>
-      <c r="G115" s="203"/>
-      <c r="H115" s="204"/>
-      <c r="I115" s="202"/>
-      <c r="J115" s="203"/>
-      <c r="K115" s="203"/>
-      <c r="L115" s="204"/>
-      <c r="M115" s="205"/>
-      <c r="N115" s="205"/>
-      <c r="O115" s="205"/>
-      <c r="P115" s="205"/>
+      <c r="D115" s="193"/>
+      <c r="E115" s="194"/>
+      <c r="F115" s="195"/>
+      <c r="G115" s="196"/>
+      <c r="H115" s="197"/>
+      <c r="I115" s="195"/>
+      <c r="J115" s="196"/>
+      <c r="K115" s="196"/>
+      <c r="L115" s="197"/>
+      <c r="M115" s="203"/>
+      <c r="N115" s="203"/>
+      <c r="O115" s="203"/>
+      <c r="P115" s="203"/>
       <c r="Q115" s="73"/>
       <c r="R115" s="74"/>
       <c r="U115" s="70"/>
@@ -14484,19 +14590,19 @@
     <row r="116" spans="2:26" s="23" customFormat="1" ht="11.25">
       <c r="B116" s="58"/>
       <c r="C116" s="59"/>
-      <c r="D116" s="200"/>
-      <c r="E116" s="201"/>
-      <c r="F116" s="202"/>
-      <c r="G116" s="203"/>
-      <c r="H116" s="204"/>
-      <c r="I116" s="202"/>
-      <c r="J116" s="203"/>
-      <c r="K116" s="203"/>
-      <c r="L116" s="204"/>
-      <c r="M116" s="205"/>
-      <c r="N116" s="205"/>
-      <c r="O116" s="205"/>
-      <c r="P116" s="205"/>
+      <c r="D116" s="193"/>
+      <c r="E116" s="194"/>
+      <c r="F116" s="195"/>
+      <c r="G116" s="196"/>
+      <c r="H116" s="197"/>
+      <c r="I116" s="195"/>
+      <c r="J116" s="196"/>
+      <c r="K116" s="196"/>
+      <c r="L116" s="197"/>
+      <c r="M116" s="203"/>
+      <c r="N116" s="203"/>
+      <c r="O116" s="203"/>
+      <c r="P116" s="203"/>
       <c r="Q116" s="73"/>
       <c r="R116" s="74"/>
       <c r="U116" s="70"/>
@@ -14523,32 +14629,32 @@
       <c r="G118" s="50"/>
     </row>
     <row r="119" spans="2:26" ht="17.25" customHeight="1">
-      <c r="B119" s="215" t="s">
+      <c r="B119" s="190" t="s">
         <v>183</v>
       </c>
-      <c r="C119" s="215" t="s">
+      <c r="C119" s="190" t="s">
         <v>198</v>
       </c>
-      <c r="D119" s="215" t="s">
+      <c r="D119" s="190" t="s">
         <v>199</v>
       </c>
-      <c r="E119" s="215" t="s">
+      <c r="E119" s="190" t="s">
         <v>200</v>
       </c>
-      <c r="F119" s="217" t="s">
+      <c r="F119" s="192" t="s">
         <v>201</v>
       </c>
-      <c r="G119" s="211" t="s">
+      <c r="G119" s="186" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="120" spans="2:26" ht="17.25" customHeight="1">
-      <c r="B120" s="216"/>
-      <c r="C120" s="216"/>
-      <c r="D120" s="216"/>
-      <c r="E120" s="216"/>
-      <c r="F120" s="217"/>
-      <c r="G120" s="212"/>
+      <c r="B120" s="191"/>
+      <c r="C120" s="191"/>
+      <c r="D120" s="191"/>
+      <c r="E120" s="191"/>
+      <c r="F120" s="192"/>
+      <c r="G120" s="187"/>
     </row>
     <row r="121" spans="2:26" ht="17.25" customHeight="1">
       <c r="B121" s="64">
@@ -14964,19 +15070,19 @@
       <c r="L137" s="88"/>
     </row>
     <row r="138" spans="2:13" s="24" customFormat="1" ht="59.25" customHeight="1">
-      <c r="B138" s="206" t="s">
+      <c r="B138" s="200" t="s">
         <v>203</v>
       </c>
-      <c r="C138" s="206"/>
-      <c r="D138" s="206"/>
-      <c r="E138" s="206"/>
-      <c r="F138" s="206"/>
-      <c r="G138" s="206"/>
-      <c r="H138" s="206"/>
-      <c r="I138" s="206"/>
-      <c r="J138" s="206"/>
-      <c r="K138" s="206"/>
-      <c r="L138" s="206"/>
+      <c r="C138" s="200"/>
+      <c r="D138" s="200"/>
+      <c r="E138" s="200"/>
+      <c r="F138" s="200"/>
+      <c r="G138" s="200"/>
+      <c r="H138" s="200"/>
+      <c r="I138" s="200"/>
+      <c r="J138" s="200"/>
+      <c r="K138" s="200"/>
+      <c r="L138" s="200"/>
     </row>
     <row r="139" spans="2:13" s="24" customFormat="1" ht="12" customHeight="1">
       <c r="B139" s="82"/>
@@ -15013,20 +15119,20 @@
       <c r="C141" s="84" t="s">
         <v>205</v>
       </c>
-      <c r="D141" s="207" t="s">
+      <c r="D141" s="201" t="s">
         <v>206</v>
       </c>
-      <c r="E141" s="207"/>
-      <c r="F141" s="207"/>
-      <c r="G141" s="207"/>
-      <c r="H141" s="208" t="s">
+      <c r="E141" s="201"/>
+      <c r="F141" s="201"/>
+      <c r="G141" s="201"/>
+      <c r="H141" s="202" t="s">
         <v>11</v>
       </c>
-      <c r="I141" s="208"/>
-      <c r="J141" s="208"/>
-      <c r="K141" s="208"/>
-      <c r="L141" s="208"/>
-      <c r="M141" s="208"/>
+      <c r="I141" s="202"/>
+      <c r="J141" s="202"/>
+      <c r="K141" s="202"/>
+      <c r="L141" s="202"/>
+      <c r="M141" s="202"/>
     </row>
     <row r="142" spans="2:13" s="24" customFormat="1" ht="14.25" customHeight="1">
       <c r="B142" s="85">
@@ -15035,61 +15141,119 @@
       <c r="C142" s="86" t="s">
         <v>207</v>
       </c>
-      <c r="D142" s="209"/>
-      <c r="E142" s="209"/>
-      <c r="F142" s="209"/>
-      <c r="G142" s="209"/>
-      <c r="H142" s="210"/>
-      <c r="I142" s="210"/>
-      <c r="J142" s="210"/>
-      <c r="K142" s="210"/>
-      <c r="L142" s="210"/>
-      <c r="M142" s="210"/>
+      <c r="D142" s="198"/>
+      <c r="E142" s="198"/>
+      <c r="F142" s="198"/>
+      <c r="G142" s="198"/>
+      <c r="H142" s="199"/>
+      <c r="I142" s="199"/>
+      <c r="J142" s="199"/>
+      <c r="K142" s="199"/>
+      <c r="L142" s="199"/>
+      <c r="M142" s="199"/>
     </row>
     <row r="143" spans="2:13" s="24" customFormat="1" ht="14.25" customHeight="1">
       <c r="B143" s="85"/>
       <c r="C143" s="86"/>
-      <c r="D143" s="209"/>
-      <c r="E143" s="209"/>
-      <c r="F143" s="209"/>
-      <c r="G143" s="209"/>
-      <c r="H143" s="210"/>
-      <c r="I143" s="210"/>
-      <c r="J143" s="210"/>
-      <c r="K143" s="210"/>
-      <c r="L143" s="210"/>
-      <c r="M143" s="210"/>
+      <c r="D143" s="198"/>
+      <c r="E143" s="198"/>
+      <c r="F143" s="198"/>
+      <c r="G143" s="198"/>
+      <c r="H143" s="199"/>
+      <c r="I143" s="199"/>
+      <c r="J143" s="199"/>
+      <c r="K143" s="199"/>
+      <c r="L143" s="199"/>
+      <c r="M143" s="199"/>
     </row>
     <row r="144" spans="2:13" s="24" customFormat="1" ht="14.25" customHeight="1">
       <c r="B144" s="85"/>
       <c r="C144" s="86"/>
-      <c r="D144" s="209"/>
-      <c r="E144" s="209"/>
-      <c r="F144" s="209"/>
-      <c r="G144" s="209"/>
-      <c r="H144" s="210"/>
-      <c r="I144" s="210"/>
-      <c r="J144" s="210"/>
-      <c r="K144" s="210"/>
-      <c r="L144" s="210"/>
-      <c r="M144" s="210"/>
+      <c r="D144" s="198"/>
+      <c r="E144" s="198"/>
+      <c r="F144" s="198"/>
+      <c r="G144" s="198"/>
+      <c r="H144" s="199"/>
+      <c r="I144" s="199"/>
+      <c r="J144" s="199"/>
+      <c r="K144" s="199"/>
+      <c r="L144" s="199"/>
+      <c r="M144" s="199"/>
     </row>
     <row r="145" spans="2:13" s="24" customFormat="1" ht="14.25" customHeight="1">
       <c r="B145" s="85"/>
       <c r="C145" s="86"/>
-      <c r="D145" s="209"/>
-      <c r="E145" s="209"/>
-      <c r="F145" s="209"/>
-      <c r="G145" s="209"/>
-      <c r="H145" s="210"/>
-      <c r="I145" s="210"/>
-      <c r="J145" s="210"/>
-      <c r="K145" s="210"/>
-      <c r="L145" s="210"/>
-      <c r="M145" s="210"/>
+      <c r="D145" s="198"/>
+      <c r="E145" s="198"/>
+      <c r="F145" s="198"/>
+      <c r="G145" s="198"/>
+      <c r="H145" s="199"/>
+      <c r="I145" s="199"/>
+      <c r="J145" s="199"/>
+      <c r="K145" s="199"/>
+      <c r="L145" s="199"/>
+      <c r="M145" s="199"/>
     </row>
   </sheetData>
   <mergeCells count="74">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="F106:H106"/>
+    <mergeCell ref="I106:L106"/>
+    <mergeCell ref="M106:P106"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="F107:H107"/>
+    <mergeCell ref="I107:L107"/>
+    <mergeCell ref="M107:P107"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="I108:L108"/>
+    <mergeCell ref="M108:P108"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="F109:H109"/>
+    <mergeCell ref="I109:L109"/>
+    <mergeCell ref="M109:P109"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="F110:H110"/>
+    <mergeCell ref="I110:L110"/>
+    <mergeCell ref="M110:P110"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="F111:H111"/>
+    <mergeCell ref="I111:L111"/>
+    <mergeCell ref="M111:P111"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="F112:H112"/>
+    <mergeCell ref="I112:L112"/>
+    <mergeCell ref="M112:P112"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="F113:H113"/>
+    <mergeCell ref="I113:L113"/>
+    <mergeCell ref="M113:P113"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="F114:H114"/>
+    <mergeCell ref="I114:L114"/>
+    <mergeCell ref="M114:P114"/>
+    <mergeCell ref="M115:P115"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="F116:H116"/>
+    <mergeCell ref="I116:L116"/>
+    <mergeCell ref="M116:P116"/>
+    <mergeCell ref="B138:L138"/>
+    <mergeCell ref="D141:G141"/>
+    <mergeCell ref="H141:M141"/>
+    <mergeCell ref="D142:G142"/>
+    <mergeCell ref="H142:M142"/>
+    <mergeCell ref="D143:G143"/>
+    <mergeCell ref="H143:M143"/>
+    <mergeCell ref="D144:G144"/>
+    <mergeCell ref="H144:M144"/>
+    <mergeCell ref="D145:G145"/>
+    <mergeCell ref="H145:M145"/>
     <mergeCell ref="G119:G120"/>
     <mergeCell ref="E1:J2"/>
     <mergeCell ref="B80:E82"/>
@@ -15106,64 +15270,6 @@
     <mergeCell ref="D115:E115"/>
     <mergeCell ref="F115:H115"/>
     <mergeCell ref="I115:L115"/>
-    <mergeCell ref="D143:G143"/>
-    <mergeCell ref="H143:M143"/>
-    <mergeCell ref="D144:G144"/>
-    <mergeCell ref="H144:M144"/>
-    <mergeCell ref="D145:G145"/>
-    <mergeCell ref="H145:M145"/>
-    <mergeCell ref="B138:L138"/>
-    <mergeCell ref="D141:G141"/>
-    <mergeCell ref="H141:M141"/>
-    <mergeCell ref="D142:G142"/>
-    <mergeCell ref="H142:M142"/>
-    <mergeCell ref="M115:P115"/>
-    <mergeCell ref="D116:E116"/>
-    <mergeCell ref="F116:H116"/>
-    <mergeCell ref="I116:L116"/>
-    <mergeCell ref="M116:P116"/>
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="F113:H113"/>
-    <mergeCell ref="I113:L113"/>
-    <mergeCell ref="M113:P113"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="F114:H114"/>
-    <mergeCell ref="I114:L114"/>
-    <mergeCell ref="M114:P114"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="F111:H111"/>
-    <mergeCell ref="I111:L111"/>
-    <mergeCell ref="M111:P111"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="F112:H112"/>
-    <mergeCell ref="I112:L112"/>
-    <mergeCell ref="M112:P112"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="I109:L109"/>
-    <mergeCell ref="M109:P109"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="F110:H110"/>
-    <mergeCell ref="I110:L110"/>
-    <mergeCell ref="M110:P110"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="F107:H107"/>
-    <mergeCell ref="I107:L107"/>
-    <mergeCell ref="M107:P107"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="F108:H108"/>
-    <mergeCell ref="I108:L108"/>
-    <mergeCell ref="M108:P108"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="F106:H106"/>
-    <mergeCell ref="I106:L106"/>
-    <mergeCell ref="M106:P106"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B85:C85"/>
   </mergeCells>
   <phoneticPr fontId="52" type="noConversion"/>
   <pageMargins left="0.78680555555555598" right="0.78680555555555598" top="0.98263888888888895" bottom="0.98263888888888895" header="0.51180555555555596" footer="0.51180555555555596"/>

</xml_diff>

<commit_message>
fix bug、update document Signed-off-by: LiuYiyang <lyy@shequchina.cn>
</commit_message>
<xml_diff>
--- a/document/AP_障害管理票_QDYL.xlsx
+++ b/document/AP_障害管理票_QDYL.xlsx
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="226">
   <si>
     <t>通番</t>
   </si>
@@ -3237,6 +3237,51 @@
         <family val="2"/>
       </rPr>
       <t>示。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>契約手続き中-&gt;名前-&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>变</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t>更</t>
+    </r>
+    <phoneticPr fontId="52" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>保存按</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>钮</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t>失效</t>
     </r>
   </si>
 </sst>
@@ -5339,6 +5384,84 @@
     <xf numFmtId="180" fontId="15" fillId="0" borderId="25" xfId="346" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="181" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="181" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5359,84 +5482,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="175" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="460">
@@ -6570,8 +6615,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674035"/>
-          <c:y val="3.5190678684544341E-2"/>
+          <c:x val="0.38523037913674041"/>
+          <c:y val="3.5190678684544348E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -6640,11 +6685,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="97052928"/>
-        <c:axId val="97054720"/>
+        <c:axId val="143182080"/>
+        <c:axId val="143187968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="97052928"/>
+        <c:axId val="143182080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6678,14 +6723,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97054720"/>
+        <c:crossAx val="143187968"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97054720"/>
+        <c:axId val="143187968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6719,7 +6764,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97052928"/>
+        <c:crossAx val="143182080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6769,7 +6814,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6806,8 +6851,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674035"/>
-          <c:y val="3.0232730603965516E-2"/>
+          <c:x val="0.38523037913674041"/>
+          <c:y val="3.0232730603965523E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -6823,10 +6868,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11177666498383211"/>
+          <c:x val="0.11177666498383214"/>
           <c:y val="0.100000113553908"/>
           <c:w val="0.78044064301210703"/>
-          <c:h val="0.65814028222689203"/>
+          <c:h val="0.65814028222689225"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -6933,11 +6978,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="132521344"/>
-        <c:axId val="132547712"/>
+        <c:axId val="144256384"/>
+        <c:axId val="144278656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="132521344"/>
+        <c:axId val="144256384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6971,14 +7016,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="132547712"/>
+        <c:crossAx val="144278656"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="132547712"/>
+        <c:axId val="144278656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7012,7 +7057,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="132521344"/>
+        <c:crossAx val="144256384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7062,7 +7107,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7099,8 +7144,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.39506259248458336"/>
-          <c:y val="3.1476997578692822E-2"/>
+          <c:x val="0.39506259248458342"/>
+          <c:y val="3.1476997578692829E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -7118,8 +7163,8 @@
           <c:yMode val="edge"/>
           <c:x val="9.2592778647397928E-2"/>
           <c:y val="0.113801452784504"/>
-          <c:w val="0.77572172333487832"/>
-          <c:h val="0.65133171912833343"/>
+          <c:w val="0.77572172333487865"/>
+          <c:h val="0.65133171912833354"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -7421,8 +7466,8 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="134048384"/>
-        <c:axId val="134062848"/>
+        <c:axId val="148851328"/>
+        <c:axId val="148865792"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -7521,11 +7566,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="134064384"/>
-        <c:axId val="134078464"/>
+        <c:axId val="148867328"/>
+        <c:axId val="148885504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="134048384"/>
+        <c:axId val="148851328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7559,14 +7604,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134062848"/>
+        <c:crossAx val="148865792"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134062848"/>
+        <c:axId val="148865792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7600,29 +7645,29 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134048384"/>
+        <c:crossAx val="148851328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="134064384"/>
+        <c:axId val="148867328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="134078464"/>
+        <c:crossAx val="148885504"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134078464"/>
+        <c:axId val="148885504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
-          <c:min val="0.75000000000000444"/>
+          <c:min val="0.75000000000000455"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
@@ -7654,7 +7699,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134064384"/>
+        <c:crossAx val="148867328"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.05"/>
@@ -7677,8 +7722,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.22633788060443111"/>
-          <c:y val="0.93462469733656872"/>
+          <c:x val="0.22633788060443114"/>
+          <c:y val="0.93462469733656883"/>
           <c:w val="0.50411630644934757"/>
           <c:h val="4.8426150121065097E-2"/>
         </c:manualLayout>
@@ -7746,7 +7791,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7783,8 +7828,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674035"/>
-          <c:y val="3.0232707900360218E-2"/>
+          <c:x val="0.38523037913674041"/>
+          <c:y val="3.0232707900360225E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -7800,10 +7845,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11177666498383211"/>
+          <c:x val="0.11177666498383214"/>
           <c:y val="0.100000113553908"/>
           <c:w val="0.78044064301210703"/>
-          <c:h val="0.65814028222689303"/>
+          <c:h val="0.65814028222689325"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -7865,11 +7910,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="133578112"/>
-        <c:axId val="133588096"/>
+        <c:axId val="151133568"/>
+        <c:axId val="151147648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="133578112"/>
+        <c:axId val="151133568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7903,14 +7948,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133588096"/>
+        <c:crossAx val="151147648"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133588096"/>
+        <c:axId val="151147648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7944,7 +7989,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133578112"/>
+        <c:crossAx val="151133568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7994,7 +8039,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8031,8 +8076,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674035"/>
-          <c:y val="3.5190678684544341E-2"/>
+          <c:x val="0.38523037913674041"/>
+          <c:y val="3.5190678684544348E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -8149,11 +8194,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="133607808"/>
-        <c:axId val="133609344"/>
+        <c:axId val="151175552"/>
+        <c:axId val="151177088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="133607808"/>
+        <c:axId val="151175552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8187,14 +8232,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133609344"/>
+        <c:crossAx val="151177088"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133609344"/>
+        <c:axId val="151177088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8228,7 +8273,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133607808"/>
+        <c:crossAx val="151175552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8278,7 +8323,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8315,8 +8360,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674035"/>
-          <c:y val="3.5190678684544341E-2"/>
+          <c:x val="0.38523037913674041"/>
+          <c:y val="3.5190678684544348E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -8433,11 +8478,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="134501504"/>
-        <c:axId val="134503040"/>
+        <c:axId val="146957440"/>
+        <c:axId val="146958976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="134501504"/>
+        <c:axId val="146957440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8471,14 +8516,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134503040"/>
+        <c:crossAx val="146958976"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134503040"/>
+        <c:axId val="146958976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8512,7 +8557,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134501504"/>
+        <c:crossAx val="146957440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8562,7 +8607,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8599,8 +8644,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674035"/>
-          <c:y val="3.0232707900360218E-2"/>
+          <c:x val="0.38523037913674041"/>
+          <c:y val="3.0232707900360225E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -8616,10 +8661,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11177666498383211"/>
+          <c:x val="0.11177666498383214"/>
           <c:y val="0.100000113553908"/>
           <c:w val="0.78044064301210703"/>
-          <c:h val="0.65814028222689303"/>
+          <c:h val="0.65814028222689325"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -8681,11 +8726,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="134526848"/>
-        <c:axId val="134528384"/>
+        <c:axId val="146974592"/>
+        <c:axId val="146976128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="134526848"/>
+        <c:axId val="146974592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8719,14 +8764,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134528384"/>
+        <c:crossAx val="146976128"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134528384"/>
+        <c:axId val="146976128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8760,7 +8805,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134526848"/>
+        <c:crossAx val="146974592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8810,7 +8855,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9560,7 +9605,7 @@
   <dimension ref="A1:AC111"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="1" topLeftCell="J32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="1" topLeftCell="J29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="I49" sqref="I49"/>
@@ -11431,17 +11476,33 @@
       <c r="AB36" s="183"/>
     </row>
     <row r="37" spans="2:28" ht="14.25" customHeight="1">
-      <c r="B37" s="90"/>
-      <c r="C37" s="105"/>
-      <c r="D37" s="114"/>
+      <c r="B37" s="90">
+        <v>35</v>
+      </c>
+      <c r="C37" s="105" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="114" t="s">
+        <v>27</v>
+      </c>
       <c r="E37" s="113"/>
-      <c r="F37" s="108"/>
+      <c r="F37" s="108" t="s">
+        <v>29</v>
+      </c>
       <c r="G37" s="101"/>
       <c r="H37" s="116"/>
-      <c r="I37" s="144"/>
-      <c r="J37" s="129"/>
-      <c r="K37" s="145"/>
-      <c r="L37" s="115"/>
+      <c r="I37" s="144" t="s">
+        <v>224</v>
+      </c>
+      <c r="J37" s="129">
+        <v>43280</v>
+      </c>
+      <c r="K37" s="156" t="s">
+        <v>38</v>
+      </c>
+      <c r="L37" s="115" t="s">
+        <v>225</v>
+      </c>
       <c r="M37" s="147"/>
       <c r="N37" s="128"/>
       <c r="O37" s="128"/>
@@ -13311,30 +13372,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="9" customHeight="1">
-      <c r="E1" s="188"/>
-      <c r="F1" s="188"/>
-      <c r="G1" s="188"/>
-      <c r="H1" s="188"/>
-      <c r="I1" s="188"/>
-      <c r="J1" s="188"/>
+      <c r="E1" s="214"/>
+      <c r="F1" s="214"/>
+      <c r="G1" s="214"/>
+      <c r="H1" s="214"/>
+      <c r="I1" s="214"/>
+      <c r="J1" s="214"/>
     </row>
     <row r="2" spans="2:10" ht="15" customHeight="1">
       <c r="B2" s="26" t="s">
         <v>128</v>
       </c>
       <c r="C2" s="26"/>
-      <c r="E2" s="188"/>
-      <c r="F2" s="188"/>
-      <c r="G2" s="188"/>
-      <c r="H2" s="188"/>
-      <c r="I2" s="188"/>
-      <c r="J2" s="188"/>
+      <c r="E2" s="214"/>
+      <c r="F2" s="214"/>
+      <c r="G2" s="214"/>
+      <c r="H2" s="214"/>
+      <c r="I2" s="214"/>
+      <c r="J2" s="214"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1">
-      <c r="B3" s="217" t="s">
+      <c r="B3" s="186" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="218"/>
+      <c r="C3" s="187"/>
       <c r="D3" s="27" t="s">
         <v>129</v>
       </c>
@@ -13412,30 +13473,30 @@
       </c>
     </row>
     <row r="13" spans="2:10" ht="17.25" customHeight="1">
-      <c r="B13" s="189" t="s">
+      <c r="B13" s="215" t="s">
         <v>134</v>
       </c>
-      <c r="C13" s="189"/>
-      <c r="D13" s="189"/>
-      <c r="E13" s="189"/>
+      <c r="C13" s="215"/>
+      <c r="D13" s="215"/>
+      <c r="E13" s="215"/>
     </row>
     <row r="14" spans="2:10" ht="17.25" customHeight="1">
-      <c r="B14" s="189"/>
-      <c r="C14" s="189"/>
-      <c r="D14" s="189"/>
-      <c r="E14" s="189"/>
+      <c r="B14" s="215"/>
+      <c r="C14" s="215"/>
+      <c r="D14" s="215"/>
+      <c r="E14" s="215"/>
     </row>
     <row r="15" spans="2:10" ht="17.25" customHeight="1">
-      <c r="B15" s="189"/>
-      <c r="C15" s="189"/>
-      <c r="D15" s="189"/>
-      <c r="E15" s="189"/>
+      <c r="B15" s="215"/>
+      <c r="C15" s="215"/>
+      <c r="D15" s="215"/>
+      <c r="E15" s="215"/>
     </row>
     <row r="16" spans="2:10" ht="17.25" customHeight="1">
-      <c r="B16" s="189"/>
-      <c r="C16" s="189"/>
-      <c r="D16" s="189"/>
-      <c r="E16" s="189"/>
+      <c r="B16" s="215"/>
+      <c r="C16" s="215"/>
+      <c r="D16" s="215"/>
+      <c r="E16" s="215"/>
     </row>
     <row r="21" spans="2:5" ht="15" customHeight="1">
       <c r="B21" s="26" t="s">
@@ -13444,10 +13505,10 @@
       <c r="C21" s="26"/>
     </row>
     <row r="22" spans="2:5" ht="15" customHeight="1">
-      <c r="B22" s="217" t="s">
+      <c r="B22" s="186" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="218"/>
+      <c r="C22" s="187"/>
       <c r="D22" s="27" t="s">
         <v>129</v>
       </c>
@@ -13629,30 +13690,30 @@
       </c>
     </row>
     <row r="36" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B36" s="189" t="s">
+      <c r="B36" s="215" t="s">
         <v>134</v>
       </c>
-      <c r="C36" s="189"/>
-      <c r="D36" s="189"/>
-      <c r="E36" s="189"/>
+      <c r="C36" s="215"/>
+      <c r="D36" s="215"/>
+      <c r="E36" s="215"/>
     </row>
     <row r="37" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B37" s="189"/>
-      <c r="C37" s="189"/>
-      <c r="D37" s="189"/>
-      <c r="E37" s="189"/>
+      <c r="B37" s="215"/>
+      <c r="C37" s="215"/>
+      <c r="D37" s="215"/>
+      <c r="E37" s="215"/>
     </row>
     <row r="38" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B38" s="189"/>
-      <c r="C38" s="189"/>
-      <c r="D38" s="189"/>
-      <c r="E38" s="189"/>
+      <c r="B38" s="215"/>
+      <c r="C38" s="215"/>
+      <c r="D38" s="215"/>
+      <c r="E38" s="215"/>
     </row>
     <row r="39" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B39" s="189"/>
-      <c r="C39" s="189"/>
-      <c r="D39" s="189"/>
-      <c r="E39" s="189"/>
+      <c r="B39" s="215"/>
+      <c r="C39" s="215"/>
+      <c r="D39" s="215"/>
+      <c r="E39" s="215"/>
     </row>
     <row r="43" spans="2:5" ht="15" customHeight="1">
       <c r="B43" s="26" t="s">
@@ -13661,10 +13722,10 @@
       <c r="C43" s="26"/>
     </row>
     <row r="44" spans="2:5" ht="15" customHeight="1">
-      <c r="B44" s="217" t="s">
+      <c r="B44" s="186" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="218"/>
+      <c r="C44" s="187"/>
       <c r="D44" s="27" t="s">
         <v>129</v>
       </c>
@@ -13818,30 +13879,30 @@
       </c>
     </row>
     <row r="56" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B56" s="189" t="s">
+      <c r="B56" s="215" t="s">
         <v>134</v>
       </c>
-      <c r="C56" s="189"/>
-      <c r="D56" s="189"/>
-      <c r="E56" s="189"/>
+      <c r="C56" s="215"/>
+      <c r="D56" s="215"/>
+      <c r="E56" s="215"/>
     </row>
     <row r="57" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B57" s="189"/>
-      <c r="C57" s="189"/>
-      <c r="D57" s="189"/>
-      <c r="E57" s="189"/>
+      <c r="B57" s="215"/>
+      <c r="C57" s="215"/>
+      <c r="D57" s="215"/>
+      <c r="E57" s="215"/>
     </row>
     <row r="58" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B58" s="189"/>
-      <c r="C58" s="189"/>
-      <c r="D58" s="189"/>
-      <c r="E58" s="189"/>
+      <c r="B58" s="215"/>
+      <c r="C58" s="215"/>
+      <c r="D58" s="215"/>
+      <c r="E58" s="215"/>
     </row>
     <row r="59" spans="2:5" ht="17.25" customHeight="1">
-      <c r="B59" s="189"/>
-      <c r="C59" s="189"/>
-      <c r="D59" s="189"/>
-      <c r="E59" s="189"/>
+      <c r="B59" s="215"/>
+      <c r="C59" s="215"/>
+      <c r="D59" s="215"/>
+      <c r="E59" s="215"/>
     </row>
     <row r="64" spans="2:5" ht="17.25" customHeight="1">
       <c r="B64" s="26" t="s">
@@ -13850,10 +13911,10 @@
       <c r="C64" s="26"/>
     </row>
     <row r="65" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B65" s="210" t="s">
+      <c r="B65" s="188" t="s">
         <v>17</v>
       </c>
-      <c r="C65" s="211"/>
+      <c r="C65" s="189"/>
       <c r="D65" s="27" t="s">
         <v>129</v>
       </c>
@@ -14033,28 +14094,28 @@
       <c r="E79" s="24"/>
     </row>
     <row r="80" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B80" s="189" t="s">
+      <c r="B80" s="215" t="s">
         <v>173</v>
       </c>
-      <c r="C80" s="189"/>
-      <c r="D80" s="189"/>
-      <c r="E80" s="189"/>
+      <c r="C80" s="215"/>
+      <c r="D80" s="215"/>
+      <c r="E80" s="215"/>
       <c r="F80" s="24"/>
       <c r="G80" s="24"/>
     </row>
     <row r="81" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B81" s="189"/>
-      <c r="C81" s="189"/>
-      <c r="D81" s="189"/>
-      <c r="E81" s="189"/>
+      <c r="B81" s="215"/>
+      <c r="C81" s="215"/>
+      <c r="D81" s="215"/>
+      <c r="E81" s="215"/>
       <c r="F81" s="50"/>
       <c r="G81" s="50"/>
     </row>
     <row r="82" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B82" s="189"/>
-      <c r="C82" s="189"/>
-      <c r="D82" s="189"/>
-      <c r="E82" s="189"/>
+      <c r="B82" s="215"/>
+      <c r="C82" s="215"/>
+      <c r="D82" s="215"/>
+      <c r="E82" s="215"/>
       <c r="F82" s="50"/>
       <c r="G82" s="50"/>
     </row>
@@ -14073,10 +14134,10 @@
       <c r="C84" s="26"/>
     </row>
     <row r="85" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B85" s="210" t="s">
+      <c r="B85" s="188" t="s">
         <v>18</v>
       </c>
-      <c r="C85" s="211"/>
+      <c r="C85" s="189"/>
       <c r="D85" s="27" t="s">
         <v>129</v>
       </c>
@@ -14148,28 +14209,28 @@
       <c r="E90" s="24"/>
     </row>
     <row r="91" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B91" s="189" t="s">
+      <c r="B91" s="215" t="s">
         <v>173</v>
       </c>
-      <c r="C91" s="189"/>
-      <c r="D91" s="189"/>
-      <c r="E91" s="189"/>
+      <c r="C91" s="215"/>
+      <c r="D91" s="215"/>
+      <c r="E91" s="215"/>
       <c r="F91" s="24"/>
       <c r="G91" s="24"/>
     </row>
     <row r="92" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B92" s="189"/>
-      <c r="C92" s="189"/>
-      <c r="D92" s="189"/>
-      <c r="E92" s="189"/>
+      <c r="B92" s="215"/>
+      <c r="C92" s="215"/>
+      <c r="D92" s="215"/>
+      <c r="E92" s="215"/>
       <c r="F92" s="50"/>
       <c r="G92" s="50"/>
     </row>
     <row r="93" spans="2:7" ht="23.25" customHeight="1">
-      <c r="B93" s="189"/>
-      <c r="C93" s="189"/>
-      <c r="D93" s="189"/>
-      <c r="E93" s="189"/>
+      <c r="B93" s="215"/>
+      <c r="C93" s="215"/>
+      <c r="D93" s="215"/>
+      <c r="E93" s="215"/>
       <c r="F93" s="50"/>
       <c r="G93" s="50"/>
     </row>
@@ -14188,10 +14249,10 @@
       <c r="C95" s="26"/>
     </row>
     <row r="96" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B96" s="210" t="s">
+      <c r="B96" s="188" t="s">
         <v>18</v>
       </c>
-      <c r="C96" s="211"/>
+      <c r="C96" s="189"/>
       <c r="D96" s="27" t="s">
         <v>129</v>
       </c>
@@ -14249,28 +14310,28 @@
       <c r="E100" s="24"/>
     </row>
     <row r="101" spans="1:50" ht="23.25" customHeight="1">
-      <c r="B101" s="189" t="s">
+      <c r="B101" s="215" t="s">
         <v>173</v>
       </c>
-      <c r="C101" s="189"/>
-      <c r="D101" s="189"/>
-      <c r="E101" s="189"/>
+      <c r="C101" s="215"/>
+      <c r="D101" s="215"/>
+      <c r="E101" s="215"/>
       <c r="F101" s="24"/>
       <c r="G101" s="24"/>
     </row>
     <row r="102" spans="1:50" ht="23.25" customHeight="1">
-      <c r="B102" s="189"/>
-      <c r="C102" s="189"/>
-      <c r="D102" s="189"/>
-      <c r="E102" s="189"/>
+      <c r="B102" s="215"/>
+      <c r="C102" s="215"/>
+      <c r="D102" s="215"/>
+      <c r="E102" s="215"/>
       <c r="F102" s="50"/>
       <c r="G102" s="50"/>
     </row>
     <row r="103" spans="1:50" ht="23.25" customHeight="1">
-      <c r="B103" s="189"/>
-      <c r="C103" s="189"/>
-      <c r="D103" s="189"/>
-      <c r="E103" s="189"/>
+      <c r="B103" s="215"/>
+      <c r="C103" s="215"/>
+      <c r="D103" s="215"/>
+      <c r="E103" s="215"/>
       <c r="F103" s="50"/>
       <c r="G103" s="50"/>
     </row>
@@ -14312,27 +14373,27 @@
       <c r="C106" s="55" t="s">
         <v>183</v>
       </c>
-      <c r="D106" s="212" t="s">
+      <c r="D106" s="190" t="s">
         <v>184</v>
       </c>
-      <c r="E106" s="213"/>
-      <c r="F106" s="214" t="s">
+      <c r="E106" s="191"/>
+      <c r="F106" s="192" t="s">
         <v>185</v>
       </c>
-      <c r="G106" s="215"/>
-      <c r="H106" s="216"/>
-      <c r="I106" s="214" t="s">
+      <c r="G106" s="193"/>
+      <c r="H106" s="194"/>
+      <c r="I106" s="192" t="s">
         <v>186</v>
       </c>
-      <c r="J106" s="215"/>
-      <c r="K106" s="215"/>
-      <c r="L106" s="216"/>
-      <c r="M106" s="214" t="s">
+      <c r="J106" s="193"/>
+      <c r="K106" s="193"/>
+      <c r="L106" s="194"/>
+      <c r="M106" s="192" t="s">
         <v>187</v>
       </c>
-      <c r="N106" s="215"/>
-      <c r="O106" s="215"/>
-      <c r="P106" s="216"/>
+      <c r="N106" s="193"/>
+      <c r="O106" s="193"/>
+      <c r="P106" s="194"/>
       <c r="Q106" s="63" t="s">
         <v>188</v>
       </c>
@@ -14353,27 +14414,27 @@
       <c r="C107" s="57" t="s">
         <v>191</v>
       </c>
-      <c r="D107" s="204" t="s">
+      <c r="D107" s="195" t="s">
         <v>192</v>
       </c>
-      <c r="E107" s="205"/>
-      <c r="F107" s="206" t="s">
+      <c r="E107" s="196"/>
+      <c r="F107" s="197" t="s">
         <v>193</v>
       </c>
-      <c r="G107" s="207"/>
-      <c r="H107" s="208"/>
-      <c r="I107" s="206" t="s">
+      <c r="G107" s="198"/>
+      <c r="H107" s="199"/>
+      <c r="I107" s="197" t="s">
         <v>194</v>
       </c>
-      <c r="J107" s="207"/>
-      <c r="K107" s="207"/>
-      <c r="L107" s="208"/>
-      <c r="M107" s="209" t="s">
+      <c r="J107" s="198"/>
+      <c r="K107" s="198"/>
+      <c r="L107" s="199"/>
+      <c r="M107" s="200" t="s">
         <v>195</v>
       </c>
-      <c r="N107" s="209"/>
-      <c r="O107" s="209"/>
-      <c r="P107" s="209"/>
+      <c r="N107" s="200"/>
+      <c r="O107" s="200"/>
+      <c r="P107" s="200"/>
       <c r="Q107" s="71" t="s">
         <v>196</v>
       </c>
@@ -14390,19 +14451,19 @@
     <row r="108" spans="1:50" s="23" customFormat="1" ht="11.25">
       <c r="B108" s="58"/>
       <c r="C108" s="59"/>
-      <c r="D108" s="193"/>
-      <c r="E108" s="194"/>
-      <c r="F108" s="195"/>
-      <c r="G108" s="196"/>
-      <c r="H108" s="197"/>
-      <c r="I108" s="195"/>
-      <c r="J108" s="196"/>
-      <c r="K108" s="196"/>
-      <c r="L108" s="197"/>
-      <c r="M108" s="203"/>
-      <c r="N108" s="203"/>
-      <c r="O108" s="203"/>
-      <c r="P108" s="203"/>
+      <c r="D108" s="201"/>
+      <c r="E108" s="202"/>
+      <c r="F108" s="203"/>
+      <c r="G108" s="204"/>
+      <c r="H108" s="205"/>
+      <c r="I108" s="203"/>
+      <c r="J108" s="204"/>
+      <c r="K108" s="204"/>
+      <c r="L108" s="205"/>
+      <c r="M108" s="206"/>
+      <c r="N108" s="206"/>
+      <c r="O108" s="206"/>
+      <c r="P108" s="206"/>
       <c r="Q108" s="73"/>
       <c r="R108" s="74"/>
       <c r="U108" s="70"/>
@@ -14415,19 +14476,19 @@
     <row r="109" spans="1:50" s="23" customFormat="1" ht="11.25">
       <c r="B109" s="58"/>
       <c r="C109" s="59"/>
-      <c r="D109" s="193"/>
-      <c r="E109" s="194"/>
-      <c r="F109" s="195"/>
-      <c r="G109" s="196"/>
-      <c r="H109" s="197"/>
-      <c r="I109" s="195"/>
-      <c r="J109" s="196"/>
-      <c r="K109" s="196"/>
-      <c r="L109" s="197"/>
-      <c r="M109" s="203"/>
-      <c r="N109" s="203"/>
-      <c r="O109" s="203"/>
-      <c r="P109" s="203"/>
+      <c r="D109" s="201"/>
+      <c r="E109" s="202"/>
+      <c r="F109" s="203"/>
+      <c r="G109" s="204"/>
+      <c r="H109" s="205"/>
+      <c r="I109" s="203"/>
+      <c r="J109" s="204"/>
+      <c r="K109" s="204"/>
+      <c r="L109" s="205"/>
+      <c r="M109" s="206"/>
+      <c r="N109" s="206"/>
+      <c r="O109" s="206"/>
+      <c r="P109" s="206"/>
       <c r="Q109" s="73"/>
       <c r="R109" s="74"/>
       <c r="U109" s="70"/>
@@ -14440,19 +14501,19 @@
     <row r="110" spans="1:50" s="23" customFormat="1" ht="11.25">
       <c r="B110" s="58"/>
       <c r="C110" s="59"/>
-      <c r="D110" s="193"/>
-      <c r="E110" s="194"/>
-      <c r="F110" s="195"/>
-      <c r="G110" s="196"/>
-      <c r="H110" s="197"/>
-      <c r="I110" s="195"/>
-      <c r="J110" s="196"/>
-      <c r="K110" s="196"/>
-      <c r="L110" s="197"/>
-      <c r="M110" s="203"/>
-      <c r="N110" s="203"/>
-      <c r="O110" s="203"/>
-      <c r="P110" s="203"/>
+      <c r="D110" s="201"/>
+      <c r="E110" s="202"/>
+      <c r="F110" s="203"/>
+      <c r="G110" s="204"/>
+      <c r="H110" s="205"/>
+      <c r="I110" s="203"/>
+      <c r="J110" s="204"/>
+      <c r="K110" s="204"/>
+      <c r="L110" s="205"/>
+      <c r="M110" s="206"/>
+      <c r="N110" s="206"/>
+      <c r="O110" s="206"/>
+      <c r="P110" s="206"/>
       <c r="Q110" s="73"/>
       <c r="R110" s="74"/>
       <c r="U110" s="70"/>
@@ -14465,19 +14526,19 @@
     <row r="111" spans="1:50" s="23" customFormat="1" ht="11.25">
       <c r="B111" s="58"/>
       <c r="C111" s="59"/>
-      <c r="D111" s="193"/>
-      <c r="E111" s="194"/>
-      <c r="F111" s="195"/>
-      <c r="G111" s="196"/>
-      <c r="H111" s="197"/>
-      <c r="I111" s="195"/>
-      <c r="J111" s="196"/>
-      <c r="K111" s="196"/>
-      <c r="L111" s="197"/>
-      <c r="M111" s="203"/>
-      <c r="N111" s="203"/>
-      <c r="O111" s="203"/>
-      <c r="P111" s="203"/>
+      <c r="D111" s="201"/>
+      <c r="E111" s="202"/>
+      <c r="F111" s="203"/>
+      <c r="G111" s="204"/>
+      <c r="H111" s="205"/>
+      <c r="I111" s="203"/>
+      <c r="J111" s="204"/>
+      <c r="K111" s="204"/>
+      <c r="L111" s="205"/>
+      <c r="M111" s="206"/>
+      <c r="N111" s="206"/>
+      <c r="O111" s="206"/>
+      <c r="P111" s="206"/>
       <c r="Q111" s="73"/>
       <c r="R111" s="74"/>
       <c r="U111" s="70"/>
@@ -14490,19 +14551,19 @@
     <row r="112" spans="1:50" s="23" customFormat="1" ht="11.25">
       <c r="B112" s="58"/>
       <c r="C112" s="59"/>
-      <c r="D112" s="193"/>
-      <c r="E112" s="194"/>
-      <c r="F112" s="195"/>
-      <c r="G112" s="196"/>
-      <c r="H112" s="197"/>
-      <c r="I112" s="195"/>
-      <c r="J112" s="196"/>
-      <c r="K112" s="196"/>
-      <c r="L112" s="197"/>
-      <c r="M112" s="203"/>
-      <c r="N112" s="203"/>
-      <c r="O112" s="203"/>
-      <c r="P112" s="203"/>
+      <c r="D112" s="201"/>
+      <c r="E112" s="202"/>
+      <c r="F112" s="203"/>
+      <c r="G112" s="204"/>
+      <c r="H112" s="205"/>
+      <c r="I112" s="203"/>
+      <c r="J112" s="204"/>
+      <c r="K112" s="204"/>
+      <c r="L112" s="205"/>
+      <c r="M112" s="206"/>
+      <c r="N112" s="206"/>
+      <c r="O112" s="206"/>
+      <c r="P112" s="206"/>
       <c r="Q112" s="73"/>
       <c r="R112" s="74"/>
       <c r="U112" s="70"/>
@@ -14515,19 +14576,19 @@
     <row r="113" spans="2:26" s="23" customFormat="1" ht="11.25">
       <c r="B113" s="58"/>
       <c r="C113" s="59"/>
-      <c r="D113" s="193"/>
-      <c r="E113" s="194"/>
-      <c r="F113" s="195"/>
-      <c r="G113" s="196"/>
-      <c r="H113" s="197"/>
-      <c r="I113" s="195"/>
-      <c r="J113" s="196"/>
-      <c r="K113" s="196"/>
-      <c r="L113" s="197"/>
-      <c r="M113" s="203"/>
-      <c r="N113" s="203"/>
-      <c r="O113" s="203"/>
-      <c r="P113" s="203"/>
+      <c r="D113" s="201"/>
+      <c r="E113" s="202"/>
+      <c r="F113" s="203"/>
+      <c r="G113" s="204"/>
+      <c r="H113" s="205"/>
+      <c r="I113" s="203"/>
+      <c r="J113" s="204"/>
+      <c r="K113" s="204"/>
+      <c r="L113" s="205"/>
+      <c r="M113" s="206"/>
+      <c r="N113" s="206"/>
+      <c r="O113" s="206"/>
+      <c r="P113" s="206"/>
       <c r="Q113" s="73"/>
       <c r="R113" s="74"/>
       <c r="U113" s="70"/>
@@ -14540,19 +14601,19 @@
     <row r="114" spans="2:26" s="23" customFormat="1" ht="11.25">
       <c r="B114" s="58"/>
       <c r="C114" s="59"/>
-      <c r="D114" s="193"/>
-      <c r="E114" s="194"/>
-      <c r="F114" s="195"/>
-      <c r="G114" s="196"/>
-      <c r="H114" s="197"/>
-      <c r="I114" s="195"/>
-      <c r="J114" s="196"/>
-      <c r="K114" s="196"/>
-      <c r="L114" s="197"/>
-      <c r="M114" s="203"/>
-      <c r="N114" s="203"/>
-      <c r="O114" s="203"/>
-      <c r="P114" s="203"/>
+      <c r="D114" s="201"/>
+      <c r="E114" s="202"/>
+      <c r="F114" s="203"/>
+      <c r="G114" s="204"/>
+      <c r="H114" s="205"/>
+      <c r="I114" s="203"/>
+      <c r="J114" s="204"/>
+      <c r="K114" s="204"/>
+      <c r="L114" s="205"/>
+      <c r="M114" s="206"/>
+      <c r="N114" s="206"/>
+      <c r="O114" s="206"/>
+      <c r="P114" s="206"/>
       <c r="Q114" s="73"/>
       <c r="R114" s="74"/>
       <c r="U114" s="70"/>
@@ -14565,19 +14626,19 @@
     <row r="115" spans="2:26" s="23" customFormat="1" ht="11.25">
       <c r="B115" s="58"/>
       <c r="C115" s="59"/>
-      <c r="D115" s="193"/>
-      <c r="E115" s="194"/>
-      <c r="F115" s="195"/>
-      <c r="G115" s="196"/>
-      <c r="H115" s="197"/>
-      <c r="I115" s="195"/>
-      <c r="J115" s="196"/>
-      <c r="K115" s="196"/>
-      <c r="L115" s="197"/>
-      <c r="M115" s="203"/>
-      <c r="N115" s="203"/>
-      <c r="O115" s="203"/>
-      <c r="P115" s="203"/>
+      <c r="D115" s="201"/>
+      <c r="E115" s="202"/>
+      <c r="F115" s="203"/>
+      <c r="G115" s="204"/>
+      <c r="H115" s="205"/>
+      <c r="I115" s="203"/>
+      <c r="J115" s="204"/>
+      <c r="K115" s="204"/>
+      <c r="L115" s="205"/>
+      <c r="M115" s="206"/>
+      <c r="N115" s="206"/>
+      <c r="O115" s="206"/>
+      <c r="P115" s="206"/>
       <c r="Q115" s="73"/>
       <c r="R115" s="74"/>
       <c r="U115" s="70"/>
@@ -14590,19 +14651,19 @@
     <row r="116" spans="2:26" s="23" customFormat="1" ht="11.25">
       <c r="B116" s="58"/>
       <c r="C116" s="59"/>
-      <c r="D116" s="193"/>
-      <c r="E116" s="194"/>
-      <c r="F116" s="195"/>
-      <c r="G116" s="196"/>
-      <c r="H116" s="197"/>
-      <c r="I116" s="195"/>
-      <c r="J116" s="196"/>
-      <c r="K116" s="196"/>
-      <c r="L116" s="197"/>
-      <c r="M116" s="203"/>
-      <c r="N116" s="203"/>
-      <c r="O116" s="203"/>
-      <c r="P116" s="203"/>
+      <c r="D116" s="201"/>
+      <c r="E116" s="202"/>
+      <c r="F116" s="203"/>
+      <c r="G116" s="204"/>
+      <c r="H116" s="205"/>
+      <c r="I116" s="203"/>
+      <c r="J116" s="204"/>
+      <c r="K116" s="204"/>
+      <c r="L116" s="205"/>
+      <c r="M116" s="206"/>
+      <c r="N116" s="206"/>
+      <c r="O116" s="206"/>
+      <c r="P116" s="206"/>
       <c r="Q116" s="73"/>
       <c r="R116" s="74"/>
       <c r="U116" s="70"/>
@@ -14629,32 +14690,32 @@
       <c r="G118" s="50"/>
     </row>
     <row r="119" spans="2:26" ht="17.25" customHeight="1">
-      <c r="B119" s="190" t="s">
+      <c r="B119" s="216" t="s">
         <v>183</v>
       </c>
-      <c r="C119" s="190" t="s">
+      <c r="C119" s="216" t="s">
         <v>198</v>
       </c>
-      <c r="D119" s="190" t="s">
+      <c r="D119" s="216" t="s">
         <v>199</v>
       </c>
-      <c r="E119" s="190" t="s">
+      <c r="E119" s="216" t="s">
         <v>200</v>
       </c>
-      <c r="F119" s="192" t="s">
+      <c r="F119" s="218" t="s">
         <v>201</v>
       </c>
-      <c r="G119" s="186" t="s">
+      <c r="G119" s="212" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="120" spans="2:26" ht="17.25" customHeight="1">
-      <c r="B120" s="191"/>
-      <c r="C120" s="191"/>
-      <c r="D120" s="191"/>
-      <c r="E120" s="191"/>
-      <c r="F120" s="192"/>
-      <c r="G120" s="187"/>
+      <c r="B120" s="217"/>
+      <c r="C120" s="217"/>
+      <c r="D120" s="217"/>
+      <c r="E120" s="217"/>
+      <c r="F120" s="218"/>
+      <c r="G120" s="213"/>
     </row>
     <row r="121" spans="2:26" ht="17.25" customHeight="1">
       <c r="B121" s="64">
@@ -15070,19 +15131,19 @@
       <c r="L137" s="88"/>
     </row>
     <row r="138" spans="2:13" s="24" customFormat="1" ht="59.25" customHeight="1">
-      <c r="B138" s="200" t="s">
+      <c r="B138" s="207" t="s">
         <v>203</v>
       </c>
-      <c r="C138" s="200"/>
-      <c r="D138" s="200"/>
-      <c r="E138" s="200"/>
-      <c r="F138" s="200"/>
-      <c r="G138" s="200"/>
-      <c r="H138" s="200"/>
-      <c r="I138" s="200"/>
-      <c r="J138" s="200"/>
-      <c r="K138" s="200"/>
-      <c r="L138" s="200"/>
+      <c r="C138" s="207"/>
+      <c r="D138" s="207"/>
+      <c r="E138" s="207"/>
+      <c r="F138" s="207"/>
+      <c r="G138" s="207"/>
+      <c r="H138" s="207"/>
+      <c r="I138" s="207"/>
+      <c r="J138" s="207"/>
+      <c r="K138" s="207"/>
+      <c r="L138" s="207"/>
     </row>
     <row r="139" spans="2:13" s="24" customFormat="1" ht="12" customHeight="1">
       <c r="B139" s="82"/>
@@ -15119,20 +15180,20 @@
       <c r="C141" s="84" t="s">
         <v>205</v>
       </c>
-      <c r="D141" s="201" t="s">
+      <c r="D141" s="208" t="s">
         <v>206</v>
       </c>
-      <c r="E141" s="201"/>
-      <c r="F141" s="201"/>
-      <c r="G141" s="201"/>
-      <c r="H141" s="202" t="s">
+      <c r="E141" s="208"/>
+      <c r="F141" s="208"/>
+      <c r="G141" s="208"/>
+      <c r="H141" s="209" t="s">
         <v>11</v>
       </c>
-      <c r="I141" s="202"/>
-      <c r="J141" s="202"/>
-      <c r="K141" s="202"/>
-      <c r="L141" s="202"/>
-      <c r="M141" s="202"/>
+      <c r="I141" s="209"/>
+      <c r="J141" s="209"/>
+      <c r="K141" s="209"/>
+      <c r="L141" s="209"/>
+      <c r="M141" s="209"/>
     </row>
     <row r="142" spans="2:13" s="24" customFormat="1" ht="14.25" customHeight="1">
       <c r="B142" s="85">
@@ -15141,119 +15202,61 @@
       <c r="C142" s="86" t="s">
         <v>207</v>
       </c>
-      <c r="D142" s="198"/>
-      <c r="E142" s="198"/>
-      <c r="F142" s="198"/>
-      <c r="G142" s="198"/>
-      <c r="H142" s="199"/>
-      <c r="I142" s="199"/>
-      <c r="J142" s="199"/>
-      <c r="K142" s="199"/>
-      <c r="L142" s="199"/>
-      <c r="M142" s="199"/>
+      <c r="D142" s="210"/>
+      <c r="E142" s="210"/>
+      <c r="F142" s="210"/>
+      <c r="G142" s="210"/>
+      <c r="H142" s="211"/>
+      <c r="I142" s="211"/>
+      <c r="J142" s="211"/>
+      <c r="K142" s="211"/>
+      <c r="L142" s="211"/>
+      <c r="M142" s="211"/>
     </row>
     <row r="143" spans="2:13" s="24" customFormat="1" ht="14.25" customHeight="1">
       <c r="B143" s="85"/>
       <c r="C143" s="86"/>
-      <c r="D143" s="198"/>
-      <c r="E143" s="198"/>
-      <c r="F143" s="198"/>
-      <c r="G143" s="198"/>
-      <c r="H143" s="199"/>
-      <c r="I143" s="199"/>
-      <c r="J143" s="199"/>
-      <c r="K143" s="199"/>
-      <c r="L143" s="199"/>
-      <c r="M143" s="199"/>
+      <c r="D143" s="210"/>
+      <c r="E143" s="210"/>
+      <c r="F143" s="210"/>
+      <c r="G143" s="210"/>
+      <c r="H143" s="211"/>
+      <c r="I143" s="211"/>
+      <c r="J143" s="211"/>
+      <c r="K143" s="211"/>
+      <c r="L143" s="211"/>
+      <c r="M143" s="211"/>
     </row>
     <row r="144" spans="2:13" s="24" customFormat="1" ht="14.25" customHeight="1">
       <c r="B144" s="85"/>
       <c r="C144" s="86"/>
-      <c r="D144" s="198"/>
-      <c r="E144" s="198"/>
-      <c r="F144" s="198"/>
-      <c r="G144" s="198"/>
-      <c r="H144" s="199"/>
-      <c r="I144" s="199"/>
-      <c r="J144" s="199"/>
-      <c r="K144" s="199"/>
-      <c r="L144" s="199"/>
-      <c r="M144" s="199"/>
+      <c r="D144" s="210"/>
+      <c r="E144" s="210"/>
+      <c r="F144" s="210"/>
+      <c r="G144" s="210"/>
+      <c r="H144" s="211"/>
+      <c r="I144" s="211"/>
+      <c r="J144" s="211"/>
+      <c r="K144" s="211"/>
+      <c r="L144" s="211"/>
+      <c r="M144" s="211"/>
     </row>
     <row r="145" spans="2:13" s="24" customFormat="1" ht="14.25" customHeight="1">
       <c r="B145" s="85"/>
       <c r="C145" s="86"/>
-      <c r="D145" s="198"/>
-      <c r="E145" s="198"/>
-      <c r="F145" s="198"/>
-      <c r="G145" s="198"/>
-      <c r="H145" s="199"/>
-      <c r="I145" s="199"/>
-      <c r="J145" s="199"/>
-      <c r="K145" s="199"/>
-      <c r="L145" s="199"/>
-      <c r="M145" s="199"/>
+      <c r="D145" s="210"/>
+      <c r="E145" s="210"/>
+      <c r="F145" s="210"/>
+      <c r="G145" s="210"/>
+      <c r="H145" s="211"/>
+      <c r="I145" s="211"/>
+      <c r="J145" s="211"/>
+      <c r="K145" s="211"/>
+      <c r="L145" s="211"/>
+      <c r="M145" s="211"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="F106:H106"/>
-    <mergeCell ref="I106:L106"/>
-    <mergeCell ref="M106:P106"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="F107:H107"/>
-    <mergeCell ref="I107:L107"/>
-    <mergeCell ref="M107:P107"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="F108:H108"/>
-    <mergeCell ref="I108:L108"/>
-    <mergeCell ref="M108:P108"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="I109:L109"/>
-    <mergeCell ref="M109:P109"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="F110:H110"/>
-    <mergeCell ref="I110:L110"/>
-    <mergeCell ref="M110:P110"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="F111:H111"/>
-    <mergeCell ref="I111:L111"/>
-    <mergeCell ref="M111:P111"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="F112:H112"/>
-    <mergeCell ref="I112:L112"/>
-    <mergeCell ref="M112:P112"/>
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="F113:H113"/>
-    <mergeCell ref="I113:L113"/>
-    <mergeCell ref="M113:P113"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="F114:H114"/>
-    <mergeCell ref="I114:L114"/>
-    <mergeCell ref="M114:P114"/>
-    <mergeCell ref="M115:P115"/>
-    <mergeCell ref="D116:E116"/>
-    <mergeCell ref="F116:H116"/>
-    <mergeCell ref="I116:L116"/>
-    <mergeCell ref="M116:P116"/>
-    <mergeCell ref="B138:L138"/>
-    <mergeCell ref="D141:G141"/>
-    <mergeCell ref="H141:M141"/>
-    <mergeCell ref="D142:G142"/>
-    <mergeCell ref="H142:M142"/>
-    <mergeCell ref="D143:G143"/>
-    <mergeCell ref="H143:M143"/>
-    <mergeCell ref="D144:G144"/>
-    <mergeCell ref="H144:M144"/>
-    <mergeCell ref="D145:G145"/>
-    <mergeCell ref="H145:M145"/>
     <mergeCell ref="G119:G120"/>
     <mergeCell ref="E1:J2"/>
     <mergeCell ref="B80:E82"/>
@@ -15270,6 +15273,64 @@
     <mergeCell ref="D115:E115"/>
     <mergeCell ref="F115:H115"/>
     <mergeCell ref="I115:L115"/>
+    <mergeCell ref="D143:G143"/>
+    <mergeCell ref="H143:M143"/>
+    <mergeCell ref="D144:G144"/>
+    <mergeCell ref="H144:M144"/>
+    <mergeCell ref="D145:G145"/>
+    <mergeCell ref="H145:M145"/>
+    <mergeCell ref="B138:L138"/>
+    <mergeCell ref="D141:G141"/>
+    <mergeCell ref="H141:M141"/>
+    <mergeCell ref="D142:G142"/>
+    <mergeCell ref="H142:M142"/>
+    <mergeCell ref="M115:P115"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="F116:H116"/>
+    <mergeCell ref="I116:L116"/>
+    <mergeCell ref="M116:P116"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="F113:H113"/>
+    <mergeCell ref="I113:L113"/>
+    <mergeCell ref="M113:P113"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="F114:H114"/>
+    <mergeCell ref="I114:L114"/>
+    <mergeCell ref="M114:P114"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="F111:H111"/>
+    <mergeCell ref="I111:L111"/>
+    <mergeCell ref="M111:P111"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="F112:H112"/>
+    <mergeCell ref="I112:L112"/>
+    <mergeCell ref="M112:P112"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="F109:H109"/>
+    <mergeCell ref="I109:L109"/>
+    <mergeCell ref="M109:P109"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="F110:H110"/>
+    <mergeCell ref="I110:L110"/>
+    <mergeCell ref="M110:P110"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="F107:H107"/>
+    <mergeCell ref="I107:L107"/>
+    <mergeCell ref="M107:P107"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="I108:L108"/>
+    <mergeCell ref="M108:P108"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="F106:H106"/>
+    <mergeCell ref="I106:L106"/>
+    <mergeCell ref="M106:P106"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B85:C85"/>
   </mergeCells>
   <phoneticPr fontId="52" type="noConversion"/>
   <pageMargins left="0.78680555555555598" right="0.78680555555555598" top="0.98263888888888895" bottom="0.98263888888888895" header="0.51180555555555596" footer="0.51180555555555596"/>

</xml_diff>

<commit_message>
fix excel fix start.py update doc Signed-off-by: LiuYiyang <lyy@shequchina.cn>
</commit_message>
<xml_diff>
--- a/document/AP_障害管理票_QDYL.xlsx
+++ b/document/AP_障害管理票_QDYL.xlsx
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="230">
   <si>
     <t>通番</t>
   </si>
@@ -3283,6 +3283,147 @@
       </rPr>
       <t>失效</t>
     </r>
+  </si>
+  <si>
+    <t>随時対応一覧-&gt;保管場所使用承諾証明書発行（名義変更）-&gt;進捗情報1</t>
+  </si>
+  <si>
+    <r>
+      <t>送付先与書類送付先不一致，且</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>变</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t>更送付先</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>时以及保存时</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t>出</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>错</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t>，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>错误</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t>提示“Unknown format code 'd' for object of type 'str'”。但是修改的内容能</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>够保存。</t>
+    </r>
+    <phoneticPr fontId="52" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>契約者一覧-&gt;名前-&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>变</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t>更</t>
+    </r>
+    <phoneticPr fontId="52" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>保存按</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>钮被</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+      </rPr>
+      <t>menu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>按钮遮挡</t>
+    </r>
+    <phoneticPr fontId="52" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -6615,8 +6756,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674041"/>
-          <c:y val="3.5190678684544348E-2"/>
+          <c:x val="0.38523037913674085"/>
+          <c:y val="3.5190678684544389E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -6685,11 +6826,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="143182080"/>
-        <c:axId val="143187968"/>
+        <c:axId val="133556480"/>
+        <c:axId val="133558272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="143182080"/>
+        <c:axId val="133556480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6723,14 +6864,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="143187968"/>
+        <c:crossAx val="133558272"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143187968"/>
+        <c:axId val="133558272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6764,7 +6905,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="143182080"/>
+        <c:crossAx val="133556480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6814,7 +6955,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6851,8 +6992,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674041"/>
-          <c:y val="3.0232730603965523E-2"/>
+          <c:x val="0.38523037913674085"/>
+          <c:y val="3.0232730603965589E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -6868,10 +7009,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11177666498383214"/>
+          <c:x val="0.11177666498383228"/>
           <c:y val="0.100000113553908"/>
           <c:w val="0.78044064301210703"/>
-          <c:h val="0.65814028222689225"/>
+          <c:h val="0.6581402822268938"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -6978,11 +7119,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="144256384"/>
-        <c:axId val="144278656"/>
+        <c:axId val="133569920"/>
+        <c:axId val="133600384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="144256384"/>
+        <c:axId val="133569920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7016,14 +7157,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="144278656"/>
+        <c:crossAx val="133600384"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144278656"/>
+        <c:axId val="133600384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7057,7 +7198,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="144256384"/>
+        <c:crossAx val="133569920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7107,7 +7248,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7144,8 +7285,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.39506259248458342"/>
-          <c:y val="3.1476997578692829E-2"/>
+          <c:x val="0.39506259248458392"/>
+          <c:y val="3.1476997578692878E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -7163,8 +7304,8 @@
           <c:yMode val="edge"/>
           <c:x val="9.2592778647397928E-2"/>
           <c:y val="0.113801452784504"/>
-          <c:w val="0.77572172333487865"/>
-          <c:h val="0.65133171912833354"/>
+          <c:w val="0.77572172333488054"/>
+          <c:h val="0.65133171912833365"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -7466,8 +7607,8 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="148851328"/>
-        <c:axId val="148865792"/>
+        <c:axId val="134507136"/>
+        <c:axId val="134517504"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -7566,11 +7707,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="148867328"/>
-        <c:axId val="148885504"/>
+        <c:axId val="134519040"/>
+        <c:axId val="134537216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="148851328"/>
+        <c:axId val="134507136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7604,14 +7745,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="148865792"/>
+        <c:crossAx val="134517504"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="148865792"/>
+        <c:axId val="134517504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7645,29 +7786,29 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="148851328"/>
+        <c:crossAx val="134507136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="148867328"/>
+        <c:axId val="134519040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="148885504"/>
+        <c:crossAx val="134537216"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="148885504"/>
+        <c:axId val="134537216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
-          <c:min val="0.75000000000000455"/>
+          <c:min val="0.75000000000000522"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
@@ -7699,7 +7840,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="148867328"/>
+        <c:crossAx val="134519040"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.05"/>
@@ -7722,8 +7863,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.22633788060443114"/>
-          <c:y val="0.93462469733656883"/>
+          <c:x val="0.2263378806044313"/>
+          <c:y val="0.93462469733656972"/>
           <c:w val="0.50411630644934757"/>
           <c:h val="4.8426150121065097E-2"/>
         </c:manualLayout>
@@ -7791,7 +7932,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7828,8 +7969,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674041"/>
-          <c:y val="3.0232707900360225E-2"/>
+          <c:x val="0.38523037913674085"/>
+          <c:y val="3.023270790036026E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -7845,10 +7986,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11177666498383214"/>
+          <c:x val="0.11177666498383228"/>
           <c:y val="0.100000113553908"/>
           <c:w val="0.78044064301210703"/>
-          <c:h val="0.65814028222689325"/>
+          <c:h val="0.6581402822268948"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -7910,11 +8051,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="151133568"/>
-        <c:axId val="151147648"/>
+        <c:axId val="133909888"/>
+        <c:axId val="133915776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="151133568"/>
+        <c:axId val="133909888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7948,14 +8089,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="151147648"/>
+        <c:crossAx val="133915776"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151147648"/>
+        <c:axId val="133915776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7989,7 +8130,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="151133568"/>
+        <c:crossAx val="133909888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8039,7 +8180,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8076,8 +8217,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674041"/>
-          <c:y val="3.5190678684544348E-2"/>
+          <c:x val="0.38523037913674085"/>
+          <c:y val="3.5190678684544389E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -8194,11 +8335,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="151175552"/>
-        <c:axId val="151177088"/>
+        <c:axId val="133935488"/>
+        <c:axId val="133937024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="151175552"/>
+        <c:axId val="133935488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8232,14 +8373,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="151177088"/>
+        <c:crossAx val="133937024"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151177088"/>
+        <c:axId val="133937024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8273,7 +8414,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="151175552"/>
+        <c:crossAx val="133935488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8323,7 +8464,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8360,8 +8501,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674041"/>
-          <c:y val="3.5190678684544348E-2"/>
+          <c:x val="0.38523037913674085"/>
+          <c:y val="3.5190678684544389E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -8478,11 +8619,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="146957440"/>
-        <c:axId val="146958976"/>
+        <c:axId val="136860800"/>
+        <c:axId val="136862336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146957440"/>
+        <c:axId val="136860800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8516,14 +8657,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146958976"/>
+        <c:crossAx val="136862336"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146958976"/>
+        <c:axId val="136862336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8557,7 +8698,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146957440"/>
+        <c:crossAx val="136860800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8607,7 +8748,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8644,8 +8785,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38523037913674041"/>
-          <c:y val="3.0232707900360225E-2"/>
+          <c:x val="0.38523037913674085"/>
+          <c:y val="3.023270790036026E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -8661,10 +8802,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11177666498383214"/>
+          <c:x val="0.11177666498383228"/>
           <c:y val="0.100000113553908"/>
           <c:w val="0.78044064301210703"/>
-          <c:h val="0.65814028222689325"/>
+          <c:h val="0.6581402822268948"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -8726,11 +8867,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="146974592"/>
-        <c:axId val="146976128"/>
+        <c:axId val="136886144"/>
+        <c:axId val="136887680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146974592"/>
+        <c:axId val="136886144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8764,14 +8905,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146976128"/>
+        <c:crossAx val="136887680"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146976128"/>
+        <c:axId val="136887680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8805,7 +8946,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146974592"/>
+        <c:crossAx val="136886144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8855,7 +8996,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9602,13 +9743,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC111"/>
+  <dimension ref="A1:AC112"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="1" topLeftCell="J29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="1" topLeftCell="M29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I49" sqref="I49"/>
+      <selection pane="bottomRight" activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -11440,7 +11581,7 @@
         <v>41</v>
       </c>
       <c r="D36" s="114" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="E36" s="113"/>
       <c r="F36" s="108" t="s">
@@ -11483,7 +11624,7 @@
         <v>44</v>
       </c>
       <c r="D37" s="114" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="E37" s="113"/>
       <c r="F37" s="108" t="s">
@@ -11503,7 +11644,9 @@
       <c r="L37" s="115" t="s">
         <v>225</v>
       </c>
-      <c r="M37" s="147"/>
+      <c r="M37" s="147" t="s">
+        <v>229</v>
+      </c>
       <c r="N37" s="128"/>
       <c r="O37" s="128"/>
       <c r="P37" s="148"/>
@@ -11521,18 +11664,36 @@
       <c r="AB37" s="183"/>
     </row>
     <row r="38" spans="2:28" ht="14.25" customHeight="1">
-      <c r="B38" s="90"/>
-      <c r="C38" s="105"/>
-      <c r="D38" s="114"/>
+      <c r="B38" s="90">
+        <v>36</v>
+      </c>
+      <c r="C38" s="105" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="114" t="s">
+        <v>54</v>
+      </c>
       <c r="E38" s="113"/>
-      <c r="F38" s="108"/>
+      <c r="F38" s="108" t="s">
+        <v>29</v>
+      </c>
       <c r="G38" s="101"/>
       <c r="H38" s="116"/>
-      <c r="I38" s="144"/>
-      <c r="J38" s="129"/>
-      <c r="K38" s="145"/>
-      <c r="L38" s="115"/>
-      <c r="M38" s="147"/>
+      <c r="I38" s="144" t="s">
+        <v>228</v>
+      </c>
+      <c r="J38" s="129">
+        <v>43280</v>
+      </c>
+      <c r="K38" s="156" t="s">
+        <v>38</v>
+      </c>
+      <c r="L38" s="115" t="s">
+        <v>225</v>
+      </c>
+      <c r="M38" s="147" t="s">
+        <v>229</v>
+      </c>
       <c r="N38" s="128"/>
       <c r="O38" s="128"/>
       <c r="P38" s="148"/>
@@ -11549,18 +11710,34 @@
       <c r="AA38" s="179"/>
       <c r="AB38" s="183"/>
     </row>
-    <row r="39" spans="2:28" ht="14.25" customHeight="1">
-      <c r="B39" s="90"/>
-      <c r="C39" s="105"/>
-      <c r="D39" s="114"/>
+    <row r="39" spans="2:28" ht="34.5" customHeight="1">
+      <c r="B39" s="90">
+        <v>37</v>
+      </c>
+      <c r="C39" s="105" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39" s="114" t="s">
+        <v>27</v>
+      </c>
       <c r="E39" s="113"/>
-      <c r="F39" s="108"/>
+      <c r="F39" s="108" t="s">
+        <v>29</v>
+      </c>
       <c r="G39" s="101"/>
       <c r="H39" s="116"/>
-      <c r="I39" s="144"/>
-      <c r="J39" s="129"/>
-      <c r="K39" s="145"/>
-      <c r="L39" s="115"/>
+      <c r="I39" s="115" t="s">
+        <v>226</v>
+      </c>
+      <c r="J39" s="129">
+        <v>43280</v>
+      </c>
+      <c r="K39" s="156" t="s">
+        <v>38</v>
+      </c>
+      <c r="L39" s="115" t="s">
+        <v>227</v>
+      </c>
       <c r="M39" s="147"/>
       <c r="N39" s="128"/>
       <c r="O39" s="128"/>
@@ -12885,15 +13062,15 @@
     </row>
     <row r="85" spans="2:28" ht="14.25" customHeight="1">
       <c r="B85" s="90"/>
-      <c r="C85" s="113"/>
+      <c r="C85" s="105"/>
       <c r="D85" s="114"/>
       <c r="E85" s="113"/>
-      <c r="F85" s="184"/>
+      <c r="F85" s="108"/>
       <c r="G85" s="101"/>
-      <c r="H85" s="115"/>
+      <c r="H85" s="116"/>
       <c r="I85" s="144"/>
-      <c r="J85" s="125"/>
-      <c r="K85" s="144"/>
+      <c r="J85" s="129"/>
+      <c r="K85" s="145"/>
       <c r="L85" s="115"/>
       <c r="M85" s="147"/>
       <c r="N85" s="128"/>
@@ -12912,8 +13089,34 @@
       <c r="AA85" s="179"/>
       <c r="AB85" s="183"/>
     </row>
-    <row r="86" spans="2:28">
-      <c r="P86" s="93"/>
+    <row r="86" spans="2:28" ht="14.25" customHeight="1">
+      <c r="B86" s="90"/>
+      <c r="C86" s="113"/>
+      <c r="D86" s="114"/>
+      <c r="E86" s="113"/>
+      <c r="F86" s="184"/>
+      <c r="G86" s="101"/>
+      <c r="H86" s="115"/>
+      <c r="I86" s="144"/>
+      <c r="J86" s="125"/>
+      <c r="K86" s="144"/>
+      <c r="L86" s="115"/>
+      <c r="M86" s="147"/>
+      <c r="N86" s="128"/>
+      <c r="O86" s="128"/>
+      <c r="P86" s="148"/>
+      <c r="Q86" s="176"/>
+      <c r="R86" s="176"/>
+      <c r="S86" s="176"/>
+      <c r="T86" s="176"/>
+      <c r="U86" s="144"/>
+      <c r="V86" s="144"/>
+      <c r="W86" s="177"/>
+      <c r="X86" s="144"/>
+      <c r="Y86" s="125"/>
+      <c r="Z86" s="179"/>
+      <c r="AA86" s="179"/>
+      <c r="AB86" s="183"/>
     </row>
     <row r="87" spans="2:28">
       <c r="P87" s="93"/>
@@ -12989,6 +13192,9 @@
     </row>
     <row r="111" spans="16:16">
       <c r="P111" s="93"/>
+    </row>
+    <row r="112" spans="16:16">
+      <c r="P112" s="93"/>
     </row>
   </sheetData>
   <phoneticPr fontId="52" type="noConversion"/>
@@ -13245,30 +13451,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33">
-    <cfRule type="expression" dxfId="13" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="3" stopIfTrue="1">
       <formula>IF($B33="完了",TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="4" stopIfTrue="1">
       <formula>IF($B33="完了",TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="5" stopIfTrue="1">
       <formula>IF($B33="完了",TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="6" stopIfTrue="1">
       <formula>IF($B33="完了",TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="7" stopIfTrue="1">
       <formula>IF($B33="完了",TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="8" stopIfTrue="1">
       <formula>IF($B33="完了",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L33">
-    <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="1" stopIfTrue="1">
       <formula>IF($B33="完了",TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
       <formula>IF($B33="完了",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13297,19 +13503,19 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="15">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P7:T7 F85:F65586 P10:T85">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P7:T7 F86:F65587 P10:T86">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D85">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D86">
       <formula1>"未着手,対応判断中,対応中,完了"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E85">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E86">
       <formula1>"新規,変更"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F84">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F85">
       <formula1>発生段階</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G85 C35:C36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C35:C36 G2:G86">
       <formula1>"DB,ソース,テストケース,その他"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7">
@@ -13318,10 +13524,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E12">
       <formula1>対応区分</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N85">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N86">
       <formula1>"●,✖"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O85">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O86">
       <formula1>"高,中,低,実害無し"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P6 P8:P9">
@@ -13339,7 +13545,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T6 T8:T9">
       <formula1>原因工程</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:AA85">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:AA86">
       <formula1>"○,×"</formula1>
     </dataValidation>
   </dataValidations>
@@ -13409,7 +13615,7 @@
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="31">
-        <f>COUNTIF(単体障害一覧!P$2:P$475,B4)</f>
+        <f>COUNTIF(単体障害一覧!P$2:P$476,B4)</f>
         <v>0</v>
       </c>
       <c r="E4" s="32" t="e">
@@ -13423,7 +13629,7 @@
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="35">
-        <f>COUNTIF(単体障害一覧!P$2:P$475,B5)</f>
+        <f>COUNTIF(単体障害一覧!P$2:P$476,B5)</f>
         <v>0</v>
       </c>
       <c r="E5" s="32" t="e">
@@ -13522,7 +13728,7 @@
       </c>
       <c r="C23" s="30"/>
       <c r="D23" s="31">
-        <f>COUNTIF(単体障害一覧!Q$2:Q$475,B23)</f>
+        <f>COUNTIF(単体障害一覧!Q$2:Q$476,B23)</f>
         <v>0</v>
       </c>
       <c r="E23" s="41" t="e">
@@ -13536,7 +13742,7 @@
       </c>
       <c r="C24" s="34"/>
       <c r="D24" s="35">
-        <f>COUNTIF(単体障害一覧!Q$2:Q$475,B24)</f>
+        <f>COUNTIF(単体障害一覧!Q$2:Q$476,B24)</f>
         <v>0</v>
       </c>
       <c r="E24" s="42" t="e">
@@ -13550,7 +13756,7 @@
       </c>
       <c r="C25" s="34"/>
       <c r="D25" s="35">
-        <f>COUNTIF(単体障害一覧!Q$2:Q$475,B25)</f>
+        <f>COUNTIF(単体障害一覧!Q$2:Q$476,B25)</f>
         <v>0</v>
       </c>
       <c r="E25" s="42" t="e">
@@ -13564,7 +13770,7 @@
       </c>
       <c r="C26" s="34"/>
       <c r="D26" s="35">
-        <f>COUNTIF(単体障害一覧!Q$2:Q$475,B26)</f>
+        <f>COUNTIF(単体障害一覧!Q$2:Q$476,B26)</f>
         <v>0</v>
       </c>
       <c r="E26" s="42" t="e">
@@ -13578,7 +13784,7 @@
       </c>
       <c r="C27" s="34"/>
       <c r="D27" s="35">
-        <f>COUNTIF(単体障害一覧!Q$2:Q$475,B27)</f>
+        <f>COUNTIF(単体障害一覧!Q$2:Q$476,B27)</f>
         <v>0</v>
       </c>
       <c r="E27" s="42" t="e">
@@ -13592,7 +13798,7 @@
       </c>
       <c r="C28" s="34"/>
       <c r="D28" s="35">
-        <f>COUNTIF(単体障害一覧!Q$2:Q$475,B28)</f>
+        <f>COUNTIF(単体障害一覧!Q$2:Q$476,B28)</f>
         <v>0</v>
       </c>
       <c r="E28" s="42" t="e">
@@ -13606,7 +13812,7 @@
       </c>
       <c r="C29" s="34"/>
       <c r="D29" s="35">
-        <f>COUNTIF(単体障害一覧!Q$2:Q$475,B29)</f>
+        <f>COUNTIF(単体障害一覧!Q$2:Q$476,B29)</f>
         <v>0</v>
       </c>
       <c r="E29" s="42" t="e">
@@ -13620,7 +13826,7 @@
       </c>
       <c r="C30" s="34"/>
       <c r="D30" s="35">
-        <f>COUNTIF(単体障害一覧!Q$2:Q$475,B30)</f>
+        <f>COUNTIF(単体障害一覧!Q$2:Q$476,B30)</f>
         <v>0</v>
       </c>
       <c r="E30" s="42" t="e">
@@ -13634,7 +13840,7 @@
       </c>
       <c r="C31" s="34"/>
       <c r="D31" s="35">
-        <f>COUNTIF(単体障害一覧!Q$2:Q$475,B31)</f>
+        <f>COUNTIF(単体障害一覧!Q$2:Q$476,B31)</f>
         <v>0</v>
       </c>
       <c r="E31" s="42" t="e">
@@ -13648,7 +13854,7 @@
       </c>
       <c r="C32" s="34"/>
       <c r="D32" s="35">
-        <f>COUNTIF(単体障害一覧!Q$2:Q$475,B32)</f>
+        <f>COUNTIF(単体障害一覧!Q$2:Q$476,B32)</f>
         <v>0</v>
       </c>
       <c r="E32" s="42" t="e">
@@ -13662,7 +13868,7 @@
       </c>
       <c r="C33" s="34"/>
       <c r="D33" s="35">
-        <f>COUNTIF(単体障害一覧!Q$2:Q$475,B33)</f>
+        <f>COUNTIF(単体障害一覧!Q$2:Q$476,B33)</f>
         <v>0</v>
       </c>
       <c r="E33" s="42" t="e">
@@ -13676,7 +13882,7 @@
       </c>
       <c r="C34" s="37"/>
       <c r="D34" s="38">
-        <f>COUNTIF(単体障害一覧!Q$2:Q$475,B34)</f>
+        <f>COUNTIF(単体障害一覧!Q$2:Q$476,B34)</f>
         <v>0</v>
       </c>
       <c r="E34" s="43" t="e">
@@ -13739,7 +13945,7 @@
       </c>
       <c r="C45" s="30"/>
       <c r="D45" s="31">
-        <f>COUNTIF(単体障害一覧!R$2:R$475,B45)</f>
+        <f>COUNTIF(単体障害一覧!R$2:R$476,B45)</f>
         <v>0</v>
       </c>
       <c r="E45" s="41" t="e">
@@ -13753,7 +13959,7 @@
       </c>
       <c r="C46" s="34"/>
       <c r="D46" s="35">
-        <f>COUNTIF(単体障害一覧!R$2:R$475,B46)</f>
+        <f>COUNTIF(単体障害一覧!R$2:R$476,B46)</f>
         <v>0</v>
       </c>
       <c r="E46" s="42" t="e">
@@ -13767,7 +13973,7 @@
       </c>
       <c r="C47" s="34"/>
       <c r="D47" s="35">
-        <f>COUNTIF(単体障害一覧!R$2:R$475,B47)</f>
+        <f>COUNTIF(単体障害一覧!R$2:R$476,B47)</f>
         <v>0</v>
       </c>
       <c r="E47" s="42" t="e">
@@ -13781,7 +13987,7 @@
       </c>
       <c r="C48" s="34"/>
       <c r="D48" s="35">
-        <f>COUNTIF(単体障害一覧!R$2:R$475,B48)</f>
+        <f>COUNTIF(単体障害一覧!R$2:R$476,B48)</f>
         <v>0</v>
       </c>
       <c r="E48" s="42" t="e">
@@ -13795,7 +14001,7 @@
       </c>
       <c r="C49" s="34"/>
       <c r="D49" s="35">
-        <f>COUNTIF(単体障害一覧!R$2:R$475,B49)</f>
+        <f>COUNTIF(単体障害一覧!R$2:R$476,B49)</f>
         <v>0</v>
       </c>
       <c r="E49" s="42" t="e">
@@ -13809,7 +14015,7 @@
       </c>
       <c r="C50" s="34"/>
       <c r="D50" s="35">
-        <f>COUNTIF(単体障害一覧!R$2:R$475,B50)</f>
+        <f>COUNTIF(単体障害一覧!R$2:R$476,B50)</f>
         <v>0</v>
       </c>
       <c r="E50" s="42" t="e">
@@ -13823,7 +14029,7 @@
       </c>
       <c r="C51" s="34"/>
       <c r="D51" s="35">
-        <f>COUNTIF(単体障害一覧!R$2:R$475,B51)</f>
+        <f>COUNTIF(単体障害一覧!R$2:R$476,B51)</f>
         <v>0</v>
       </c>
       <c r="E51" s="42" t="e">
@@ -13837,7 +14043,7 @@
       </c>
       <c r="C52" s="34"/>
       <c r="D52" s="35">
-        <f>COUNTIF(単体障害一覧!R$2:R$475,B52)</f>
+        <f>COUNTIF(単体障害一覧!R$2:R$476,B52)</f>
         <v>0</v>
       </c>
       <c r="E52" s="42" t="e">
@@ -13851,7 +14057,7 @@
       </c>
       <c r="C53" s="34"/>
       <c r="D53" s="35">
-        <f>COUNTIF(単体障害一覧!R$2:R$475,B53)</f>
+        <f>COUNTIF(単体障害一覧!R$2:R$476,B53)</f>
         <v>0</v>
       </c>
       <c r="E53" s="42" t="e">
@@ -13865,7 +14071,7 @@
       </c>
       <c r="C54" s="37"/>
       <c r="D54" s="38">
-        <f>COUNTIF(単体障害一覧!R$2:R$475,B54)</f>
+        <f>COUNTIF(単体障害一覧!R$2:R$476,B54)</f>
         <v>0</v>
       </c>
       <c r="E54" s="43" t="e">
@@ -13928,7 +14134,7 @@
       </c>
       <c r="C66" s="45"/>
       <c r="D66" s="31">
-        <f>COUNTIF(単体障害一覧!S$2:S$475,B66)</f>
+        <f>COUNTIF(単体障害一覧!S$2:S$476,B66)</f>
         <v>0</v>
       </c>
       <c r="E66" s="41" t="e">
@@ -13942,7 +14148,7 @@
       </c>
       <c r="C67" s="47"/>
       <c r="D67" s="35">
-        <f>COUNTIF(単体障害一覧!S$2:S$475,B67)</f>
+        <f>COUNTIF(単体障害一覧!S$2:S$476,B67)</f>
         <v>0</v>
       </c>
       <c r="E67" s="42" t="e">
@@ -13956,7 +14162,7 @@
       </c>
       <c r="C68" s="47"/>
       <c r="D68" s="35">
-        <f>COUNTIF(単体障害一覧!S$2:S$475,B68)</f>
+        <f>COUNTIF(単体障害一覧!S$2:S$476,B68)</f>
         <v>0</v>
       </c>
       <c r="E68" s="42" t="e">
@@ -13970,7 +14176,7 @@
       </c>
       <c r="C69" s="47"/>
       <c r="D69" s="35">
-        <f>COUNTIF(単体障害一覧!S$2:S$475,B69)</f>
+        <f>COUNTIF(単体障害一覧!S$2:S$476,B69)</f>
         <v>0</v>
       </c>
       <c r="E69" s="42" t="e">
@@ -13984,7 +14190,7 @@
       </c>
       <c r="C70" s="47"/>
       <c r="D70" s="35">
-        <f>COUNTIF(単体障害一覧!S$2:S$475,B70)</f>
+        <f>COUNTIF(単体障害一覧!S$2:S$476,B70)</f>
         <v>0</v>
       </c>
       <c r="E70" s="42" t="e">
@@ -14022,7 +14228,7 @@
       </c>
       <c r="C74" s="47"/>
       <c r="D74" s="35">
-        <f>COUNTIF(単体障害一覧!S$2:S$475,B74)</f>
+        <f>COUNTIF(単体障害一覧!S$2:S$476,B74)</f>
         <v>0</v>
       </c>
       <c r="E74" s="42" t="e">
@@ -14036,7 +14242,7 @@
       </c>
       <c r="C75" s="47"/>
       <c r="D75" s="35">
-        <f>COUNTIF(単体障害一覧!S$2:S$475,B75)</f>
+        <f>COUNTIF(単体障害一覧!S$2:S$476,B75)</f>
         <v>0</v>
       </c>
       <c r="E75" s="42" t="e">
@@ -14050,7 +14256,7 @@
       </c>
       <c r="C76" s="47"/>
       <c r="D76" s="35">
-        <f>COUNTIF(単体障害一覧!S$2:S$475,B76)</f>
+        <f>COUNTIF(単体障害一覧!S$2:S$476,B76)</f>
         <v>0</v>
       </c>
       <c r="E76" s="42" t="e">
@@ -14064,7 +14270,7 @@
       </c>
       <c r="C77" s="47"/>
       <c r="D77" s="35">
-        <f>COUNTIF(単体障害一覧!S$2:S$475,B77)</f>
+        <f>COUNTIF(単体障害一覧!S$2:S$476,B77)</f>
         <v>0</v>
       </c>
       <c r="E77" s="42" t="e">
@@ -14078,7 +14284,7 @@
       </c>
       <c r="C78" s="49"/>
       <c r="D78" s="38">
-        <f>COUNTIF(単体障害一覧!S$2:S$475,B78)</f>
+        <f>COUNTIF(単体障害一覧!S$2:S$476,B78)</f>
         <v>0</v>
       </c>
       <c r="E78" s="43" t="e">
@@ -14151,7 +14357,7 @@
       </c>
       <c r="C86" s="45"/>
       <c r="D86" s="31">
-        <f>COUNTIF(単体障害一覧!T$2:T$475,B86)</f>
+        <f>COUNTIF(単体障害一覧!T$2:T$476,B86)</f>
         <v>0</v>
       </c>
       <c r="E86" s="41" t="e">
@@ -14165,7 +14371,7 @@
       </c>
       <c r="C87" s="47"/>
       <c r="D87" s="35">
-        <f>COUNTIF(単体障害一覧!T$2:T$475,B87)</f>
+        <f>COUNTIF(単体障害一覧!T$2:T$476,B87)</f>
         <v>0</v>
       </c>
       <c r="E87" s="42" t="e">
@@ -14179,7 +14385,7 @@
       </c>
       <c r="C88" s="47"/>
       <c r="D88" s="35">
-        <f>COUNTIF(単体障害一覧!T$2:T$475,B88)</f>
+        <f>COUNTIF(単体障害一覧!T$2:T$476,B88)</f>
         <v>0</v>
       </c>
       <c r="E88" s="42" t="e">
@@ -14193,7 +14399,7 @@
       </c>
       <c r="C89" s="49"/>
       <c r="D89" s="38">
-        <f>COUNTIF(単体障害一覧!T$2:T$475,B89)</f>
+        <f>COUNTIF(単体障害一覧!T$2:T$476,B89)</f>
         <v>0</v>
       </c>
       <c r="E89" s="43" t="e">
@@ -14266,7 +14472,7 @@
       </c>
       <c r="C97" s="45"/>
       <c r="D97" s="31">
-        <f>COUNTIF(単体障害一覧!B$2:B$475,B97)</f>
+        <f>COUNTIF(単体障害一覧!B$2:B$476,B97)</f>
         <v>0</v>
       </c>
       <c r="E97" s="41" t="e">
@@ -14280,7 +14486,7 @@
       </c>
       <c r="C98" s="47"/>
       <c r="D98" s="35">
-        <f>COUNTIF(単体障害一覧!B$2:B$475,B98)</f>
+        <f>COUNTIF(単体障害一覧!B$2:B$476,B98)</f>
         <v>0</v>
       </c>
       <c r="E98" s="42" t="e">
@@ -14294,7 +14500,7 @@
       </c>
       <c r="C99" s="49"/>
       <c r="D99" s="38">
-        <f>COUNTIF(単体障害一覧!B$2:B$475,B99)</f>
+        <f>COUNTIF(単体障害一覧!B$2:B$476,B99)</f>
         <v>0</v>
       </c>
       <c r="E99" s="43" t="e">
@@ -14722,11 +14928,11 @@
         <v>39707</v>
       </c>
       <c r="C121" s="65">
-        <f>SUMPRODUCT((単体障害一覧!J$2:J$475&lt;B121)*(単体障害一覧!J$2:J$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!J$2:J$476&lt;B121)*(単体障害一覧!J$2:J$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="D121" s="65">
-        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$475&lt;B121)*(単体障害一覧!Y$2:Y$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$476&lt;B121)*(単体障害一覧!Y$2:Y$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="E121" s="66">
@@ -14748,11 +14954,11 @@
         <v>39713</v>
       </c>
       <c r="C122" s="65">
-        <f>SUMPRODUCT((単体障害一覧!J$2:J$475&lt;B122)*(単体障害一覧!J$2:J$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!J$2:J$476&lt;B122)*(単体障害一覧!J$2:J$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="D122" s="65">
-        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$475&lt;B122)*(単体障害一覧!Y$2:Y$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$476&lt;B122)*(単体障害一覧!Y$2:Y$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="E122" s="66" t="e">
@@ -14774,11 +14980,11 @@
         <v>39719</v>
       </c>
       <c r="C123" s="65">
-        <f>SUMPRODUCT((単体障害一覧!J$2:J$475&lt;B123)*(単体障害一覧!J$2:J$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!J$2:J$476&lt;B123)*(単体障害一覧!J$2:J$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="D123" s="65">
-        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$475&lt;B123)*(単体障害一覧!Y$2:Y$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$476&lt;B123)*(単体障害一覧!Y$2:Y$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="E123" s="66" t="e">
@@ -14800,11 +15006,11 @@
         <v>39725</v>
       </c>
       <c r="C124" s="65">
-        <f>SUMPRODUCT((単体障害一覧!J$2:J$475&lt;B124)*(単体障害一覧!J$2:J$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!J$2:J$476&lt;B124)*(単体障害一覧!J$2:J$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="D124" s="65">
-        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$475&lt;B124)*(単体障害一覧!Y$2:Y$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$476&lt;B124)*(単体障害一覧!Y$2:Y$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="E124" s="66" t="e">
@@ -14826,11 +15032,11 @@
         <v>39731</v>
       </c>
       <c r="C125" s="65">
-        <f>SUMPRODUCT((単体障害一覧!J$2:J$475&lt;B125)*(単体障害一覧!J$2:J$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!J$2:J$476&lt;B125)*(単体障害一覧!J$2:J$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="D125" s="65">
-        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$475&lt;B125)*(単体障害一覧!Y$2:Y$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$476&lt;B125)*(単体障害一覧!Y$2:Y$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="E125" s="66" t="e">
@@ -14852,11 +15058,11 @@
         <v>39737</v>
       </c>
       <c r="C126" s="65">
-        <f>SUMPRODUCT((単体障害一覧!J$2:J$475&lt;B126)*(単体障害一覧!J$2:J$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!J$2:J$476&lt;B126)*(単体障害一覧!J$2:J$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="D126" s="65">
-        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$475&lt;B126)*(単体障害一覧!Y$2:Y$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$476&lt;B126)*(単体障害一覧!Y$2:Y$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="E126" s="66" t="e">
@@ -14878,11 +15084,11 @@
         <v>39743</v>
       </c>
       <c r="C127" s="65">
-        <f>SUMPRODUCT((単体障害一覧!J$2:J$475&lt;B127)*(単体障害一覧!J$2:J$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!J$2:J$476&lt;B127)*(単体障害一覧!J$2:J$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="D127" s="65">
-        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$475&lt;B127)*(単体障害一覧!Y$2:Y$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$476&lt;B127)*(単体障害一覧!Y$2:Y$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="E127" s="66" t="e">
@@ -14904,11 +15110,11 @@
         <v>39749</v>
       </c>
       <c r="C128" s="65">
-        <f>SUMPRODUCT((単体障害一覧!J$2:J$475&lt;B128)*(単体障害一覧!J$2:J$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!J$2:J$476&lt;B128)*(単体障害一覧!J$2:J$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="D128" s="65">
-        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$475&lt;B128)*(単体障害一覧!Y$2:Y$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$476&lt;B128)*(単体障害一覧!Y$2:Y$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="E128" s="66" t="e">
@@ -14930,11 +15136,11 @@
         <v>39755</v>
       </c>
       <c r="C129" s="65">
-        <f>SUMPRODUCT((単体障害一覧!J$2:J$475&lt;B129)*(単体障害一覧!J$2:J$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!J$2:J$476&lt;B129)*(単体障害一覧!J$2:J$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="D129" s="65">
-        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$475&lt;B129)*(単体障害一覧!Y$2:Y$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$476&lt;B129)*(単体障害一覧!Y$2:Y$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="E129" s="66" t="e">
@@ -14956,11 +15162,11 @@
         <v>39761</v>
       </c>
       <c r="C130" s="65">
-        <f>SUMPRODUCT((単体障害一覧!J$2:J$475&lt;B130)*(単体障害一覧!J$2:J$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!J$2:J$476&lt;B130)*(単体障害一覧!J$2:J$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="D130" s="65">
-        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$475&lt;B130)*(単体障害一覧!Y$2:Y$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$476&lt;B130)*(単体障害一覧!Y$2:Y$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="E130" s="66" t="e">
@@ -14982,11 +15188,11 @@
         <v>39767</v>
       </c>
       <c r="C131" s="65">
-        <f>SUMPRODUCT((単体障害一覧!J$2:J$475&lt;B131)*(単体障害一覧!J$2:J$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!J$2:J$476&lt;B131)*(単体障害一覧!J$2:J$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="D131" s="65">
-        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$475&lt;B131)*(単体障害一覧!Y$2:Y$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$476&lt;B131)*(単体障害一覧!Y$2:Y$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="E131" s="66" t="e">
@@ -15008,11 +15214,11 @@
         <v>39773</v>
       </c>
       <c r="C132" s="65">
-        <f>SUMPRODUCT((単体障害一覧!J$2:J$475&lt;B132)*(単体障害一覧!J$2:J$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!J$2:J$476&lt;B132)*(単体障害一覧!J$2:J$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="D132" s="65">
-        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$475&lt;B132)*(単体障害一覧!Y$2:Y$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$476&lt;B132)*(単体障害一覧!Y$2:Y$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="E132" s="66" t="e">
@@ -15034,11 +15240,11 @@
         <v>39779</v>
       </c>
       <c r="C133" s="65">
-        <f>SUMPRODUCT((単体障害一覧!J$2:J$475&lt;B133)*(単体障害一覧!J$2:J$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!J$2:J$476&lt;B133)*(単体障害一覧!J$2:J$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="D133" s="65">
-        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$475&lt;B133)*(単体障害一覧!Y$2:Y$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$476&lt;B133)*(単体障害一覧!Y$2:Y$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="E133" s="66" t="e">
@@ -15060,11 +15266,11 @@
         <v>39785</v>
       </c>
       <c r="C134" s="65">
-        <f>SUMPRODUCT((単体障害一覧!J$2:J$475&lt;B134)*(単体障害一覧!J$2:J$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!J$2:J$476&lt;B134)*(単体障害一覧!J$2:J$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="D134" s="65">
-        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$475&lt;B134)*(単体障害一覧!Y$2:Y$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$476&lt;B134)*(単体障害一覧!Y$2:Y$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="E134" s="66" t="e">
@@ -15086,11 +15292,11 @@
         <v>39791</v>
       </c>
       <c r="C135" s="65">
-        <f>SUMPRODUCT((単体障害一覧!J$2:J$475&lt;B135)*(単体障害一覧!J$2:J$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!J$2:J$476&lt;B135)*(単体障害一覧!J$2:J$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="D135" s="65">
-        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$475&lt;B135)*(単体障害一覧!Y$2:Y$475&lt;&gt;""))</f>
+        <f>SUMPRODUCT((単体障害一覧!Y$2:Y$476&lt;B135)*(単体障害一覧!Y$2:Y$476&lt;&gt;""))</f>
         <v>0</v>
       </c>
       <c r="E135" s="66" t="e">

</xml_diff>